<commit_message>
Thu Dec  9 07:32:40 CST 2021
</commit_message>
<xml_diff>
--- a/笔记/CISSP/CISSP知识点.xlsx
+++ b/笔记/CISSP/CISSP知识点.xlsx
@@ -70,6 +70,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
       <t>客体必须保持自身的正确性，只能由</t>
     </r>
     <r>
@@ -77,6 +82,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>被授权的主体进行修改</t>
@@ -85,6 +91,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>。维护完整性意味着客体本身</t>
@@ -94,6 +101,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>不会被改变或篡改</t>
@@ -102,6 +110,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>。</t>
@@ -112,6 +121,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
       <t>必须对数据、客体和资源的访问进行适当控制。此外，应当使用活动日志记录，从而保证只有经过</t>
     </r>
     <r>
@@ -119,6 +133,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>授权的用户才能够访问资源</t>
@@ -127,6 +142,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>。这些措施包括：严格的访问控制、严密的身份认证过程、入侵检测系统、对客体/数据进行加密、</t>
@@ -136,6 +152,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>散列总和认证</t>
@@ -144,6 +161,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>、输入/功能检验。</t>
@@ -186,7 +204,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,8 +221,30 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,121 +258,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -348,10 +290,91 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="34">
@@ -369,181 +392,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -641,17 +664,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -680,15 +697,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -700,6 +708,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -730,11 +747,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -743,148 +766,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1249,8 +1272,8 @@
   <sheetPr/>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
Thu Jan  6 00:24:24 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CISSP/CISSP知识点.xlsx
+++ b/笔记/CISSP/CISSP知识点.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590">
   <si>
     <t>章节</t>
   </si>
@@ -1442,6 +1442,1073 @@
   </si>
   <si>
     <t>开发，测试、培训和维护，实施</t>
+  </si>
+  <si>
+    <t>法律和法规要求</t>
+  </si>
+  <si>
+    <t>要求实施 BCP</t>
+  </si>
+  <si>
+    <t>业务影响分析</t>
+  </si>
+  <si>
+    <t>业务影响分析是分析中断对组织的长期影响的过程。业务影响分析帮助一个组织确定其基本的业务功能，并了解灾难对每项功能的影响；业务影响分析为业务连续性计划及其要求提供主要理由。BIA帮助一个组织确定其哪些业务功能更有弹性，哪些更脆弱。</t>
+  </si>
+  <si>
+    <t>业务影响分析（BIA）可以帮助确定关键业务功能。</t>
+  </si>
+  <si>
+    <t>定量决策</t>
+  </si>
+  <si>
+    <t>涉及使用数字和公示得出结论。这类数据结果通常用货币价值表示与业务相关的选项。</t>
+  </si>
+  <si>
+    <t>定性决策</t>
+  </si>
+  <si>
+    <t>考虑非数字因素，如声誉、投资者/客户信心、员工稳定性和其他相关事项。</t>
+  </si>
+  <si>
+    <t>通常用优先级别（高、中、低）表示。</t>
+  </si>
+  <si>
+    <t>确定优先级</t>
+  </si>
+  <si>
+    <r>
+      <t>BCP 团队要完成的第一个 BIA 任务是确定业务优先级。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>根据业务范围，当灾难发生时，有些活动对维持日常运营极为关键。确认优先级或关键性涉及创建业务流程的综合列表，并按重要性进行排序。</t>
+    </r>
+  </si>
+  <si>
+    <t>当整个 BCP 团队开会讨论时，团队成员可基于这些优先级列表为整个组织创建优先级主列表。</t>
+  </si>
+  <si>
+    <t>开始定量评估，BCP 团队需要一起制定组织资产清单，并为每项资产分配货币形式的资产价值（AV）。这些数字将在后续BIA步骤中使用，从而实施基于财务的 BIA。</t>
+  </si>
+  <si>
+    <t>MTD RTO RPO</t>
+  </si>
+  <si>
+    <t>MTD</t>
+  </si>
+  <si>
+    <t>MTD（Maximum Tolerable Downtime，最大允许中断时间），有时也称为最大容忍中断时间（Maximum Tolerable Outage, MTO）。MTD 是业务功能出现故障但不会对业务产生无法弥补的损害所允许的最长时间。</t>
+  </si>
+  <si>
+    <t>执行 BCP 和 DRP 计划时，MTD 提供了重要信息。</t>
+  </si>
+  <si>
+    <t>RTO</t>
+  </si>
+  <si>
+    <t>RTO（Recovery Time Objective，恢复时间目标），是指当中断发生后实际恢复业务功能所需的时间。一旦定义了恢复目标，就可以设计和规划所需的步骤去完成恢复任务。</t>
+  </si>
+  <si>
+    <t>RPO</t>
+  </si>
+  <si>
+    <t>RPO（Recovery Point Objective，恢复点目标）表示对可容忍的数据损失的测量，以时间段表示。</t>
+  </si>
+  <si>
+    <t>风险识别</t>
+  </si>
+  <si>
+    <t>风险的两种形式：自然风险与人为风险。</t>
+  </si>
+  <si>
+    <t>BIA 过程的风险识别部分本质上是纯粹的定性分析。在这个过程中，BCP 团队不应关注每种风险实际发生的可能性，或风险发生或会对业务持续运营造成的损害程度。</t>
+  </si>
+  <si>
+    <t>可能性评估</t>
+  </si>
+  <si>
+    <t>业务影响评估的下一个阶段是确定每种风险发生的可能性。</t>
+  </si>
+  <si>
+    <t>可能性评估采用年发生比率（Annualized Rate Of Occurrence, ARO）表示，ARO反映了业务每年预期遭受特定灾难的次数。</t>
+  </si>
+  <si>
+    <t>BCP 团队必须一起为先前识别的每种风险确定 ARO，这些数字应当基于公司的历史、团队成员的专业经验以及专家的建议。</t>
+  </si>
+  <si>
+    <t>影响评估</t>
+  </si>
+  <si>
+    <t>该阶段，需要分析识别的风险与可能性评估期间收集的数据，并且尝试确定如果每种风险发生会对业务产生什么影响。</t>
+  </si>
+  <si>
+    <t>业务影响涉及三个特定的度量：暴露因子、单一损失期望和年度损失期望。</t>
+  </si>
+  <si>
+    <t>暴露因子</t>
+  </si>
+  <si>
+    <r>
+      <t>暴露因子（Exposure Factor, EF）是指</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>风险对资产造成损失的程度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，以资产价值的百分比来表示。</t>
+    </r>
+  </si>
+  <si>
+    <t>如建筑物发生火灾后造成70%的建筑物被毁坏，那么建筑物火灾的暴露因子就是70%</t>
+  </si>
+  <si>
+    <t>单一损失期望</t>
+  </si>
+  <si>
+    <r>
+      <t>单一损失期望（Single Loss Expectancy, SLE）是指</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>每次风险发生后预计造成的货币损失</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。SLE = AV * EF</t>
+    </r>
+  </si>
+  <si>
+    <t>如建筑物价值 500000 美元，单一损失期望就是 500000 的 70%（上文的暴露因子）, 即 350000美元。</t>
+  </si>
+  <si>
+    <t>每项资产分配货币形式的资产价值（AV）</t>
+  </si>
+  <si>
+    <t>年度损失期望</t>
+  </si>
+  <si>
+    <t>年度损失期望（Annualized Loss Expectancy, ALE）是指一年内由于风险引起资产损失而预计对公司造成的货币损失。ALE = SLE * ARO</t>
+  </si>
+  <si>
+    <t>如果建筑物每30年才发生一次火灾，那么ARO就是 1/30，ALE是350000美元SLE的3.333%, 即11667美元。可以理解为：由于建筑物火灾，公司每年预计损失11667美元。</t>
+  </si>
+  <si>
+    <t>定性影响评估</t>
+  </si>
+  <si>
+    <t>业务中断所造成的、非货币价值可以衡量的影响。</t>
+  </si>
+  <si>
+    <t>客户中间丧失的信誉、长时间停工后员工的流失、对公众的社会/道德责任。</t>
+  </si>
+  <si>
+    <t>资源优先级</t>
+  </si>
+  <si>
+    <r>
+      <t>BIA 的最后一个步骤是划分针对各种不同风险所分配的业务连续性资源的优先级</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。</t>
+    </r>
+  </si>
+  <si>
+    <t>从定量角度来看，这个过程相对简单。只需要生成一个BIA过程期间分析过的所有风险的列表，然后按照影响评估阶段计算出来的年度损失期望的降序进行分类，这样就生成了应当解决的风险优先级列表。</t>
+  </si>
+  <si>
+    <r>
+      <t>BCP过程的前两个阶段（项目范围和计划编制、业务影响评估）主要</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>确定BCP过程如何工作并确定必须防止其出现中断的业务资产的优先顺序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>BCP开发的下一个阶段是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>连续性计划编制，这个阶段专注于连续性策略的开发和实现，从而最小化已发生风险可能对保护资产的影响</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。</t>
+    </r>
+  </si>
+  <si>
+    <t>策略开发、预备和处理、计划批准、计划实现、培训和教育</t>
+  </si>
+  <si>
+    <t>策略开发</t>
+  </si>
+  <si>
+    <t>业务连续性计划的策略开发阶段为业务影响评估和BCP开发的连续性计划阶段之间架起了桥梁。</t>
+  </si>
+  <si>
+    <t>BCP团队应当回顾一下BIA前期建立的MTD评估时间，并且确定哪些风险被认为是可接受的，哪些必须采取BCP连续性措施加以缓解。</t>
+  </si>
+  <si>
+    <t>一旦 BCP 团队确定哪些风险需要环节以及将为每个环节任务提供的资源水平，就准备进入里连续性计划的“预备和处理”阶段</t>
+  </si>
+  <si>
+    <t>预备和处理</t>
+  </si>
+  <si>
+    <t>BCP 团队设计了具体的过程和机制，将在策略开发阶段缓解被任务不可接受的风险。下列三种资产类型必须通过BCP预备和处理进行保护</t>
+  </si>
+  <si>
+    <t>人</t>
+  </si>
+  <si>
+    <t>人是最优价值的资产，人的安全必须始终优先于公司的商业目标。</t>
+  </si>
+  <si>
+    <t>建筑物设备</t>
+  </si>
+  <si>
+    <t>在预备场所内恢复受影响的关键性业务。</t>
+  </si>
+  <si>
+    <t>基础设施</t>
+  </si>
+  <si>
+    <t>包括计算机防火抑制系统和不间断电源。预备系统：冗余性保护（冗余构件、冗余系统、冗余链路等）。</t>
+  </si>
+  <si>
+    <t>计划批准和计划实现</t>
+  </si>
+  <si>
+    <t>一旦 BCP 团队完成了 BCP 文档的设计阶段，就该申请获得高级管理层的批准了。</t>
+  </si>
+  <si>
+    <t>一旦得到高级管理层的批准，就应当推动并开始实现你的计划。BCP团队应该共同开发一个实现计划，这个计划利用特定的资源，从而尽可能迅速地在给出修改范围和组织环境的情况下取得所声明的过程和预备措施的目标。</t>
+  </si>
+  <si>
+    <t>在完全部署所有这些资源之后，BCP团队应当监督恰当的BCP维护程序，以便确保计划能够响应业务需求的发展。</t>
+  </si>
+  <si>
+    <t>培训和教育</t>
+  </si>
+  <si>
+    <t>培训和教育是BCP实现中的一个重要内容。计划中（直接或间接）涉及的所有人都应当接受某些与整个计划和个人职责相关的培训。</t>
+  </si>
+  <si>
+    <t>组织中的每个人都应当接受至少一份计划综述简报，从而使他们具有信心，相信业务领导已经考虑到连续性业务的可能风险，并且制定了计划来缓解对组织的影响。</t>
+  </si>
+  <si>
+    <t>具有直接的BCP职责的人们应当收到培训，对其具体的BCP任务进行评估，确保在灾难发生时他们能够有效地完成其任务。此外，至少应当为每个BCP任务培训一名后补人员，以便确保在人员受伤或危机时刻人员不能到位时的冗余性。</t>
+  </si>
+  <si>
+    <t>BCP文档化</t>
+  </si>
+  <si>
+    <t>确保所有BCP人员都有一个连续性的书面文档，在紧急事件发生时，甚至在资深BCP团队成员不在现场指导时可以作为参考。</t>
+  </si>
+  <si>
+    <r>
+      <t>提供了BCP过程的历史记录，这对于将来人员试图理解不同过程的内因并对计划进行</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>必要的修改</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是有用的。</t>
+    </r>
+  </si>
+  <si>
+    <t>促使团队成员将他们的想法记录到纸上，这个过程常常有助于确定计划中的缺陷。可以像不属于BCP团队的人分发简报，从而进行“理智的分析”。</t>
+  </si>
+  <si>
+    <t>BCP维护、测试和演习</t>
+  </si>
+  <si>
+    <t>BCP文档和计划本身必须是实际使用中的文档。每个组织都会遇到几乎持续的变化，这种动态特性也确保了业务连续性要求随之发生变化。</t>
+  </si>
+  <si>
+    <t>在更新BCP的任何时候，必须进行良好的版本控制。所有旧的BCP版本都应该进行物理销毁，并且被最新版本代替。</t>
+  </si>
+  <si>
+    <t>BCP文档还应当概述一个正式的测试计划，以确保计划是最新的，并且所有人员都接收了充分培训，从而在实际的灾难事件发生时能够履行他们的职责。</t>
+  </si>
+  <si>
+    <t>1.9 协助制定和实施人员安全政策和程序</t>
+  </si>
+  <si>
+    <t>必须高度重视人员安全问题</t>
+  </si>
+  <si>
+    <t>人是信息安全的关键因素</t>
+  </si>
+  <si>
+    <t>大多数重大信息安全事件通常都来自组织内部</t>
+  </si>
+  <si>
+    <t>加强内部人员安全管理的主要措施</t>
+  </si>
+  <si>
+    <t>对工作申请者实施背景检查</t>
+  </si>
+  <si>
+    <t>签署雇佣合同和保密协议</t>
+  </si>
+  <si>
+    <t>加强在职人员的安全管理</t>
+  </si>
+  <si>
+    <t>严格控制人员离职程序</t>
+  </si>
+  <si>
+    <t>人员安全策略和程序</t>
+  </si>
+  <si>
+    <t>职责分离</t>
+  </si>
+  <si>
+    <t>工作职责</t>
+  </si>
+  <si>
+    <t>工作轮换</t>
+  </si>
+  <si>
+    <t>强制休假</t>
+  </si>
+  <si>
+    <r>
+      <t>职责分离属于安全概念，是指把关键的、重要的和敏感的工作任务分配给若干不同的管理员或高级执行者。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>这样能阻止任何一个人具备破坏或削弱重要安全机制的能力</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。可以将职责分离视为对管理员的最小特权原则的应用。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>职责分离也能够防止共谋，共谋是指负面活动由两人或多人共同王城，其意图往往是伪造、偷窃或间谍行为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。</t>
+    </r>
+  </si>
+  <si>
+    <t>工作职责要求员工在常规的基础上执行的特定工作任务。根据他们的职责，员工需要访问各种不同的对象、资源和服务。</t>
+  </si>
+  <si>
+    <t>为了保持最大的安全性，应该按照最小特权原则分配访问权限。</t>
+  </si>
+  <si>
+    <t>最小特权原则规定：在安全环境中，应该授予用户完成工作任务或工作职责所必须的最小访问权限。这条原则的实际应用要求对所有资源和功能进行低级别的粒度访问控制。</t>
+  </si>
+  <si>
+    <t>岗位轮换</t>
+  </si>
+  <si>
+    <t>组织通过让员工在不同的工作岗位间轮换职位来提高整体安全性。</t>
+  </si>
+  <si>
+    <r>
+      <t>知识冗余类型：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>当许多员工中的每一位都有能力胜任所要求的若干工作岗位时，如果因为疾病或其他事件导致一位或多位员工在较长的时间无法工作，那么组织遭受严重停工或生产效率降低的可能性就比较小。</t>
+    </r>
+  </si>
+  <si>
+    <t>人员流动可以减少伪造、数据更改、偷窃、阴谋破坏和信息滥用的风险。岗位轮换也提供了一种同级审计形式，并且能够防止共谋。</t>
+  </si>
+  <si>
+    <t>交叉培训</t>
+  </si>
+  <si>
+    <r>
+      <t>交叉培训被当做岗位轮换的替代方案。在交叉培训时，员工只是做好了完成其他工作的准备；而不是定期轮岗。</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>交叉培训作为一类应急响应程序使现有的其他人员在恰当的员工不能工作时能填补职位空缺。</t>
+    </r>
+  </si>
+  <si>
+    <t>强制性休假</t>
+  </si>
+  <si>
+    <r>
+      <t>用于审计和认证员工的工作任务和特权，此时另一位员工接替其工作。</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>通过这种做法，往往很容易发现滥用、伪造或疏忽行为。</t>
+    </r>
+  </si>
+  <si>
+    <t>雇佣新员工步骤</t>
+  </si>
+  <si>
+    <t>如果没有职责描述，就不能对招聘哪类人员达成共识。因此，制定职责描述是定义域人员相关的安全需求并招聘到新员工的第一步。角色通常与等级特权一致，而职责描述与特定分配的职责和任务相对应</t>
+  </si>
+  <si>
+    <t>候选人筛选及招聘</t>
+  </si>
+  <si>
+    <t>背景检查，可以防止</t>
+  </si>
+  <si>
+    <t>因为人员解雇而导致法律诉讼</t>
+  </si>
+  <si>
+    <t>因为雇佣疏忽而导致第三方的法律诉讼</t>
+  </si>
+  <si>
+    <t>雇佣不合格的人员</t>
+  </si>
+  <si>
+    <t>丧失商业秘密</t>
+  </si>
+  <si>
+    <t>雇佣协议和策略</t>
+  </si>
+  <si>
+    <t>协议文档概略说明了组织的规则和限制、安全策略、可接受的使用和行为准则、详细的工作描述、破坏活动及其后果、要求员工胜任工作所需的时间。</t>
+  </si>
+  <si>
+    <r>
+      <t>保密协议（Non-Disclosure Agreement, NDA）。NDA用来保护组织的机密信息不会被以前的员工泄露。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>当员工签署NDA时，他们同意不对组织外的任何人泄露被定义为机密的信息。违反了NDA的行为尝尝会遭到严厉的触发。</t>
+    </r>
+  </si>
+  <si>
+    <t>入职和离职程序</t>
+  </si>
+  <si>
+    <t>入职是在组织的 IAM（Identify and Access Management, 身份和访问管理）系统中添加新员工的过程。当员工的角色或职位发生变化，或该员工获得其他特权或访问权限时，都可以使用入职流程。</t>
+  </si>
+  <si>
+    <t>离职正好相反，当员工离开公司后，将其身份从 IAM 系统删除</t>
+  </si>
+  <si>
+    <t>离职</t>
+  </si>
+  <si>
+    <t>确保员工已归还交通工具和家中的所有公司设备或用品。</t>
+  </si>
+  <si>
+    <t>删除或禁用员工的网络用户账户。</t>
+  </si>
+  <si>
+    <t>通知人力资源部发放最后的薪资，支付所有未使用假期的折算费用，并终止所有福利待遇。</t>
+  </si>
+  <si>
+    <t>安排一名安全部门人员陪同被解雇员工在工作区域收拾个人物品。</t>
+  </si>
+  <si>
+    <t>通知所有安保人员、巡查人员或监控出入口的人员，以确保前雇员在没有护送的清下无法再次进入办公大楼。</t>
+  </si>
+  <si>
+    <t>供应商、顾问和承包商的协议和控制</t>
+  </si>
+  <si>
+    <r>
+      <t>利用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>SLA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>确保组织向其内部和（或）外部客户提供的各种服务，能够维持在服务提供商和供应商</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>双方达成一致的适当服务水平上</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。</t>
+    </r>
+  </si>
+  <si>
+    <t>SLA 以及供应商、顾问和承包商控制是降低风险和回避风险的一个重要部分。</t>
+  </si>
+  <si>
+    <t>SLA中处理的常见问题</t>
+  </si>
+  <si>
+    <t>系统运行时间（作为总体运行时间的百分比）</t>
+  </si>
+  <si>
+    <t>最长连续停机时间（以秒或分钟等计算）</t>
+  </si>
+  <si>
+    <t>最大负载</t>
+  </si>
+  <si>
+    <t>平均负载</t>
+  </si>
+  <si>
+    <t>诊断任务</t>
+  </si>
+  <si>
+    <t>故障转移时间</t>
+  </si>
+  <si>
+    <t>合规策略要求</t>
+  </si>
+  <si>
+    <t>合规是符合或遵守规则、策略、法规、标准或要求的行为。</t>
+  </si>
+  <si>
+    <t>合规性对安全治理来说是一个重要的问题。在人员层面，合规性涉及的是员工个体是否遵守公司策略以及是否按照定义的程序来执行他们的工作任务。</t>
+  </si>
+  <si>
+    <t>人员层面，合规性涉及的是员工个人是否遵守公司策略以及是否按照定义的程序来执行他们的工作任务。</t>
+  </si>
+  <si>
+    <t>许多组织依靠员工的合规性来保证高质量、一致性、效率和节约成本。如果员工不坚持合规性，组织的利润、市场份额、公认度和声誉可能就会受损。</t>
+  </si>
+  <si>
+    <t>员工需要接受培训，以便知道它们需要做什么；只有这样，如果出现违规或缺乏合规，才可能追究它们的责任。</t>
+  </si>
+  <si>
+    <t>隐私策略要求</t>
+  </si>
+  <si>
+    <t>隐私性定义</t>
+  </si>
+  <si>
+    <t>主动防止对个人可确认的信心（也就是与某人或某个组织直接联系的数据点）的未授权访问。</t>
+  </si>
+  <si>
+    <t>防止对被视为个人的或秘密的信息进行为授权的访问。</t>
+  </si>
+  <si>
+    <t>防止未被同意或知晓的观察、监控或检查行为。</t>
+  </si>
+  <si>
+    <t>无论个人或组织对网上个人隐私性问题的态度如何，都必须在组织的安全策略中被确定。</t>
+  </si>
+  <si>
+    <t>隐私性不仅是外部访问者对提供的联机信息进行访问的问题，而且也是客户、员工、供应商和承包商的问题。如果要收集与个人或公司相关的任何类型信息，那么必须解决隐私性问题。</t>
+  </si>
+  <si>
+    <t>1.10 理解并应用风选管理概念</t>
+  </si>
+  <si>
+    <t>风险和风险管理</t>
+  </si>
+  <si>
+    <t>风险（Risk）</t>
+  </si>
+  <si>
+    <t>指信息资产遭受损坏并给企业带来负面响应的潜在可能性。</t>
+  </si>
+  <si>
+    <t>风险管理（Risk Management）</t>
+  </si>
+  <si>
+    <t>就是识别风险、评估风险、采取措施将风险减少到可接受水平，并维持这个风险水平的过程。风险管理是信息安全管理的核心内容。</t>
+  </si>
+  <si>
+    <t>资产</t>
+  </si>
+  <si>
+    <r>
+      <t>资产是指环境中应该加以保护的任何事务。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>如果组织认为自己控制之下的某种资源有价值并需要保护，那么这种资源就被标记为可以进行风险管理和风险分析。</t>
+    </r>
+  </si>
+  <si>
+    <t>资产出现损失或泄露会危及整体的安全性，造成生产效率的降低，利润的减少、额外支持的增加、组织停工以及造成许多无形的不良后果。</t>
+  </si>
+  <si>
+    <t>威胁</t>
+  </si>
+  <si>
+    <t>任何可能发生的、为组织或某种特定资产带来所不希望的或不想要结果的事情被称为威胁。</t>
+  </si>
+  <si>
+    <t>威胁是指会造成资产损失、破坏、变更、丢失或泄露的任何行为或非行为，或者是阻碍访问或阻止资产维护的行为。</t>
+  </si>
+  <si>
+    <t>脆弱性</t>
+  </si>
+  <si>
+    <r>
+      <t>资产中的弱点或防护措施/对策的缺乏被称为脆弱性</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。</t>
+    </r>
+  </si>
+  <si>
+    <t>脆弱性就是IT基础设施或组织其他方面的缺陷、漏洞、疏忽、错误、局限性、过失或敏感之处。如果脆弱性被他人加以利用，那么就有可能造成资产的破坏或损失。</t>
+  </si>
+  <si>
+    <t>暴露</t>
+  </si>
+  <si>
+    <r>
+      <t>暴露是指由于威胁而容易造成资产损失</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，脆弱性会被或将被威胁主体或威胁事件加以利用的可能性是存在的。</t>
+    </r>
+  </si>
+  <si>
+    <t>暴露并不意味着实施的威胁（造成损失的事件）实际发生，而仅仅是指如果存在脆弱性并且威胁可以利用脆弱性，那么就有可能发生威胁事件或出现潜在的暴露。</t>
+  </si>
+  <si>
+    <t>风险</t>
+  </si>
+  <si>
+    <t>风险是某种威胁利用脆弱性并导致资产损害的可能性、是对可能性、概率或偶然性的评估。</t>
+  </si>
+  <si>
+    <t>风险 = 威胁 * 脆弱性</t>
+  </si>
+  <si>
+    <t>减少威胁主体或脆弱性将直接降低风险发生的几率</t>
+  </si>
+  <si>
+    <t>防护措施</t>
+  </si>
+  <si>
+    <t>防护措施或对策是指能消除脆弱性或对付一种或多种特定威胁的任何方法。</t>
+  </si>
+  <si>
+    <t>防护措施可以使：安装软件补丁程序、修改配置、雇请安排人员、改变IT基础设施、更改流程、改善安全策略、更有效地培训员工等。</t>
+  </si>
+  <si>
+    <t>防护措施可以是通过消除或减少组织内任何位置的威胁或翠荣兴来降低风险的任何行为或产品。防火措施是削弱和消除风险的唯一方法。</t>
+  </si>
+  <si>
+    <t>攻击</t>
+  </si>
+  <si>
+    <t>攻击指的是威胁主体对脆弱性的利用。攻击是任何有意利用组织安全基础设施的脆弱性并导致资产的损害、损失或泄露的企图。攻击还可以被视为违反或未遵守素质安全策略的任何行为。</t>
+  </si>
+  <si>
+    <t>破坏（Breach）</t>
+  </si>
+  <si>
+    <r>
+      <t>破坏指安全机制被威胁主体绕过或阻止。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>当破坏与攻击相结合时，就可能导致渗透或入侵。渗透指威胁主体通过规避安全控制获得对组织基础设施的访问，并能直接危及资产。</t>
+    </r>
+  </si>
+  <si>
+    <t>风险元素相互关系</t>
+  </si>
+  <si>
+    <t>资产、威胁、脆弱性、暴露、风险和防护措施是相互关联的。威胁利用脆弱性，脆弱性导致暴露。暴露就是风险，风险又被防护措施减轻。防护措施保护被威胁危及安全的资产。</t>
+  </si>
+  <si>
+    <t>识别威胁和脆弱性</t>
+  </si>
+  <si>
+    <r>
+      <t>风险管理的一个基本部分就是对威胁进行标识并检查，这涉及创建详尽的组织中认定资产可能存在的所有威胁列表。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>列表中应包括威胁主体和威胁事件。威胁可能来自任何地方，对IT的威胁不只限制在IT源。</t>
+    </r>
+  </si>
+  <si>
+    <t>应该是团队进行风险评估和分析。团队成员应该来自组织内部的不同部门。</t>
+  </si>
+  <si>
+    <t>风险评估/分析</t>
+  </si>
+  <si>
+    <r>
+      <t>上层管理者必须决定哪些风险是可以接受的，哪些风险是不可以接受的。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>决定哪些风险可以接受时，要求详细的、复杂的资产与风险评估。</t>
+    </r>
+  </si>
+  <si>
+    <t>定量的风险分析</t>
+  </si>
+  <si>
+    <t>把真实的货币价值分配给损失的资产。</t>
+  </si>
+  <si>
+    <t>定性的风险分析</t>
+  </si>
+  <si>
+    <t>把主观的和无形的价值分配给损失的资产。</t>
+  </si>
+  <si>
+    <t>对构成风险的各个要素和潜在损失水平赋予数值或货币金额。当度量风险的所有要素（资产价值、威胁频频率、弱点利用程度、安全措施的效率和成本等）都被赋值，风险评估的整个过程和结果就都可以被量化。</t>
+  </si>
+  <si>
+    <t>定量分析有两个关键指标：事件发生的频率（用ARO来表示）和威胁事件可能引起的损失（用EF来表示）</t>
+  </si>
+  <si>
+    <t>分配资产价值（AV）-&gt; 计算暴露因子（EF）-&gt; 计算单一损失期望（SLE）-&gt; 评估年度发生率（ARO）-&gt; 计算年度损失期望（ALE）-&gt;进行防护措施的成本/效益分析</t>
+  </si>
+  <si>
+    <t>定量分析基础概念</t>
+  </si>
+  <si>
+    <r>
+      <t>暴露因子代表组织的某种特定资产被已实施的风险损坏所造成损失的百分比。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>EF表示在发生单个风险时全部资产价值损失的预计值。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>EF被表示为百分数。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>单一损失期望（SLE）是与针对特定资产的单个已实施风险相关联的成本。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>如果某个资产被特定威胁损害，SLE计算对组织造成的确切损失。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>SLE=资产价值（AV）* 暴露因子（EF）</t>
+    </r>
+  </si>
+  <si>
+    <t>年度发生比率（ARO）指的是特定威胁或风险在一年内将会发生的预计频率。</t>
+  </si>
+  <si>
+    <t>年度损失期望（ALE）指的是针对某种特定的资产，所有已实施的威胁每年可能造成的损失成本。ALE = 单一损失期望（SLE）*年发生比率（ARO）</t>
+  </si>
+  <si>
+    <t>定性风险评估</t>
+  </si>
+  <si>
+    <t>很强的主观性，分级如“高、中、低”</t>
+  </si>
+  <si>
+    <t>操作方法如：小组讨论（Delphi）、检查列表、温泉、人员访谈、调查等。</t>
+  </si>
+  <si>
+    <t>操作容易，但因为操作者经验和直觉的偏差而使分析结果失准。</t>
+  </si>
+  <si>
+    <r>
+      <t>准确性稍好，但是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>精确性不够</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。要求分析者具备一定的经验和能力。</t>
+    </r>
+  </si>
+  <si>
+    <t>风险处理</t>
+  </si>
+  <si>
+    <t>风险分析的结果</t>
+  </si>
+  <si>
+    <t>所有资产的完整且详细的评估</t>
+  </si>
+  <si>
+    <t>所有威胁和风险、发生概率以及一旦发生的损失范围的详细列表</t>
+  </si>
+  <si>
+    <t>针对特定威胁的并且标识出有效性与ALE的反骨措施和对策列表</t>
+  </si>
+  <si>
+    <t>每种防护措施的成本/效益分析</t>
+  </si>
+  <si>
+    <t>Risk Mitigation、Risk Assignment、Risk Acceptance、Risk Deterrnece、Risk Avoidence、Risk Rejection</t>
+  </si>
+  <si>
+    <t>风险消减（Risk Mitigation）</t>
+  </si>
+  <si>
+    <r>
+      <t>降低风险或风险消减是一种消除翠荣兴或阻止威胁的防护措施的实施。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>选取性价比好的防御措施是风险管理的一部分，但不是风险评估的元素。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>风险通过消除风险的原因是可以避免的。</t>
+    </r>
+  </si>
+  <si>
+    <t>风险转让（Risk Assignment）</t>
+  </si>
+  <si>
+    <t>风险转让或转移风险是把风险带来的损失转嫁给另外一个实体或组织。购买保险和外包就是转让或转移风险的常见形式。</t>
+  </si>
+  <si>
+    <t>风险接受（Risk Acceptance）</t>
+  </si>
+  <si>
+    <t>风险接受或接受风险是管理层对可能采用的防护措施进行成本/效益分析评估，并且确定对策的成本远远超过风险可能造成的损失的成本。接受风险还意味着管理层已经同意接受风险发生所造成的结果和损失。</t>
+  </si>
+  <si>
+    <t>组织是否接受风险的决定依据与对风险的容忍程度。风险容忍度是组织忍受发生风险所造成的损失的能力，这也是所说的风险容忍和风险偏好。</t>
+  </si>
+  <si>
+    <t>风险威慑（RIsk Deterrence）</t>
+  </si>
+  <si>
+    <t>风险威慑是对可能违反安全和政策的人员实施威慑的过程。</t>
+  </si>
+  <si>
+    <t>安全摄像机、安全警卫等</t>
+  </si>
+  <si>
+    <t>规避风险（RIsk Avoidance）</t>
+  </si>
+  <si>
+    <t>风险规避是选择替代的选项或活动的过程，替代选项或活动的风险低于默认的、通用的、权益的或廉价的选项。</t>
+  </si>
+  <si>
+    <t>风险拒绝（Risk Rejection）</t>
+  </si>
+  <si>
+    <t>最后不可接受的应对措施是拒绝风险或忽略风险。否认存在风险，希望永远不会实现，这都不是对风险的有效或审慎的对策。</t>
+  </si>
+  <si>
+    <t>固有风险（Inherent Risk）</t>
+  </si>
+  <si>
+    <t>固有风险是在执行任何风险管理工作之前，环境、系统或产品中存在的自然、原生或违约风险的水平。</t>
+  </si>
+  <si>
+    <t>由于供应链、开发人员运营、系统的设计和架构或组织的只是和技能基础，可能存在固有风险。</t>
+  </si>
+  <si>
+    <t>固有风险也称为初始风险或起始风险。</t>
+  </si>
+  <si>
+    <t>剩余风险（Residual risk）</t>
+  </si>
+  <si>
+    <t>一旦实施了对策，继续存在的风险就被称为剩余风险。剩余风险是由针对特定资产的任何威胁组成的，高层管理部门选择不对这些资产实施防护措施。剩余风险就是管理侧选择接受而非去缓解的风险。</t>
+  </si>
+  <si>
+    <t>多数情况下，剩余风险的存在表明 成本/效益 分析说明可采用的防护措施不划算。</t>
+  </si>
+  <si>
+    <t>计算总风险的公示是：威胁*脆弱性*资产价值 = 总风险</t>
+  </si>
+  <si>
+    <t>总风险和剩余风险的差额称为控制间隙。控制间隙指通过实施保障措施而减少的风险。计算剩余风险的公示是：总风险 - 控制间隙 = 剩余风险</t>
+  </si>
+  <si>
+    <t>风险实施</t>
+  </si>
+  <si>
+    <r>
+      <t>安全控制、对策和防护措施可以通过行政管理型、逻辑/技术性或物理性控制来实现。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>这三类安全机制以纵深防御的方式来实现，以提供最大化利益。</t>
+    </r>
+  </si>
+  <si>
+    <t>技术性控制</t>
   </si>
 </sst>
 </file>
@@ -2322,10 +3389,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2386,6 +3453,53 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>168910</xdr:colOff>
+      <xdr:row>236</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1227455</xdr:colOff>
+      <xdr:row>240</xdr:row>
+      <xdr:rowOff>259715</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25297130" y="124082810"/>
+          <a:ext cx="7767955" cy="2110105"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2646,12 +3760,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:XFD523"/>
+  <dimension ref="A1:XFD524"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C225" sqref="C225:D225"/>
+      <selection pane="bottomLeft" activeCell="C377" sqref="C377:D377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1"/>
@@ -2660,8 +3774,9 @@
     <col min="2" max="2" width="40.15625" style="1" customWidth="1"/>
     <col min="3" max="3" width="28.7734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="83.3359375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="64.0625" style="1" customWidth="1"/>
-    <col min="6" max="16383" width="41.2734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="67.3125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="52.6015625" style="1" customWidth="1"/>
+    <col min="7" max="16383" width="41.2734375" style="1" customWidth="1"/>
     <col min="16384" max="16384" width="41.2734375" style="2"/>
   </cols>
   <sheetData>
@@ -2713,7 +3828,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" ht="51" spans="1:6">
+    <row r="4" spans="1:6">
       <c r="A4" s="5"/>
       <c r="B4" s="10"/>
       <c r="C4" s="9" t="s">
@@ -2783,7 +3898,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" ht="68" spans="1:6">
+    <row r="10" ht="51" spans="1:6">
       <c r="A10" s="5"/>
       <c r="B10" s="10"/>
       <c r="C10" s="9" t="s">
@@ -3961,7 +5076,7 @@
       <c r="C114" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="D114" s="33" t="s">
+      <c r="D114" s="20" t="s">
         <v>191</v>
       </c>
       <c r="E114" s="5"/>
@@ -4791,7 +5906,7 @@
       <c r="A187" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="B187" s="16" t="s">
+      <c r="B187" s="13" t="s">
         <v>304</v>
       </c>
       <c r="C187" s="19" t="s">
@@ -4804,7 +5919,7 @@
     </row>
     <row r="188" s="1" customFormat="1" ht="55" customHeight="1" spans="1:16384">
       <c r="A188" s="5"/>
-      <c r="B188" s="18"/>
+      <c r="B188" s="15"/>
       <c r="C188" s="19" t="s">
         <v>306</v>
       </c>
@@ -4815,7 +5930,7 @@
     </row>
     <row r="189" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A189" s="5"/>
-      <c r="B189" s="16" t="s">
+      <c r="B189" s="13" t="s">
         <v>307</v>
       </c>
       <c r="C189" s="19" t="s">
@@ -4828,7 +5943,7 @@
     </row>
     <row r="190" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A190" s="5"/>
-      <c r="B190" s="17"/>
+      <c r="B190" s="14"/>
       <c r="C190" s="19" t="s">
         <v>309</v>
       </c>
@@ -4839,7 +5954,7 @@
     </row>
     <row r="191" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A191" s="5"/>
-      <c r="B191" s="17"/>
+      <c r="B191" s="14"/>
       <c r="C191" s="19" t="s">
         <v>310</v>
       </c>
@@ -4850,7 +5965,7 @@
     </row>
     <row r="192" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A192" s="5"/>
-      <c r="B192" s="17"/>
+      <c r="B192" s="14"/>
       <c r="C192" s="19" t="s">
         <v>311</v>
       </c>
@@ -4861,7 +5976,7 @@
     </row>
     <row r="193" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A193" s="5"/>
-      <c r="B193" s="17"/>
+      <c r="B193" s="14"/>
       <c r="C193" s="19" t="s">
         <v>312</v>
       </c>
@@ -4872,7 +5987,7 @@
     </row>
     <row r="194" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A194" s="5"/>
-      <c r="B194" s="17"/>
+      <c r="B194" s="14"/>
       <c r="C194" s="19" t="s">
         <v>313</v>
       </c>
@@ -4883,7 +5998,7 @@
     </row>
     <row r="195" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A195" s="5"/>
-      <c r="B195" s="18"/>
+      <c r="B195" s="15"/>
       <c r="C195" s="19" t="s">
         <v>314</v>
       </c>
@@ -4894,7 +6009,7 @@
     </row>
     <row r="196" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A196" s="5"/>
-      <c r="B196" s="16" t="s">
+      <c r="B196" s="13" t="s">
         <v>315</v>
       </c>
       <c r="C196" s="19" t="s">
@@ -4907,7 +6022,7 @@
     </row>
     <row r="197" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A197" s="5"/>
-      <c r="B197" s="17"/>
+      <c r="B197" s="14"/>
       <c r="C197" s="19" t="s">
         <v>317</v>
       </c>
@@ -4918,7 +6033,7 @@
     </row>
     <row r="198" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A198" s="5"/>
-      <c r="B198" s="17"/>
+      <c r="B198" s="14"/>
       <c r="C198" s="19" t="s">
         <v>318</v>
       </c>
@@ -4929,7 +6044,7 @@
     </row>
     <row r="199" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A199" s="5"/>
-      <c r="B199" s="17"/>
+      <c r="B199" s="14"/>
       <c r="C199" s="19" t="s">
         <v>319</v>
       </c>
@@ -4940,7 +6055,7 @@
     </row>
     <row r="200" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A200" s="5"/>
-      <c r="B200" s="17"/>
+      <c r="B200" s="14"/>
       <c r="C200" s="19" t="s">
         <v>320</v>
       </c>
@@ -4951,7 +6066,7 @@
     </row>
     <row r="201" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A201" s="5"/>
-      <c r="B201" s="17"/>
+      <c r="B201" s="14"/>
       <c r="C201" s="19" t="s">
         <v>321</v>
       </c>
@@ -4962,7 +6077,7 @@
     </row>
     <row r="202" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A202" s="5"/>
-      <c r="B202" s="17"/>
+      <c r="B202" s="14"/>
       <c r="C202" s="19" t="s">
         <v>322</v>
       </c>
@@ -4973,7 +6088,7 @@
     </row>
     <row r="203" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A203" s="5"/>
-      <c r="B203" s="17"/>
+      <c r="B203" s="14"/>
       <c r="C203" s="19" t="s">
         <v>323</v>
       </c>
@@ -4984,7 +6099,7 @@
     </row>
     <row r="204" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A204" s="5"/>
-      <c r="B204" s="17"/>
+      <c r="B204" s="14"/>
       <c r="C204" s="19" t="s">
         <v>324</v>
       </c>
@@ -4995,7 +6110,7 @@
     </row>
     <row r="205" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A205" s="5"/>
-      <c r="B205" s="18"/>
+      <c r="B205" s="15"/>
       <c r="C205" s="19" t="s">
         <v>325</v>
       </c>
@@ -5006,7 +6121,7 @@
     </row>
     <row r="206" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A206" s="5"/>
-      <c r="B206" s="16" t="s">
+      <c r="B206" s="13" t="s">
         <v>304</v>
       </c>
       <c r="C206" s="16" t="s">
@@ -5021,7 +6136,7 @@
     </row>
     <row r="207" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A207" s="5"/>
-      <c r="B207" s="17"/>
+      <c r="B207" s="14"/>
       <c r="C207" s="17"/>
       <c r="D207" s="5" t="s">
         <v>328</v>
@@ -5032,7 +6147,7 @@
     </row>
     <row r="208" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A208" s="5"/>
-      <c r="B208" s="17"/>
+      <c r="B208" s="14"/>
       <c r="C208" s="17"/>
       <c r="D208" s="5" t="s">
         <v>329</v>
@@ -5043,7 +6158,7 @@
     </row>
     <row r="209" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A209" s="5"/>
-      <c r="B209" s="17"/>
+      <c r="B209" s="14"/>
       <c r="C209" s="18"/>
       <c r="D209" s="5" t="s">
         <v>330</v>
@@ -5054,7 +6169,7 @@
     </row>
     <row r="210" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A210" s="5"/>
-      <c r="B210" s="18"/>
+      <c r="B210" s="15"/>
       <c r="C210" s="19" t="s">
         <v>331</v>
       </c>
@@ -5065,7 +6180,7 @@
     </row>
     <row r="211" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A211" s="5"/>
-      <c r="B211" s="16" t="s">
+      <c r="B211" s="13" t="s">
         <v>327</v>
       </c>
       <c r="C211" s="19" t="s">
@@ -5078,7 +6193,7 @@
     </row>
     <row r="212" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A212" s="5"/>
-      <c r="B212" s="17"/>
+      <c r="B212" s="14"/>
       <c r="C212" s="19" t="s">
         <v>333</v>
       </c>
@@ -5089,7 +6204,7 @@
     </row>
     <row r="213" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A213" s="5"/>
-      <c r="B213" s="17"/>
+      <c r="B213" s="14"/>
       <c r="C213" s="19" t="s">
         <v>334</v>
       </c>
@@ -5100,7 +6215,7 @@
     </row>
     <row r="214" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A214" s="5"/>
-      <c r="B214" s="18"/>
+      <c r="B214" s="15"/>
       <c r="C214" s="19" t="s">
         <v>335</v>
       </c>
@@ -5111,7 +6226,7 @@
     </row>
     <row r="215" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A215" s="5"/>
-      <c r="B215" s="16" t="s">
+      <c r="B215" s="13" t="s">
         <v>336</v>
       </c>
       <c r="C215" s="19" t="s">
@@ -5124,7 +6239,7 @@
     </row>
     <row r="216" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A216" s="5"/>
-      <c r="B216" s="17"/>
+      <c r="B216" s="14"/>
       <c r="C216" s="19" t="s">
         <v>338</v>
       </c>
@@ -5135,7 +6250,7 @@
     </row>
     <row r="217" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A217" s="5"/>
-      <c r="B217" s="17"/>
+      <c r="B217" s="14"/>
       <c r="C217" s="19" t="s">
         <v>339</v>
       </c>
@@ -5146,7 +6261,7 @@
     </row>
     <row r="218" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A218" s="5"/>
-      <c r="B218" s="18"/>
+      <c r="B218" s="15"/>
       <c r="C218" s="19" t="s">
         <v>340</v>
       </c>
@@ -5157,7 +6272,7 @@
     </row>
     <row r="219" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A219" s="5"/>
-      <c r="B219" s="16" t="s">
+      <c r="B219" s="13" t="s">
         <v>341</v>
       </c>
       <c r="C219" s="19" t="s">
@@ -5170,7 +6285,7 @@
     </row>
     <row r="220" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A220" s="5"/>
-      <c r="B220" s="17"/>
+      <c r="B220" s="14"/>
       <c r="C220" s="19" t="s">
         <v>343</v>
       </c>
@@ -5181,7 +6296,7 @@
     </row>
     <row r="221" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A221" s="5"/>
-      <c r="B221" s="17"/>
+      <c r="B221" s="14"/>
       <c r="C221" s="19" t="s">
         <v>344</v>
       </c>
@@ -5192,7 +6307,7 @@
     </row>
     <row r="222" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A222" s="5"/>
-      <c r="B222" s="17"/>
+      <c r="B222" s="14"/>
       <c r="C222" s="19" t="s">
         <v>345</v>
       </c>
@@ -5203,7 +6318,7 @@
     </row>
     <row r="223" s="1" customFormat="1" customHeight="1" spans="1:16384">
       <c r="A223" s="5"/>
-      <c r="B223" s="17"/>
+      <c r="B223" s="14"/>
       <c r="C223" s="19" t="s">
         <v>346</v>
       </c>
@@ -5212,8 +6327,9 @@
       <c r="F223" s="5"/>
       <c r="XFD223" s="2"/>
     </row>
-    <row r="224" ht="38" customHeight="1" spans="2:6">
-      <c r="B224" s="17"/>
+    <row r="224" ht="38" customHeight="1" spans="1:6">
+      <c r="A224" s="5"/>
+      <c r="B224" s="14"/>
       <c r="C224" s="19" t="s">
         <v>347</v>
       </c>
@@ -5222,8 +6338,8 @@
       <c r="F224" s="5"/>
     </row>
     <row r="225" ht="38" customHeight="1" spans="1:6">
-      <c r="A225"/>
-      <c r="B225" s="17"/>
+      <c r="A225" s="5"/>
+      <c r="B225" s="14"/>
       <c r="C225" s="19" t="s">
         <v>348</v>
       </c>
@@ -5231,8 +6347,9 @@
       <c r="E225" s="5"/>
       <c r="F225" s="5"/>
     </row>
-    <row r="226" ht="38" customHeight="1" spans="2:6">
-      <c r="B226" s="17"/>
+    <row r="226" ht="38" customHeight="1" spans="1:6">
+      <c r="A226" s="5"/>
+      <c r="B226" s="14"/>
       <c r="C226" s="19" t="s">
         <v>349</v>
       </c>
@@ -5240,8 +6357,9 @@
       <c r="E226" s="5"/>
       <c r="F226" s="5"/>
     </row>
-    <row r="227" ht="38" customHeight="1" spans="2:6">
-      <c r="B227" s="18"/>
+    <row r="227" ht="38" customHeight="1" spans="1:6">
+      <c r="A227" s="5"/>
+      <c r="B227" s="15"/>
       <c r="C227" s="19" t="s">
         <v>350</v>
       </c>
@@ -5249,8 +6367,9 @@
       <c r="E227" s="5"/>
       <c r="F227" s="5"/>
     </row>
-    <row r="228" ht="38" customHeight="1" spans="2:6">
-      <c r="B228" s="5" t="s">
+    <row r="228" ht="38" customHeight="1" spans="1:6">
+      <c r="A228" s="5"/>
+      <c r="B228" s="26" t="s">
         <v>351</v>
       </c>
       <c r="C228" s="27" t="s">
@@ -5260,8 +6379,9 @@
       <c r="E228" s="5"/>
       <c r="F228" s="5"/>
     </row>
-    <row r="229" ht="38" customHeight="1" spans="2:6">
-      <c r="B229" s="5" t="s">
+    <row r="229" ht="38" customHeight="1" spans="1:6">
+      <c r="A229" s="5"/>
+      <c r="B229" s="26" t="s">
         <v>353</v>
       </c>
       <c r="C229" s="19" t="s">
@@ -5271,1080 +6391,1646 @@
       <c r="E229" s="5"/>
       <c r="F229" s="5"/>
     </row>
-    <row r="230" ht="38" customHeight="1" spans="2:6">
-      <c r="B230" s="5"/>
-      <c r="C230" s="19"/>
+    <row r="230" ht="38" customHeight="1" spans="1:6">
+      <c r="A230" s="5"/>
+      <c r="B230" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="C230" s="19" t="s">
+        <v>356</v>
+      </c>
       <c r="D230" s="20"/>
       <c r="E230" s="5"/>
       <c r="F230" s="5"/>
     </row>
-    <row r="231" ht="38" customHeight="1" spans="2:6">
-      <c r="B231" s="5"/>
-      <c r="C231" s="19"/>
+    <row r="231" ht="38" customHeight="1" spans="1:6">
+      <c r="A231" s="5"/>
+      <c r="B231" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="C231" s="19" t="s">
+        <v>358</v>
+      </c>
       <c r="D231" s="20"/>
       <c r="E231" s="5"/>
       <c r="F231" s="5"/>
     </row>
-    <row r="232" ht="38" customHeight="1" spans="2:6">
-      <c r="B232" s="5"/>
-      <c r="C232" s="19"/>
+    <row r="232" ht="38" customHeight="1" spans="1:6">
+      <c r="A232" s="5"/>
+      <c r="B232" s="14"/>
+      <c r="C232" s="21" t="s">
+        <v>359</v>
+      </c>
       <c r="D232" s="20"/>
       <c r="E232" s="5"/>
       <c r="F232" s="5"/>
     </row>
-    <row r="233" ht="38" customHeight="1" spans="2:6">
-      <c r="B233" s="5"/>
-      <c r="C233" s="19"/>
-      <c r="D233" s="20"/>
+    <row r="233" ht="38" customHeight="1" spans="1:6">
+      <c r="A233" s="5"/>
+      <c r="B233" s="14"/>
+      <c r="C233" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="D233" s="5" t="s">
+        <v>361</v>
+      </c>
       <c r="E233" s="5"/>
       <c r="F233" s="5"/>
     </row>
-    <row r="234" ht="38" customHeight="1" spans="2:6">
-      <c r="B234" s="5"/>
-      <c r="C234" s="19"/>
-      <c r="D234" s="20"/>
-      <c r="E234" s="5"/>
+    <row r="234" ht="38" customHeight="1" spans="1:6">
+      <c r="A234" s="5"/>
+      <c r="B234" s="15"/>
+      <c r="C234" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="D234" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="E234" s="5" t="s">
+        <v>364</v>
+      </c>
       <c r="F234" s="5"/>
     </row>
     <row r="235" ht="38" customHeight="1" spans="1:6">
-      <c r="A235"/>
-      <c r="B235" s="5"/>
-      <c r="C235" s="19"/>
+      <c r="A235" s="5"/>
+      <c r="B235" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="C235" s="21" t="s">
+        <v>366</v>
+      </c>
       <c r="D235" s="20"/>
       <c r="E235" s="5"/>
       <c r="F235" s="5"/>
     </row>
-    <row r="236" ht="38" customHeight="1" spans="2:6">
-      <c r="B236" s="5"/>
-      <c r="C236" s="19"/>
+    <row r="236" ht="38" customHeight="1" spans="1:6">
+      <c r="A236" s="5"/>
+      <c r="B236" s="14"/>
+      <c r="C236" s="19" t="s">
+        <v>367</v>
+      </c>
       <c r="D236" s="20"/>
       <c r="E236" s="5"/>
       <c r="F236" s="5"/>
     </row>
-    <row r="237" ht="38" customHeight="1" spans="2:6">
-      <c r="B237" s="5"/>
-      <c r="C237" s="19"/>
+    <row r="237" ht="38" customHeight="1" spans="1:6">
+      <c r="A237" s="5"/>
+      <c r="B237" s="15"/>
+      <c r="C237" s="19" t="s">
+        <v>368</v>
+      </c>
       <c r="D237" s="20"/>
       <c r="E237" s="5"/>
       <c r="F237" s="5"/>
     </row>
-    <row r="238" ht="38" customHeight="1" spans="2:6">
-      <c r="B238" s="5"/>
-      <c r="C238" s="19"/>
-      <c r="D238" s="20"/>
-      <c r="E238" s="5"/>
+    <row r="238" ht="38" customHeight="1" spans="1:6">
+      <c r="A238" s="5"/>
+      <c r="B238" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="C238" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="D238" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="E238" s="5" t="s">
+        <v>372</v>
+      </c>
       <c r="F238" s="5"/>
     </row>
-    <row r="239" ht="38" customHeight="1" spans="2:6">
-      <c r="B239" s="5"/>
-      <c r="C239" s="19"/>
-      <c r="D239" s="20"/>
+    <row r="239" ht="38" customHeight="1" spans="1:6">
+      <c r="A239" s="5"/>
+      <c r="B239" s="14"/>
+      <c r="C239" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="D239" s="5" t="s">
+        <v>374</v>
+      </c>
       <c r="E239" s="5"/>
       <c r="F239" s="5"/>
     </row>
-    <row r="240" ht="38" customHeight="1" spans="2:6">
-      <c r="B240" s="5"/>
-      <c r="C240" s="19"/>
-      <c r="D240" s="20"/>
+    <row r="240" ht="38" customHeight="1" spans="1:6">
+      <c r="A240" s="5"/>
+      <c r="B240" s="15"/>
+      <c r="C240" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="D240" s="5" t="s">
+        <v>376</v>
+      </c>
       <c r="E240" s="5"/>
       <c r="F240" s="5"/>
     </row>
-    <row r="241" ht="38" customHeight="1" spans="2:6">
-      <c r="B241" s="5"/>
-      <c r="C241" s="19"/>
+    <row r="241" ht="38" customHeight="1" spans="1:6">
+      <c r="A241" s="5"/>
+      <c r="B241" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="C241" s="19" t="s">
+        <v>378</v>
+      </c>
       <c r="D241" s="20"/>
       <c r="E241" s="5"/>
       <c r="F241" s="5"/>
     </row>
-    <row r="242" ht="38" customHeight="1" spans="2:6">
-      <c r="B242" s="5"/>
-      <c r="C242" s="19"/>
+    <row r="242" ht="38" customHeight="1" spans="1:6">
+      <c r="A242" s="5"/>
+      <c r="B242" s="15"/>
+      <c r="C242" s="19" t="s">
+        <v>379</v>
+      </c>
       <c r="D242" s="20"/>
       <c r="E242" s="5"/>
       <c r="F242" s="5"/>
     </row>
-    <row r="243" ht="38" customHeight="1" spans="2:6">
-      <c r="B243" s="5"/>
-      <c r="C243" s="19"/>
+    <row r="243" ht="38" customHeight="1" spans="1:6">
+      <c r="A243" s="5"/>
+      <c r="B243" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="C243" s="21" t="s">
+        <v>381</v>
+      </c>
       <c r="D243" s="20"/>
       <c r="E243" s="5"/>
       <c r="F243" s="5"/>
     </row>
-    <row r="244" ht="38" customHeight="1" spans="2:6">
-      <c r="B244" s="5"/>
-      <c r="C244" s="19"/>
+    <row r="244" ht="38" customHeight="1" spans="1:6">
+      <c r="A244" s="5"/>
+      <c r="B244" s="14"/>
+      <c r="C244" s="19" t="s">
+        <v>382</v>
+      </c>
       <c r="D244" s="20"/>
       <c r="E244" s="5"/>
       <c r="F244" s="5"/>
     </row>
     <row r="245" ht="38" customHeight="1" spans="1:6">
-      <c r="A245"/>
-      <c r="B245" s="5"/>
-      <c r="C245" s="19"/>
+      <c r="A245" s="5"/>
+      <c r="B245" s="15"/>
+      <c r="C245" s="19" t="s">
+        <v>383</v>
+      </c>
       <c r="D245" s="20"/>
       <c r="E245" s="5"/>
       <c r="F245" s="5"/>
     </row>
-    <row r="246" ht="38" customHeight="1" spans="2:6">
-      <c r="B246" s="5"/>
-      <c r="C246" s="19"/>
+    <row r="246" ht="38" customHeight="1" spans="1:6">
+      <c r="A246" s="5"/>
+      <c r="B246" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="C246" s="19" t="s">
+        <v>385</v>
+      </c>
       <c r="D246" s="20"/>
       <c r="E246" s="5"/>
       <c r="F246" s="5"/>
     </row>
-    <row r="247" ht="38" customHeight="1" spans="2:6">
-      <c r="B247" s="5"/>
-      <c r="C247" s="19"/>
+    <row r="247" ht="38" customHeight="1" spans="1:6">
+      <c r="A247" s="5"/>
+      <c r="B247" s="15"/>
+      <c r="C247" s="21" t="s">
+        <v>386</v>
+      </c>
       <c r="D247" s="20"/>
       <c r="E247" s="5"/>
       <c r="F247" s="5"/>
     </row>
-    <row r="248" ht="38" customHeight="1" spans="2:6">
-      <c r="B248" s="5"/>
-      <c r="C248" s="19"/>
+    <row r="248" ht="38" customHeight="1" spans="1:6">
+      <c r="A248" s="5"/>
+      <c r="B248" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="C248" s="27" t="s">
+        <v>388</v>
+      </c>
       <c r="D248" s="20"/>
-      <c r="E248" s="5"/>
+      <c r="E248" s="5" t="s">
+        <v>389</v>
+      </c>
       <c r="F248" s="5"/>
     </row>
-    <row r="249" ht="38" customHeight="1" spans="2:6">
-      <c r="B249" s="5"/>
-      <c r="C249" s="19"/>
+    <row r="249" ht="38" customHeight="1" spans="1:6">
+      <c r="A249" s="5"/>
+      <c r="B249" s="26" t="s">
+        <v>390</v>
+      </c>
+      <c r="C249" s="27" t="s">
+        <v>391</v>
+      </c>
       <c r="D249" s="20"/>
-      <c r="E249" s="5"/>
-      <c r="F249" s="5"/>
-    </row>
-    <row r="250" ht="38" customHeight="1" spans="2:6">
-      <c r="B250" s="5"/>
-      <c r="C250" s="19"/>
+      <c r="E249" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="F249" s="5" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="250" ht="38" customHeight="1" spans="1:6">
+      <c r="A250" s="5"/>
+      <c r="B250" s="26" t="s">
+        <v>394</v>
+      </c>
+      <c r="C250" s="19" t="s">
+        <v>395</v>
+      </c>
       <c r="D250" s="20"/>
-      <c r="E250" s="5"/>
+      <c r="E250" s="5" t="s">
+        <v>396</v>
+      </c>
       <c r="F250" s="5"/>
     </row>
-    <row r="251" ht="38" customHeight="1" spans="2:6">
-      <c r="B251" s="5"/>
-      <c r="C251" s="19"/>
+    <row r="251" ht="38" customHeight="1" spans="1:6">
+      <c r="A251" s="5"/>
+      <c r="B251" s="13" t="s">
+        <v>397</v>
+      </c>
+      <c r="C251" s="19" t="s">
+        <v>398</v>
+      </c>
       <c r="D251" s="20"/>
       <c r="E251" s="5"/>
       <c r="F251" s="5"/>
     </row>
-    <row r="252" ht="38" customHeight="1" spans="2:6">
-      <c r="B252" s="5"/>
-      <c r="C252" s="19"/>
+    <row r="252" ht="38" customHeight="1" spans="1:6">
+      <c r="A252" s="5"/>
+      <c r="B252" s="15"/>
+      <c r="C252" s="19" t="s">
+        <v>399</v>
+      </c>
       <c r="D252" s="20"/>
       <c r="E252" s="5"/>
       <c r="F252" s="5"/>
     </row>
-    <row r="253" ht="38" customHeight="1" spans="2:6">
-      <c r="B253" s="5"/>
-      <c r="C253" s="19"/>
+    <row r="253" ht="38" customHeight="1" spans="1:6">
+      <c r="A253" s="5"/>
+      <c r="B253" s="13" t="s">
+        <v>400</v>
+      </c>
+      <c r="C253" s="21" t="s">
+        <v>401</v>
+      </c>
       <c r="D253" s="20"/>
       <c r="E253" s="5"/>
       <c r="F253" s="5"/>
     </row>
-    <row r="254" ht="38" customHeight="1" spans="2:6">
-      <c r="B254" s="5"/>
-      <c r="C254" s="19"/>
+    <row r="254" ht="38" customHeight="1" spans="1:6">
+      <c r="A254" s="5"/>
+      <c r="B254" s="15"/>
+      <c r="C254" s="21" t="s">
+        <v>402</v>
+      </c>
       <c r="D254" s="20"/>
       <c r="E254" s="5"/>
       <c r="F254" s="5"/>
     </row>
     <row r="255" ht="38" customHeight="1" spans="1:6">
-      <c r="A255"/>
-      <c r="B255" s="5"/>
-      <c r="C255" s="19"/>
+      <c r="A255" s="5"/>
+      <c r="B255" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="C255" s="27" t="s">
+        <v>403</v>
+      </c>
       <c r="D255" s="20"/>
       <c r="E255" s="5"/>
       <c r="F255" s="5"/>
     </row>
-    <row r="256" ht="38" customHeight="1" spans="2:6">
-      <c r="B256" s="5"/>
-      <c r="C256" s="19"/>
+    <row r="256" ht="38" customHeight="1" spans="1:6">
+      <c r="A256" s="5"/>
+      <c r="B256" s="15"/>
+      <c r="C256" s="27" t="s">
+        <v>404</v>
+      </c>
       <c r="D256" s="20"/>
-      <c r="E256" s="5"/>
+      <c r="E256" s="5" t="s">
+        <v>405</v>
+      </c>
       <c r="F256" s="5"/>
     </row>
-    <row r="257" ht="38" customHeight="1" spans="2:6">
-      <c r="B257" s="5"/>
-      <c r="C257" s="19"/>
+    <row r="257" ht="38" customHeight="1" spans="1:6">
+      <c r="A257" s="5"/>
+      <c r="B257" s="13" t="s">
+        <v>406</v>
+      </c>
+      <c r="C257" s="19" t="s">
+        <v>407</v>
+      </c>
       <c r="D257" s="20"/>
       <c r="E257" s="5"/>
       <c r="F257" s="5"/>
     </row>
-    <row r="258" ht="38" customHeight="1" spans="2:6">
-      <c r="B258" s="5"/>
-      <c r="C258" s="19"/>
+    <row r="258" ht="38" customHeight="1" spans="1:6">
+      <c r="A258" s="5"/>
+      <c r="B258" s="14"/>
+      <c r="C258" s="21" t="s">
+        <v>408</v>
+      </c>
       <c r="D258" s="20"/>
       <c r="E258" s="5"/>
       <c r="F258" s="5"/>
     </row>
-    <row r="259" ht="38" customHeight="1" spans="2:6">
-      <c r="B259" s="5"/>
-      <c r="C259" s="19"/>
+    <row r="259" ht="38" customHeight="1" spans="1:6">
+      <c r="A259" s="5"/>
+      <c r="B259" s="15"/>
+      <c r="C259" s="19" t="s">
+        <v>409</v>
+      </c>
       <c r="D259" s="20"/>
       <c r="E259" s="5"/>
       <c r="F259" s="5"/>
     </row>
-    <row r="260" ht="38" customHeight="1" spans="2:6">
-      <c r="B260" s="5"/>
-      <c r="C260" s="19"/>
+    <row r="260" ht="38" customHeight="1" spans="1:6">
+      <c r="A260" s="5"/>
+      <c r="B260" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="C260" s="19" t="s">
+        <v>411</v>
+      </c>
       <c r="D260" s="20"/>
       <c r="E260" s="5"/>
       <c r="F260" s="5"/>
     </row>
-    <row r="261" ht="38" customHeight="1" spans="2:6">
-      <c r="B261" s="5"/>
-      <c r="C261" s="19"/>
-      <c r="D261" s="20"/>
+    <row r="261" ht="38" customHeight="1" spans="1:6">
+      <c r="A261" s="5"/>
+      <c r="B261" s="14"/>
+      <c r="C261" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="D261" s="5" t="s">
+        <v>413</v>
+      </c>
       <c r="E261" s="5"/>
       <c r="F261" s="5"/>
     </row>
-    <row r="262" ht="38" customHeight="1" spans="2:6">
-      <c r="B262" s="5"/>
-      <c r="C262" s="19"/>
-      <c r="D262" s="20"/>
+    <row r="262" ht="38" customHeight="1" spans="1:6">
+      <c r="A262" s="5"/>
+      <c r="B262" s="14"/>
+      <c r="C262" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="D262" s="5" t="s">
+        <v>415</v>
+      </c>
       <c r="E262" s="5"/>
       <c r="F262" s="5"/>
     </row>
-    <row r="263" ht="38" customHeight="1" spans="2:6">
-      <c r="B263" s="5"/>
-      <c r="C263" s="19"/>
-      <c r="D263" s="20"/>
+    <row r="263" ht="38" customHeight="1" spans="1:6">
+      <c r="A263" s="5"/>
+      <c r="B263" s="15"/>
+      <c r="C263" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="D263" s="5" t="s">
+        <v>417</v>
+      </c>
       <c r="E263" s="5"/>
       <c r="F263" s="5"/>
     </row>
-    <row r="264" ht="38" customHeight="1" spans="2:6">
-      <c r="B264" s="5"/>
-      <c r="C264" s="19"/>
+    <row r="264" ht="38" customHeight="1" spans="1:6">
+      <c r="A264" s="5"/>
+      <c r="B264" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="C264" s="19" t="s">
+        <v>419</v>
+      </c>
       <c r="D264" s="20"/>
       <c r="E264" s="5"/>
       <c r="F264" s="5"/>
     </row>
     <row r="265" ht="38" customHeight="1" spans="1:6">
-      <c r="A265"/>
-      <c r="B265" s="5"/>
-      <c r="C265" s="19"/>
+      <c r="A265" s="5"/>
+      <c r="B265" s="14"/>
+      <c r="C265" s="19" t="s">
+        <v>420</v>
+      </c>
       <c r="D265" s="20"/>
       <c r="E265" s="5"/>
       <c r="F265" s="5"/>
     </row>
-    <row r="266" ht="38" customHeight="1" spans="2:6">
-      <c r="B266" s="5"/>
-      <c r="C266" s="19"/>
+    <row r="266" ht="38" customHeight="1" spans="1:6">
+      <c r="A266" s="5"/>
+      <c r="B266" s="15"/>
+      <c r="C266" s="19" t="s">
+        <v>421</v>
+      </c>
       <c r="D266" s="20"/>
       <c r="E266" s="5"/>
       <c r="F266" s="5"/>
     </row>
-    <row r="267" ht="38" customHeight="1" spans="2:6">
-      <c r="B267" s="5"/>
-      <c r="C267" s="19"/>
+    <row r="267" ht="38" customHeight="1" spans="1:6">
+      <c r="A267" s="5"/>
+      <c r="B267" s="13" t="s">
+        <v>422</v>
+      </c>
+      <c r="C267" s="19" t="s">
+        <v>423</v>
+      </c>
       <c r="D267" s="20"/>
       <c r="E267" s="5"/>
       <c r="F267" s="5"/>
     </row>
-    <row r="268" ht="38" customHeight="1" spans="2:6">
-      <c r="B268" s="5"/>
-      <c r="C268" s="19"/>
+    <row r="268" ht="38" customHeight="1" spans="1:6">
+      <c r="A268" s="5"/>
+      <c r="B268" s="14"/>
+      <c r="C268" s="19" t="s">
+        <v>424</v>
+      </c>
       <c r="D268" s="20"/>
       <c r="E268" s="5"/>
       <c r="F268" s="5"/>
     </row>
-    <row r="269" ht="38" customHeight="1" spans="2:6">
-      <c r="B269" s="5"/>
-      <c r="C269" s="19"/>
+    <row r="269" ht="38" customHeight="1" spans="1:6">
+      <c r="A269" s="5"/>
+      <c r="B269" s="15"/>
+      <c r="C269" s="19" t="s">
+        <v>425</v>
+      </c>
       <c r="D269" s="20"/>
       <c r="E269" s="5"/>
       <c r="F269" s="5"/>
     </row>
-    <row r="270" ht="38" customHeight="1" spans="2:6">
-      <c r="B270" s="5"/>
-      <c r="C270" s="19"/>
+    <row r="270" ht="38" customHeight="1" spans="1:6">
+      <c r="A270" s="5"/>
+      <c r="B270" s="13" t="s">
+        <v>426</v>
+      </c>
+      <c r="C270" s="19" t="s">
+        <v>427</v>
+      </c>
       <c r="D270" s="20"/>
       <c r="E270" s="5"/>
       <c r="F270" s="5"/>
     </row>
-    <row r="271" ht="38" customHeight="1" spans="2:6">
-      <c r="B271" s="5"/>
-      <c r="C271" s="19"/>
+    <row r="271" ht="38" customHeight="1" spans="1:6">
+      <c r="A271" s="5"/>
+      <c r="B271" s="14"/>
+      <c r="C271" s="27" t="s">
+        <v>428</v>
+      </c>
       <c r="D271" s="20"/>
       <c r="E271" s="5"/>
       <c r="F271" s="5"/>
     </row>
-    <row r="272" ht="38" customHeight="1" spans="2:6">
-      <c r="B272" s="5"/>
-      <c r="C272" s="19"/>
+    <row r="272" ht="38" customHeight="1" spans="1:6">
+      <c r="A272" s="5"/>
+      <c r="B272" s="15"/>
+      <c r="C272" s="19" t="s">
+        <v>429</v>
+      </c>
       <c r="D272" s="20"/>
       <c r="E272" s="5"/>
       <c r="F272" s="5"/>
     </row>
-    <row r="273" ht="38" customHeight="1" spans="2:6">
-      <c r="B273" s="5"/>
-      <c r="C273" s="19"/>
+    <row r="273" ht="38" customHeight="1" spans="1:6">
+      <c r="A273" s="5"/>
+      <c r="B273" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="C273" s="19" t="s">
+        <v>431</v>
+      </c>
       <c r="D273" s="20"/>
       <c r="E273" s="5"/>
       <c r="F273" s="5"/>
     </row>
-    <row r="274" ht="38" customHeight="1" spans="2:6">
-      <c r="B274" s="5"/>
-      <c r="C274" s="19"/>
+    <row r="274" ht="38" customHeight="1" spans="1:6">
+      <c r="A274" s="5"/>
+      <c r="B274" s="14"/>
+      <c r="C274" s="19" t="s">
+        <v>432</v>
+      </c>
       <c r="D274" s="20"/>
       <c r="E274" s="5"/>
       <c r="F274" s="5"/>
     </row>
     <row r="275" ht="38" customHeight="1" spans="1:6">
-      <c r="A275"/>
-      <c r="B275" s="5"/>
-      <c r="C275" s="19"/>
+      <c r="A275" s="5"/>
+      <c r="B275" s="15"/>
+      <c r="C275" s="19" t="s">
+        <v>433</v>
+      </c>
       <c r="D275" s="20"/>
       <c r="E275" s="5"/>
       <c r="F275" s="5"/>
     </row>
-    <row r="276" ht="38" customHeight="1" spans="2:6">
-      <c r="B276" s="5"/>
-      <c r="C276" s="19"/>
+    <row r="276" ht="38" customHeight="1" spans="1:6">
+      <c r="A276" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="B276" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="C276" s="19" t="s">
+        <v>436</v>
+      </c>
       <c r="D276" s="20"/>
       <c r="E276" s="5"/>
       <c r="F276" s="5"/>
     </row>
-    <row r="277" ht="38" customHeight="1" spans="2:6">
-      <c r="B277" s="5"/>
-      <c r="C277" s="19"/>
+    <row r="277" ht="38" customHeight="1" spans="1:6">
+      <c r="A277" s="5"/>
+      <c r="B277" s="17"/>
+      <c r="C277" s="19" t="s">
+        <v>437</v>
+      </c>
       <c r="D277" s="20"/>
       <c r="E277" s="5"/>
       <c r="F277" s="5"/>
     </row>
-    <row r="278" ht="38" customHeight="1" spans="2:6">
-      <c r="B278" s="5"/>
-      <c r="C278" s="19"/>
-      <c r="D278" s="20"/>
+    <row r="278" ht="38" customHeight="1" spans="1:6">
+      <c r="A278" s="5"/>
+      <c r="B278" s="17"/>
+      <c r="C278" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="D278" s="20" t="s">
+        <v>439</v>
+      </c>
       <c r="E278" s="5"/>
       <c r="F278" s="5"/>
     </row>
-    <row r="279" ht="38" customHeight="1" spans="2:6">
-      <c r="B279" s="5"/>
-      <c r="C279" s="19"/>
-      <c r="D279" s="20"/>
+    <row r="279" ht="38" customHeight="1" spans="1:6">
+      <c r="A279" s="5"/>
+      <c r="B279" s="17"/>
+      <c r="C279" s="5"/>
+      <c r="D279" s="20" t="s">
+        <v>440</v>
+      </c>
       <c r="E279" s="5"/>
       <c r="F279" s="5"/>
     </row>
-    <row r="280" ht="38" customHeight="1" spans="2:6">
-      <c r="B280" s="5"/>
-      <c r="C280" s="19"/>
-      <c r="D280" s="20"/>
+    <row r="280" ht="38" customHeight="1" spans="1:6">
+      <c r="A280" s="5"/>
+      <c r="B280" s="17"/>
+      <c r="C280" s="5"/>
+      <c r="D280" s="20" t="s">
+        <v>441</v>
+      </c>
       <c r="E280" s="5"/>
       <c r="F280" s="5"/>
     </row>
-    <row r="281" ht="38" customHeight="1" spans="2:6">
-      <c r="B281" s="5"/>
-      <c r="C281" s="19"/>
-      <c r="D281" s="20"/>
+    <row r="281" ht="38" customHeight="1" spans="1:6">
+      <c r="A281" s="5"/>
+      <c r="B281" s="18"/>
+      <c r="C281" s="5"/>
+      <c r="D281" s="20" t="s">
+        <v>442</v>
+      </c>
       <c r="E281" s="5"/>
       <c r="F281" s="5"/>
     </row>
-    <row r="282" ht="38" customHeight="1" spans="2:6">
-      <c r="B282" s="5"/>
-      <c r="C282" s="19"/>
+    <row r="282" ht="38" customHeight="1" spans="1:6">
+      <c r="A282" s="5"/>
+      <c r="B282" s="16" t="s">
+        <v>443</v>
+      </c>
+      <c r="C282" s="19" t="s">
+        <v>444</v>
+      </c>
       <c r="D282" s="20"/>
       <c r="E282" s="5"/>
       <c r="F282" s="5"/>
     </row>
-    <row r="283" ht="38" customHeight="1" spans="2:6">
-      <c r="B283" s="5"/>
-      <c r="C283" s="19"/>
+    <row r="283" ht="38" customHeight="1" spans="1:6">
+      <c r="A283" s="5"/>
+      <c r="B283" s="17"/>
+      <c r="C283" s="19" t="s">
+        <v>445</v>
+      </c>
       <c r="D283" s="20"/>
       <c r="E283" s="5"/>
       <c r="F283" s="5"/>
     </row>
-    <row r="284" ht="38" customHeight="1" spans="2:6">
-      <c r="B284" s="5"/>
-      <c r="C284" s="19"/>
+    <row r="284" ht="38" customHeight="1" spans="1:6">
+      <c r="A284" s="5"/>
+      <c r="B284" s="17"/>
+      <c r="C284" s="19" t="s">
+        <v>446</v>
+      </c>
       <c r="D284" s="20"/>
       <c r="E284" s="5"/>
       <c r="F284" s="5"/>
     </row>
     <row r="285" ht="38" customHeight="1" spans="1:6">
-      <c r="A285"/>
-      <c r="B285" s="5"/>
-      <c r="C285" s="19"/>
+      <c r="A285" s="5"/>
+      <c r="B285" s="18"/>
+      <c r="C285" s="19" t="s">
+        <v>447</v>
+      </c>
       <c r="D285" s="20"/>
       <c r="E285" s="5"/>
       <c r="F285" s="5"/>
     </row>
-    <row r="286" ht="38" customHeight="1" spans="2:6">
-      <c r="B286" s="5"/>
-      <c r="C286" s="19"/>
+    <row r="286" ht="56" customHeight="1" spans="1:6">
+      <c r="A286" s="5"/>
+      <c r="B286" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="C286" s="27" t="s">
+        <v>448</v>
+      </c>
       <c r="D286" s="20"/>
       <c r="E286" s="5"/>
       <c r="F286" s="5"/>
     </row>
-    <row r="287" ht="38" customHeight="1" spans="2:6">
-      <c r="B287" s="5"/>
-      <c r="C287" s="19"/>
+    <row r="287" ht="38" customHeight="1" spans="1:6">
+      <c r="A287" s="5"/>
+      <c r="B287" s="16" t="s">
+        <v>445</v>
+      </c>
+      <c r="C287" s="19" t="s">
+        <v>449</v>
+      </c>
       <c r="D287" s="20"/>
       <c r="E287" s="5"/>
       <c r="F287" s="5"/>
     </row>
-    <row r="288" ht="38" customHeight="1" spans="2:6">
-      <c r="B288" s="5"/>
-      <c r="C288" s="19"/>
+    <row r="288" ht="38" customHeight="1" spans="1:6">
+      <c r="A288" s="5"/>
+      <c r="B288" s="17"/>
+      <c r="C288" s="21" t="s">
+        <v>450</v>
+      </c>
       <c r="D288" s="20"/>
       <c r="E288" s="5"/>
       <c r="F288" s="5"/>
     </row>
-    <row r="289" ht="38" customHeight="1" spans="2:6">
-      <c r="B289" s="5"/>
-      <c r="C289" s="19"/>
+    <row r="289" ht="38" customHeight="1" spans="1:6">
+      <c r="A289" s="5"/>
+      <c r="B289" s="18"/>
+      <c r="C289" s="21" t="s">
+        <v>451</v>
+      </c>
       <c r="D289" s="20"/>
       <c r="E289" s="5"/>
       <c r="F289" s="5"/>
     </row>
-    <row r="290" ht="38" customHeight="1" spans="2:6">
-      <c r="B290" s="5"/>
-      <c r="C290" s="19"/>
+    <row r="290" ht="38" customHeight="1" spans="1:6">
+      <c r="A290" s="5"/>
+      <c r="B290" s="16" t="s">
+        <v>452</v>
+      </c>
+      <c r="C290" s="19" t="s">
+        <v>453</v>
+      </c>
       <c r="D290" s="20"/>
       <c r="E290" s="5"/>
       <c r="F290" s="5"/>
     </row>
-    <row r="291" ht="38" customHeight="1" spans="2:6">
-      <c r="B291" s="5"/>
-      <c r="C291" s="19"/>
+    <row r="291" ht="38" customHeight="1" spans="1:6">
+      <c r="A291" s="5"/>
+      <c r="B291" s="17"/>
+      <c r="C291" s="21" t="s">
+        <v>454</v>
+      </c>
       <c r="D291" s="20"/>
       <c r="E291" s="5"/>
       <c r="F291" s="5"/>
     </row>
-    <row r="292" ht="38" customHeight="1" spans="2:6">
-      <c r="B292" s="5"/>
-      <c r="C292" s="19"/>
+    <row r="292" ht="38" customHeight="1" spans="1:6">
+      <c r="A292" s="5"/>
+      <c r="B292" s="18"/>
+      <c r="C292" s="21" t="s">
+        <v>455</v>
+      </c>
       <c r="D292" s="20"/>
       <c r="E292" s="5"/>
       <c r="F292" s="5"/>
     </row>
-    <row r="293" ht="38" customHeight="1" spans="2:6">
-      <c r="B293" s="5"/>
-      <c r="C293" s="19"/>
+    <row r="293" ht="38" customHeight="1" spans="1:6">
+      <c r="A293" s="5"/>
+      <c r="B293" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="C293" s="27" t="s">
+        <v>457</v>
+      </c>
       <c r="D293" s="20"/>
       <c r="E293" s="5"/>
       <c r="F293" s="5"/>
     </row>
-    <row r="294" ht="38" customHeight="1" spans="2:6">
-      <c r="B294" s="5"/>
-      <c r="C294" s="19"/>
+    <row r="294" ht="38" customHeight="1" spans="1:6">
+      <c r="A294" s="5"/>
+      <c r="B294" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="C294" s="27" t="s">
+        <v>459</v>
+      </c>
       <c r="D294" s="20"/>
       <c r="E294" s="5"/>
       <c r="F294" s="5"/>
     </row>
     <row r="295" ht="38" customHeight="1" spans="1:6">
-      <c r="A295"/>
-      <c r="B295" s="5"/>
-      <c r="C295" s="19"/>
+      <c r="A295" s="5"/>
+      <c r="B295" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="C295" s="19" t="s">
+        <v>461</v>
+      </c>
       <c r="D295" s="20"/>
       <c r="E295" s="5"/>
       <c r="F295" s="5"/>
     </row>
-    <row r="296" ht="38" customHeight="1" spans="2:6">
-      <c r="B296" s="5"/>
-      <c r="C296" s="19"/>
-      <c r="D296" s="20"/>
+    <row r="296" ht="38" customHeight="1" spans="1:6">
+      <c r="A296" s="5"/>
+      <c r="B296" s="16" t="s">
+        <v>462</v>
+      </c>
+      <c r="C296" s="16" t="s">
+        <v>463</v>
+      </c>
+      <c r="D296" s="5" t="s">
+        <v>464</v>
+      </c>
       <c r="E296" s="5"/>
       <c r="F296" s="5"/>
     </row>
-    <row r="297" ht="38" customHeight="1" spans="2:6">
-      <c r="B297" s="5"/>
-      <c r="C297" s="19"/>
-      <c r="D297" s="20"/>
+    <row r="297" ht="38" customHeight="1" spans="1:6">
+      <c r="A297" s="5"/>
+      <c r="B297" s="17"/>
+      <c r="C297" s="17"/>
+      <c r="D297" s="5" t="s">
+        <v>465</v>
+      </c>
       <c r="E297" s="5"/>
       <c r="F297" s="5"/>
     </row>
-    <row r="298" ht="38" customHeight="1" spans="2:6">
-      <c r="B298" s="5"/>
-      <c r="C298" s="19"/>
-      <c r="D298" s="20"/>
+    <row r="298" ht="38" customHeight="1" spans="1:6">
+      <c r="A298" s="5"/>
+      <c r="B298" s="17"/>
+      <c r="C298" s="17"/>
+      <c r="D298" s="5" t="s">
+        <v>466</v>
+      </c>
       <c r="E298" s="5"/>
       <c r="F298" s="5"/>
     </row>
-    <row r="299" ht="38" customHeight="1" spans="2:6">
-      <c r="B299" s="5"/>
-      <c r="C299" s="19"/>
-      <c r="D299" s="20"/>
+    <row r="299" ht="38" customHeight="1" spans="1:6">
+      <c r="A299" s="5"/>
+      <c r="B299" s="18"/>
+      <c r="C299" s="18"/>
+      <c r="D299" s="5" t="s">
+        <v>467</v>
+      </c>
       <c r="E299" s="5"/>
       <c r="F299" s="5"/>
     </row>
-    <row r="300" ht="38" customHeight="1" spans="2:6">
-      <c r="B300" s="5"/>
-      <c r="C300" s="19"/>
+    <row r="300" ht="38" customHeight="1" spans="1:6">
+      <c r="A300" s="5"/>
+      <c r="B300" s="16" t="s">
+        <v>468</v>
+      </c>
+      <c r="C300" s="19" t="s">
+        <v>469</v>
+      </c>
       <c r="D300" s="20"/>
       <c r="E300" s="5"/>
       <c r="F300" s="5"/>
     </row>
-    <row r="301" ht="38" customHeight="1" spans="2:6">
-      <c r="B301" s="5"/>
-      <c r="C301" s="19"/>
+    <row r="301" ht="38" customHeight="1" spans="1:6">
+      <c r="A301" s="5"/>
+      <c r="B301" s="18"/>
+      <c r="C301" s="21" t="s">
+        <v>470</v>
+      </c>
       <c r="D301" s="20"/>
       <c r="E301" s="5"/>
       <c r="F301" s="5"/>
     </row>
-    <row r="302" ht="38" customHeight="1" spans="2:6">
-      <c r="B302" s="5"/>
-      <c r="C302" s="19"/>
+    <row r="302" ht="38" customHeight="1" spans="1:6">
+      <c r="A302" s="5"/>
+      <c r="B302" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="C302" s="19" t="s">
+        <v>472</v>
+      </c>
       <c r="D302" s="20"/>
       <c r="E302" s="5"/>
       <c r="F302" s="5"/>
     </row>
-    <row r="303" ht="38" customHeight="1" spans="2:6">
-      <c r="B303" s="5"/>
-      <c r="C303" s="19"/>
+    <row r="303" ht="38" customHeight="1" spans="1:6">
+      <c r="A303" s="5"/>
+      <c r="B303" s="17"/>
+      <c r="C303" s="19" t="s">
+        <v>473</v>
+      </c>
       <c r="D303" s="20"/>
       <c r="E303" s="5"/>
       <c r="F303" s="5"/>
     </row>
-    <row r="304" ht="38" customHeight="1" spans="2:6">
-      <c r="B304" s="5"/>
-      <c r="C304" s="19"/>
-      <c r="D304" s="20"/>
+    <row r="304" ht="38" customHeight="1" spans="1:6">
+      <c r="A304" s="5"/>
+      <c r="B304" s="17"/>
+      <c r="C304" s="16" t="s">
+        <v>474</v>
+      </c>
+      <c r="D304" s="5" t="s">
+        <v>475</v>
+      </c>
       <c r="E304" s="5"/>
       <c r="F304" s="5"/>
     </row>
     <row r="305" ht="38" customHeight="1" spans="1:6">
-      <c r="A305"/>
-      <c r="B305" s="5"/>
-      <c r="C305" s="19"/>
-      <c r="D305" s="20"/>
+      <c r="A305" s="5"/>
+      <c r="B305" s="17"/>
+      <c r="C305" s="17"/>
+      <c r="D305" s="5" t="s">
+        <v>476</v>
+      </c>
       <c r="E305" s="5"/>
       <c r="F305" s="5"/>
     </row>
-    <row r="306" ht="38" customHeight="1" spans="2:6">
-      <c r="B306" s="5"/>
-      <c r="C306" s="19"/>
-      <c r="D306" s="20"/>
+    <row r="306" ht="38" customHeight="1" spans="1:6">
+      <c r="A306" s="5"/>
+      <c r="B306" s="17"/>
+      <c r="C306" s="17"/>
+      <c r="D306" s="5" t="s">
+        <v>477</v>
+      </c>
       <c r="E306" s="5"/>
       <c r="F306" s="5"/>
     </row>
-    <row r="307" ht="38" customHeight="1" spans="2:6">
-      <c r="B307" s="5"/>
-      <c r="C307" s="19"/>
-      <c r="D307" s="20"/>
+    <row r="307" ht="38" customHeight="1" spans="1:6">
+      <c r="A307" s="5"/>
+      <c r="B307" s="17"/>
+      <c r="C307" s="17"/>
+      <c r="D307" s="5" t="s">
+        <v>478</v>
+      </c>
       <c r="E307" s="5"/>
       <c r="F307" s="5"/>
     </row>
-    <row r="308" ht="38" customHeight="1" spans="2:6">
-      <c r="B308" s="5"/>
-      <c r="C308" s="19"/>
-      <c r="D308" s="20"/>
+    <row r="308" ht="38" customHeight="1" spans="1:6">
+      <c r="A308" s="5"/>
+      <c r="B308" s="18"/>
+      <c r="C308" s="18"/>
+      <c r="D308" s="5" t="s">
+        <v>479</v>
+      </c>
       <c r="E308" s="5"/>
       <c r="F308" s="5"/>
     </row>
-    <row r="309" ht="38" customHeight="1" spans="2:6">
-      <c r="B309" s="5"/>
-      <c r="C309" s="19"/>
+    <row r="309" ht="38" customHeight="1" spans="1:6">
+      <c r="A309" s="5"/>
+      <c r="B309" s="16" t="s">
+        <v>480</v>
+      </c>
+      <c r="C309" s="27" t="s">
+        <v>481</v>
+      </c>
       <c r="D309" s="20"/>
       <c r="E309" s="5"/>
       <c r="F309" s="5"/>
     </row>
-    <row r="310" ht="38" customHeight="1" spans="2:6">
-      <c r="B310" s="5"/>
-      <c r="C310" s="19"/>
+    <row r="310" ht="38" customHeight="1" spans="1:6">
+      <c r="A310" s="5"/>
+      <c r="B310" s="17"/>
+      <c r="C310" s="19" t="s">
+        <v>482</v>
+      </c>
       <c r="D310" s="20"/>
       <c r="E310" s="5"/>
       <c r="F310" s="5"/>
     </row>
-    <row r="311" ht="38" customHeight="1" spans="2:6">
-      <c r="B311" s="5"/>
-      <c r="C311" s="19"/>
-      <c r="D311" s="20"/>
+    <row r="311" ht="38" customHeight="1" spans="1:6">
+      <c r="A311" s="5"/>
+      <c r="B311" s="17"/>
+      <c r="C311" s="16" t="s">
+        <v>483</v>
+      </c>
+      <c r="D311" s="5" t="s">
+        <v>484</v>
+      </c>
       <c r="E311" s="5"/>
       <c r="F311" s="5"/>
     </row>
-    <row r="312" ht="38" customHeight="1" spans="2:6">
-      <c r="B312" s="5"/>
-      <c r="C312" s="19"/>
-      <c r="D312" s="20"/>
+    <row r="312" ht="38" customHeight="1" spans="1:6">
+      <c r="A312" s="5"/>
+      <c r="B312" s="17"/>
+      <c r="C312" s="17"/>
+      <c r="D312" s="5" t="s">
+        <v>485</v>
+      </c>
       <c r="E312" s="5"/>
       <c r="F312" s="5"/>
     </row>
-    <row r="313" ht="38" customHeight="1" spans="2:6">
-      <c r="B313" s="5"/>
-      <c r="C313" s="19"/>
-      <c r="D313" s="20"/>
+    <row r="313" ht="38" customHeight="1" spans="1:6">
+      <c r="A313" s="5"/>
+      <c r="B313" s="17"/>
+      <c r="C313" s="17"/>
+      <c r="D313" s="5" t="s">
+        <v>486</v>
+      </c>
       <c r="E313" s="5"/>
       <c r="F313" s="5"/>
     </row>
-    <row r="314" ht="38" customHeight="1" spans="2:6">
-      <c r="B314" s="5"/>
-      <c r="C314" s="19"/>
-      <c r="D314" s="20"/>
+    <row r="314" ht="38" customHeight="1" spans="1:6">
+      <c r="A314" s="5"/>
+      <c r="B314" s="17"/>
+      <c r="C314" s="17"/>
+      <c r="D314" s="5" t="s">
+        <v>487</v>
+      </c>
       <c r="E314" s="5"/>
       <c r="F314" s="5"/>
     </row>
     <row r="315" ht="38" customHeight="1" spans="1:6">
-      <c r="A315"/>
-      <c r="B315" s="5"/>
-      <c r="C315" s="19"/>
-      <c r="D315" s="20"/>
+      <c r="A315" s="5"/>
+      <c r="B315" s="17"/>
+      <c r="C315" s="17"/>
+      <c r="D315" s="5" t="s">
+        <v>488</v>
+      </c>
       <c r="E315" s="5"/>
       <c r="F315" s="5"/>
     </row>
-    <row r="316" ht="38" customHeight="1" spans="2:6">
-      <c r="B316" s="5"/>
-      <c r="C316" s="19"/>
-      <c r="D316" s="20"/>
+    <row r="316" ht="38" customHeight="1" spans="1:6">
+      <c r="A316" s="5"/>
+      <c r="B316" s="18"/>
+      <c r="C316" s="18"/>
+      <c r="D316" s="5" t="s">
+        <v>489</v>
+      </c>
       <c r="E316" s="5"/>
       <c r="F316" s="5"/>
     </row>
-    <row r="317" ht="38" customHeight="1" spans="2:6">
-      <c r="B317" s="5"/>
-      <c r="C317" s="19"/>
+    <row r="317" ht="38" customHeight="1" spans="1:6">
+      <c r="A317" s="5"/>
+      <c r="B317" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="C317" s="21" t="s">
+        <v>491</v>
+      </c>
       <c r="D317" s="20"/>
       <c r="E317" s="5"/>
       <c r="F317" s="5"/>
     </row>
-    <row r="318" ht="38" customHeight="1" spans="2:6">
-      <c r="B318" s="5"/>
-      <c r="C318" s="19"/>
+    <row r="318" ht="38" customHeight="1" spans="1:6">
+      <c r="A318" s="5"/>
+      <c r="B318" s="17"/>
+      <c r="C318" s="19" t="s">
+        <v>492</v>
+      </c>
       <c r="D318" s="20"/>
       <c r="E318" s="5"/>
       <c r="F318" s="5"/>
     </row>
-    <row r="319" ht="38" customHeight="1" spans="2:6">
-      <c r="B319" s="5"/>
-      <c r="C319" s="19"/>
+    <row r="319" ht="38" customHeight="1" spans="1:6">
+      <c r="A319" s="5"/>
+      <c r="B319" s="17"/>
+      <c r="C319" s="19" t="s">
+        <v>493</v>
+      </c>
       <c r="D319" s="20"/>
       <c r="E319" s="5"/>
       <c r="F319" s="5"/>
     </row>
-    <row r="320" ht="38" customHeight="1" spans="2:6">
-      <c r="B320" s="5"/>
-      <c r="C320" s="19"/>
+    <row r="320" ht="38" customHeight="1" spans="1:6">
+      <c r="A320" s="5"/>
+      <c r="B320" s="17"/>
+      <c r="C320" s="19" t="s">
+        <v>494</v>
+      </c>
       <c r="D320" s="20"/>
       <c r="E320" s="5"/>
       <c r="F320" s="5"/>
     </row>
-    <row r="321" ht="38" customHeight="1" spans="2:6">
-      <c r="B321" s="5"/>
-      <c r="C321" s="19"/>
+    <row r="321" ht="38" customHeight="1" spans="1:6">
+      <c r="A321" s="5"/>
+      <c r="B321" s="18"/>
+      <c r="C321" s="19" t="s">
+        <v>495</v>
+      </c>
       <c r="D321" s="20"/>
       <c r="E321" s="5"/>
       <c r="F321" s="5"/>
     </row>
-    <row r="322" ht="38" customHeight="1" spans="2:6">
-      <c r="B322" s="5"/>
-      <c r="C322" s="19"/>
-      <c r="D322" s="20"/>
+    <row r="322" ht="38" customHeight="1" spans="1:6">
+      <c r="A322" s="5"/>
+      <c r="B322" s="16" t="s">
+        <v>496</v>
+      </c>
+      <c r="C322" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="D322" s="5" t="s">
+        <v>498</v>
+      </c>
       <c r="E322" s="5"/>
       <c r="F322" s="5"/>
     </row>
-    <row r="323" ht="38" customHeight="1" spans="2:6">
-      <c r="B323" s="5"/>
-      <c r="C323" s="19"/>
-      <c r="D323" s="20"/>
+    <row r="323" ht="38" customHeight="1" spans="1:6">
+      <c r="A323" s="5"/>
+      <c r="B323" s="17"/>
+      <c r="C323" s="17"/>
+      <c r="D323" s="5" t="s">
+        <v>499</v>
+      </c>
       <c r="E323" s="5"/>
       <c r="F323" s="5"/>
     </row>
-    <row r="324" ht="38" customHeight="1" spans="2:6">
-      <c r="B324" s="5"/>
-      <c r="C324" s="19"/>
-      <c r="D324" s="20"/>
+    <row r="324" ht="38" customHeight="1" spans="1:6">
+      <c r="A324" s="5"/>
+      <c r="B324" s="17"/>
+      <c r="C324" s="18"/>
+      <c r="D324" s="5" t="s">
+        <v>500</v>
+      </c>
       <c r="E324" s="5"/>
       <c r="F324" s="5"/>
     </row>
     <row r="325" ht="38" customHeight="1" spans="1:6">
-      <c r="A325"/>
-      <c r="B325" s="5"/>
-      <c r="C325" s="19"/>
+      <c r="A325" s="5"/>
+      <c r="B325" s="17"/>
+      <c r="C325" s="21" t="s">
+        <v>501</v>
+      </c>
       <c r="D325" s="20"/>
       <c r="E325" s="5"/>
       <c r="F325" s="5"/>
     </row>
-    <row r="326" ht="38" customHeight="1" spans="2:6">
-      <c r="B326" s="5"/>
-      <c r="C326" s="19"/>
+    <row r="326" ht="38" customHeight="1" spans="1:6">
+      <c r="A326" s="5"/>
+      <c r="B326" s="18"/>
+      <c r="C326" s="19" t="s">
+        <v>502</v>
+      </c>
       <c r="D326" s="20"/>
       <c r="E326" s="5"/>
       <c r="F326" s="5"/>
     </row>
-    <row r="327" ht="38" customHeight="1" spans="2:6">
-      <c r="B327" s="5"/>
-      <c r="C327" s="19"/>
-      <c r="D327" s="20"/>
+    <row r="327" ht="38" customHeight="1" spans="1:6">
+      <c r="A327" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B327" s="16" t="s">
+        <v>504</v>
+      </c>
+      <c r="C327" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="D327" s="5" t="s">
+        <v>506</v>
+      </c>
       <c r="E327" s="5"/>
       <c r="F327" s="5"/>
     </row>
     <row r="328" ht="38" customHeight="1" spans="2:6">
-      <c r="B328" s="5"/>
-      <c r="C328" s="19"/>
-      <c r="D328" s="20"/>
+      <c r="B328" s="18"/>
+      <c r="C328" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="D328" s="5" t="s">
+        <v>508</v>
+      </c>
       <c r="E328" s="5"/>
       <c r="F328" s="5"/>
     </row>
     <row r="329" ht="38" customHeight="1" spans="2:6">
-      <c r="B329" s="5"/>
-      <c r="C329" s="19"/>
+      <c r="B329" s="16" t="s">
+        <v>509</v>
+      </c>
+      <c r="C329" s="21" t="s">
+        <v>510</v>
+      </c>
       <c r="D329" s="20"/>
       <c r="E329" s="5"/>
       <c r="F329" s="5"/>
     </row>
     <row r="330" ht="38" customHeight="1" spans="2:6">
-      <c r="B330" s="5"/>
-      <c r="C330" s="19"/>
+      <c r="B330" s="18"/>
+      <c r="C330" s="19" t="s">
+        <v>511</v>
+      </c>
       <c r="D330" s="20"/>
       <c r="E330" s="5"/>
       <c r="F330" s="5"/>
     </row>
     <row r="331" ht="38" customHeight="1" spans="2:6">
-      <c r="B331" s="5"/>
-      <c r="C331" s="19"/>
+      <c r="B331" s="16" t="s">
+        <v>512</v>
+      </c>
+      <c r="C331" s="19" t="s">
+        <v>513</v>
+      </c>
       <c r="D331" s="20"/>
       <c r="E331" s="5"/>
       <c r="F331" s="5"/>
     </row>
     <row r="332" ht="38" customHeight="1" spans="2:6">
-      <c r="B332" s="5"/>
-      <c r="C332" s="19"/>
+      <c r="B332" s="18"/>
+      <c r="C332" s="19" t="s">
+        <v>514</v>
+      </c>
       <c r="D332" s="20"/>
       <c r="E332" s="5"/>
       <c r="F332" s="5"/>
     </row>
     <row r="333" ht="38" customHeight="1" spans="2:6">
-      <c r="B333" s="5"/>
-      <c r="C333" s="19"/>
+      <c r="B333" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="C333" s="21" t="s">
+        <v>516</v>
+      </c>
       <c r="D333" s="20"/>
       <c r="E333" s="5"/>
       <c r="F333" s="5"/>
     </row>
     <row r="334" ht="38" customHeight="1" spans="2:6">
-      <c r="B334" s="5"/>
-      <c r="C334" s="19"/>
+      <c r="B334" s="18"/>
+      <c r="C334" s="19" t="s">
+        <v>517</v>
+      </c>
       <c r="D334" s="20"/>
       <c r="E334" s="5"/>
       <c r="F334" s="5"/>
     </row>
-    <row r="335" ht="38" customHeight="1" spans="1:6">
-      <c r="A335"/>
-      <c r="B335" s="5"/>
-      <c r="C335" s="19"/>
+    <row r="335" ht="38" customHeight="1" spans="2:6">
+      <c r="B335" s="16" t="s">
+        <v>518</v>
+      </c>
+      <c r="C335" s="21" t="s">
+        <v>519</v>
+      </c>
       <c r="D335" s="20"/>
       <c r="E335" s="5"/>
       <c r="F335" s="5"/>
     </row>
-    <row r="336" ht="38" customHeight="1" spans="2:6">
-      <c r="B336" s="5"/>
-      <c r="C336" s="19"/>
+    <row r="336" ht="38" customHeight="1" spans="1:6">
+      <c r="A336" s="2"/>
+      <c r="B336" s="18"/>
+      <c r="C336" s="19" t="s">
+        <v>520</v>
+      </c>
       <c r="D336" s="20"/>
       <c r="E336" s="5"/>
       <c r="F336" s="5"/>
     </row>
     <row r="337" ht="38" customHeight="1" spans="2:6">
-      <c r="B337" s="5"/>
-      <c r="C337" s="19"/>
-      <c r="D337" s="20"/>
+      <c r="B337" s="16" t="s">
+        <v>521</v>
+      </c>
+      <c r="C337" s="30" t="s">
+        <v>522</v>
+      </c>
+      <c r="D337" s="31"/>
       <c r="E337" s="5"/>
       <c r="F337" s="5"/>
     </row>
     <row r="338" ht="38" customHeight="1" spans="2:6">
-      <c r="B338" s="5"/>
-      <c r="C338" s="19"/>
+      <c r="B338" s="17"/>
+      <c r="C338" s="30" t="s">
+        <v>523</v>
+      </c>
       <c r="D338" s="20"/>
       <c r="E338" s="5"/>
       <c r="F338" s="5"/>
     </row>
     <row r="339" ht="38" customHeight="1" spans="2:6">
-      <c r="B339" s="5"/>
-      <c r="C339" s="19"/>
+      <c r="B339" s="18"/>
+      <c r="C339" s="19" t="s">
+        <v>524</v>
+      </c>
       <c r="D339" s="20"/>
       <c r="E339" s="5"/>
       <c r="F339" s="5"/>
     </row>
     <row r="340" ht="38" customHeight="1" spans="2:6">
-      <c r="B340" s="5"/>
-      <c r="C340" s="19"/>
+      <c r="B340" s="16" t="s">
+        <v>525</v>
+      </c>
+      <c r="C340" s="30" t="s">
+        <v>526</v>
+      </c>
       <c r="D340" s="20"/>
       <c r="E340" s="5"/>
       <c r="F340" s="5"/>
     </row>
     <row r="341" ht="38" customHeight="1" spans="2:6">
-      <c r="B341" s="5"/>
-      <c r="C341" s="19"/>
+      <c r="B341" s="17"/>
+      <c r="C341" s="19" t="s">
+        <v>527</v>
+      </c>
       <c r="D341" s="20"/>
       <c r="E341" s="5"/>
       <c r="F341" s="5"/>
     </row>
     <row r="342" ht="38" customHeight="1" spans="2:6">
-      <c r="B342" s="5"/>
-      <c r="C342" s="19"/>
+      <c r="B342" s="18"/>
+      <c r="C342" s="30" t="s">
+        <v>528</v>
+      </c>
       <c r="D342" s="20"/>
       <c r="E342" s="5"/>
       <c r="F342" s="5"/>
     </row>
     <row r="343" ht="38" customHeight="1" spans="2:6">
-      <c r="B343" s="5"/>
-      <c r="C343" s="19"/>
+      <c r="B343" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="C343" s="19" t="s">
+        <v>530</v>
+      </c>
       <c r="D343" s="20"/>
       <c r="E343" s="5"/>
       <c r="F343" s="5"/>
     </row>
     <row r="344" ht="38" customHeight="1" spans="2:6">
-      <c r="B344" s="5"/>
-      <c r="C344" s="19"/>
+      <c r="B344" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="C344" s="30" t="s">
+        <v>532</v>
+      </c>
       <c r="D344" s="20"/>
       <c r="E344" s="5"/>
       <c r="F344" s="5"/>
     </row>
-    <row r="345" ht="38" customHeight="1" spans="1:6">
-      <c r="A345"/>
-      <c r="B345" s="5"/>
-      <c r="C345" s="19"/>
+    <row r="345" ht="38" customHeight="1" spans="2:6">
+      <c r="B345" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="C345" s="30" t="s">
+        <v>534</v>
+      </c>
       <c r="D345" s="20"/>
       <c r="E345" s="5"/>
       <c r="F345" s="5"/>
     </row>
-    <row r="346" ht="38" customHeight="1" spans="2:6">
-      <c r="B346" s="5"/>
-      <c r="C346" s="19"/>
+    <row r="346" ht="38" customHeight="1" spans="1:6">
+      <c r="A346" s="2"/>
+      <c r="B346" s="16" t="s">
+        <v>535</v>
+      </c>
+      <c r="C346" s="30" t="s">
+        <v>536</v>
+      </c>
       <c r="D346" s="20"/>
       <c r="E346" s="5"/>
       <c r="F346" s="5"/>
     </row>
     <row r="347" ht="38" customHeight="1" spans="2:6">
-      <c r="B347" s="5"/>
-      <c r="C347" s="19"/>
+      <c r="B347" s="18"/>
+      <c r="C347" s="19" t="s">
+        <v>537</v>
+      </c>
       <c r="D347" s="20"/>
       <c r="E347" s="5"/>
       <c r="F347" s="5"/>
     </row>
     <row r="348" ht="38" customHeight="1" spans="2:6">
-      <c r="B348" s="5"/>
-      <c r="C348" s="19"/>
+      <c r="B348" s="16" t="s">
+        <v>538</v>
+      </c>
+      <c r="C348" s="30" t="s">
+        <v>539</v>
+      </c>
       <c r="D348" s="20"/>
       <c r="E348" s="5"/>
       <c r="F348" s="5"/>
     </row>
     <row r="349" ht="38" customHeight="1" spans="2:6">
-      <c r="B349" s="5"/>
-      <c r="C349" s="19"/>
-      <c r="D349" s="20"/>
+      <c r="B349" s="17"/>
+      <c r="C349" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="D349" s="5" t="s">
+        <v>541</v>
+      </c>
       <c r="E349" s="5"/>
       <c r="F349" s="5"/>
     </row>
     <row r="350" ht="38" customHeight="1" spans="2:6">
-      <c r="B350" s="5"/>
-      <c r="C350" s="19"/>
-      <c r="D350" s="20"/>
+      <c r="B350" s="18"/>
+      <c r="C350" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="D350" s="5" t="s">
+        <v>543</v>
+      </c>
       <c r="E350" s="5"/>
       <c r="F350" s="5"/>
     </row>
     <row r="351" ht="38" customHeight="1" spans="2:6">
-      <c r="B351" s="5"/>
-      <c r="C351" s="19"/>
+      <c r="B351" s="16" t="s">
+        <v>540</v>
+      </c>
+      <c r="C351" s="19" t="s">
+        <v>544</v>
+      </c>
       <c r="D351" s="20"/>
       <c r="E351" s="5"/>
       <c r="F351" s="5"/>
     </row>
     <row r="352" ht="38" customHeight="1" spans="2:6">
-      <c r="B352" s="5"/>
-      <c r="C352" s="19"/>
-      <c r="D352" s="20"/>
+      <c r="B352" s="17"/>
+      <c r="C352" s="21" t="s">
+        <v>545</v>
+      </c>
+      <c r="D352" s="33"/>
       <c r="E352" s="5"/>
       <c r="F352" s="5"/>
     </row>
     <row r="353" ht="38" customHeight="1" spans="2:6">
-      <c r="B353" s="5"/>
-      <c r="C353" s="19"/>
+      <c r="B353" s="18"/>
+      <c r="C353" s="19" t="s">
+        <v>546</v>
+      </c>
       <c r="D353" s="20"/>
       <c r="E353" s="5"/>
       <c r="F353" s="5"/>
     </row>
     <row r="354" ht="38" customHeight="1" spans="2:6">
-      <c r="B354" s="5"/>
-      <c r="C354" s="19"/>
+      <c r="B354" s="16" t="s">
+        <v>547</v>
+      </c>
+      <c r="C354" s="21" t="s">
+        <v>548</v>
+      </c>
       <c r="D354" s="20"/>
       <c r="E354" s="5"/>
       <c r="F354" s="5"/>
     </row>
-    <row r="355" ht="38" customHeight="1" spans="1:6">
-      <c r="A355"/>
-      <c r="B355" s="5"/>
-      <c r="C355" s="19"/>
+    <row r="355" ht="38" customHeight="1" spans="2:6">
+      <c r="B355" s="17"/>
+      <c r="C355" s="21" t="s">
+        <v>549</v>
+      </c>
       <c r="D355" s="20"/>
       <c r="E355" s="5"/>
       <c r="F355" s="5"/>
     </row>
-    <row r="356" ht="38" customHeight="1" spans="2:6">
-      <c r="B356" s="5"/>
-      <c r="C356" s="19"/>
+    <row r="356" ht="38" customHeight="1" spans="1:6">
+      <c r="A356" s="2"/>
+      <c r="B356" s="17"/>
+      <c r="C356" s="21" t="s">
+        <v>550</v>
+      </c>
       <c r="D356" s="20"/>
       <c r="E356" s="5"/>
       <c r="F356" s="5"/>
     </row>
     <row r="357" ht="38" customHeight="1" spans="2:6">
-      <c r="B357" s="5"/>
-      <c r="C357" s="19"/>
+      <c r="B357" s="18"/>
+      <c r="C357" s="21" t="s">
+        <v>551</v>
+      </c>
       <c r="D357" s="20"/>
       <c r="E357" s="5"/>
       <c r="F357" s="5"/>
     </row>
     <row r="358" ht="38" customHeight="1" spans="2:6">
-      <c r="B358" s="5"/>
-      <c r="C358" s="19"/>
+      <c r="B358" s="16" t="s">
+        <v>552</v>
+      </c>
+      <c r="C358" s="19" t="s">
+        <v>553</v>
+      </c>
       <c r="D358" s="20"/>
       <c r="E358" s="5"/>
       <c r="F358" s="5"/>
     </row>
     <row r="359" ht="38" customHeight="1" spans="2:6">
-      <c r="B359" s="5"/>
-      <c r="C359" s="19"/>
+      <c r="B359" s="17"/>
+      <c r="C359" s="19" t="s">
+        <v>554</v>
+      </c>
       <c r="D359" s="20"/>
       <c r="E359" s="5"/>
       <c r="F359" s="5"/>
     </row>
     <row r="360" ht="38" customHeight="1" spans="2:6">
-      <c r="B360" s="5"/>
-      <c r="C360" s="19"/>
+      <c r="B360" s="17"/>
+      <c r="C360" s="19" t="s">
+        <v>555</v>
+      </c>
       <c r="D360" s="20"/>
       <c r="E360" s="5"/>
       <c r="F360" s="5"/>
     </row>
     <row r="361" ht="38" customHeight="1" spans="2:6">
-      <c r="B361" s="5"/>
-      <c r="C361" s="19"/>
+      <c r="B361" s="18"/>
+      <c r="C361" s="27" t="s">
+        <v>556</v>
+      </c>
       <c r="D361" s="20"/>
       <c r="E361" s="5"/>
       <c r="F361" s="5"/>
     </row>
     <row r="362" ht="38" customHeight="1" spans="2:6">
-      <c r="B362" s="5"/>
-      <c r="C362" s="19"/>
-      <c r="D362" s="20"/>
+      <c r="B362" s="16" t="s">
+        <v>557</v>
+      </c>
+      <c r="C362" s="16" t="s">
+        <v>558</v>
+      </c>
+      <c r="D362" s="5" t="s">
+        <v>559</v>
+      </c>
       <c r="E362" s="5"/>
       <c r="F362" s="5"/>
     </row>
     <row r="363" ht="38" customHeight="1" spans="2:6">
-      <c r="B363" s="5"/>
-      <c r="C363" s="19"/>
-      <c r="D363" s="20"/>
+      <c r="B363" s="17"/>
+      <c r="C363" s="17"/>
+      <c r="D363" s="5" t="s">
+        <v>560</v>
+      </c>
       <c r="E363" s="5"/>
       <c r="F363" s="5"/>
     </row>
     <row r="364" ht="38" customHeight="1" spans="2:6">
-      <c r="B364" s="5"/>
-      <c r="C364" s="19"/>
-      <c r="D364" s="20"/>
+      <c r="B364" s="17"/>
+      <c r="C364" s="17"/>
+      <c r="D364" s="5" t="s">
+        <v>561</v>
+      </c>
       <c r="E364" s="5"/>
       <c r="F364" s="5"/>
     </row>
-    <row r="365" ht="38" customHeight="1" spans="1:6">
-      <c r="A365"/>
-      <c r="B365" s="5"/>
-      <c r="C365" s="19"/>
-      <c r="D365" s="20"/>
+    <row r="365" ht="38" customHeight="1" spans="2:6">
+      <c r="B365" s="17"/>
+      <c r="C365" s="18"/>
+      <c r="D365" s="5" t="s">
+        <v>562</v>
+      </c>
       <c r="E365" s="5"/>
       <c r="F365" s="5"/>
     </row>
-    <row r="366" ht="38" customHeight="1" spans="2:6">
-      <c r="B366" s="5"/>
-      <c r="C366" s="19"/>
+    <row r="366" ht="38" customHeight="1" spans="1:6">
+      <c r="A366" s="2"/>
+      <c r="B366" s="18"/>
+      <c r="C366" s="21" t="s">
+        <v>563</v>
+      </c>
       <c r="D366" s="20"/>
       <c r="E366" s="5"/>
       <c r="F366" s="5"/>
     </row>
     <row r="367" ht="38" customHeight="1" spans="2:6">
-      <c r="B367" s="5"/>
-      <c r="C367" s="19"/>
+      <c r="B367" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="C367" s="21" t="s">
+        <v>565</v>
+      </c>
       <c r="D367" s="20"/>
       <c r="E367" s="5"/>
       <c r="F367" s="5"/>
     </row>
     <row r="368" ht="38" customHeight="1" spans="2:6">
-      <c r="B368" s="5"/>
-      <c r="C368" s="19"/>
+      <c r="B368" s="5" t="s">
+        <v>566</v>
+      </c>
+      <c r="C368" s="19" t="s">
+        <v>567</v>
+      </c>
       <c r="D368" s="20"/>
       <c r="E368" s="5"/>
       <c r="F368" s="5"/>
     </row>
     <row r="369" ht="38" customHeight="1" spans="2:6">
-      <c r="B369" s="5"/>
-      <c r="C369" s="19"/>
+      <c r="B369" s="16" t="s">
+        <v>568</v>
+      </c>
+      <c r="C369" s="19" t="s">
+        <v>569</v>
+      </c>
       <c r="D369" s="20"/>
       <c r="E369" s="5"/>
       <c r="F369" s="5"/>
     </row>
     <row r="370" ht="38" customHeight="1" spans="2:6">
-      <c r="B370" s="5"/>
-      <c r="C370" s="19"/>
+      <c r="B370" s="18"/>
+      <c r="C370" s="19" t="s">
+        <v>570</v>
+      </c>
       <c r="D370" s="20"/>
       <c r="E370" s="5"/>
       <c r="F370" s="5"/>
     </row>
     <row r="371" ht="38" customHeight="1" spans="2:6">
-      <c r="B371" s="5"/>
-      <c r="C371" s="19"/>
+      <c r="B371" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="C371" s="19" t="s">
+        <v>572</v>
+      </c>
       <c r="D371" s="20"/>
-      <c r="E371" s="5"/>
+      <c r="E371" s="5" t="s">
+        <v>573</v>
+      </c>
       <c r="F371" s="5"/>
     </row>
     <row r="372" ht="38" customHeight="1" spans="2:6">
-      <c r="B372" s="5"/>
-      <c r="C372" s="19"/>
+      <c r="B372" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="C372" s="19" t="s">
+        <v>575</v>
+      </c>
       <c r="D372" s="20"/>
       <c r="E372" s="5"/>
       <c r="F372" s="5"/>
     </row>
     <row r="373" ht="38" customHeight="1" spans="2:6">
-      <c r="B373" s="5"/>
-      <c r="C373" s="19"/>
+      <c r="B373" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="C373" s="19" t="s">
+        <v>577</v>
+      </c>
       <c r="D373" s="20"/>
       <c r="E373" s="5"/>
       <c r="F373" s="5"/>
     </row>
     <row r="374" ht="38" customHeight="1" spans="2:6">
-      <c r="B374" s="5"/>
-      <c r="C374" s="19"/>
+      <c r="B374" s="16" t="s">
+        <v>578</v>
+      </c>
+      <c r="C374" s="19" t="s">
+        <v>579</v>
+      </c>
       <c r="D374" s="20"/>
       <c r="E374" s="5"/>
       <c r="F374" s="5"/>
     </row>
-    <row r="375" ht="38" customHeight="1" spans="1:6">
-      <c r="A375"/>
-      <c r="B375" s="5"/>
-      <c r="C375" s="19"/>
+    <row r="375" ht="38" customHeight="1" spans="2:6">
+      <c r="B375" s="17"/>
+      <c r="C375" s="19" t="s">
+        <v>580</v>
+      </c>
       <c r="D375" s="20"/>
       <c r="E375" s="5"/>
       <c r="F375" s="5"/>
     </row>
-    <row r="376" ht="38" customHeight="1" spans="2:6">
-      <c r="B376" s="5"/>
-      <c r="C376" s="19"/>
+    <row r="376" ht="38" customHeight="1" spans="1:6">
+      <c r="A376" s="2"/>
+      <c r="B376" s="18"/>
+      <c r="C376" s="19" t="s">
+        <v>581</v>
+      </c>
       <c r="D376" s="20"/>
       <c r="E376" s="5"/>
       <c r="F376" s="5"/>
     </row>
     <row r="377" ht="38" customHeight="1" spans="2:6">
-      <c r="B377" s="5"/>
-      <c r="C377" s="19"/>
+      <c r="B377" s="16" t="s">
+        <v>582</v>
+      </c>
+      <c r="C377" s="19" t="s">
+        <v>583</v>
+      </c>
       <c r="D377" s="20"/>
-      <c r="E377" s="5"/>
+      <c r="E377" s="5" t="s">
+        <v>584</v>
+      </c>
       <c r="F377" s="5"/>
     </row>
     <row r="378" ht="38" customHeight="1" spans="2:6">
-      <c r="B378" s="5"/>
-      <c r="C378" s="19"/>
+      <c r="B378" s="17"/>
+      <c r="C378" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="D378" s="20"/>
       <c r="E378" s="5"/>
       <c r="F378" s="5"/>
     </row>
     <row r="379" ht="38" customHeight="1" spans="2:6">
-      <c r="B379" s="5"/>
-      <c r="C379" s="19"/>
+      <c r="B379" s="18"/>
+      <c r="C379" s="19" t="s">
+        <v>586</v>
+      </c>
       <c r="D379" s="20"/>
       <c r="E379" s="5"/>
       <c r="F379" s="5"/>
     </row>
     <row r="380" ht="38" customHeight="1" spans="2:6">
-      <c r="B380" s="5"/>
-      <c r="C380" s="19"/>
+      <c r="B380" s="5" t="s">
+        <v>587</v>
+      </c>
+      <c r="C380" s="21" t="s">
+        <v>588</v>
+      </c>
       <c r="D380" s="20"/>
       <c r="E380" s="5"/>
       <c r="F380" s="5"/>
     </row>
     <row r="381" ht="38" customHeight="1" spans="2:6">
-      <c r="B381" s="5"/>
+      <c r="B381" s="5" t="s">
+        <v>589</v>
+      </c>
       <c r="C381" s="19"/>
       <c r="D381" s="20"/>
       <c r="E381" s="5"/>
@@ -6371,15 +8057,15 @@
       <c r="E384" s="5"/>
       <c r="F384" s="5"/>
     </row>
-    <row r="385" ht="38" customHeight="1" spans="1:6">
-      <c r="A385"/>
+    <row r="385" ht="38" customHeight="1" spans="2:6">
       <c r="B385" s="5"/>
       <c r="C385" s="19"/>
       <c r="D385" s="20"/>
       <c r="E385" s="5"/>
       <c r="F385" s="5"/>
     </row>
-    <row r="386" ht="38" customHeight="1" spans="2:6">
+    <row r="386" ht="38" customHeight="1" spans="1:6">
+      <c r="A386" s="2"/>
       <c r="B386" s="5"/>
       <c r="C386" s="19"/>
       <c r="D386" s="20"/>
@@ -6442,15 +8128,15 @@
       <c r="E394" s="5"/>
       <c r="F394" s="5"/>
     </row>
-    <row r="395" ht="38" customHeight="1" spans="1:6">
-      <c r="A395"/>
+    <row r="395" ht="38" customHeight="1" spans="2:6">
       <c r="B395" s="5"/>
       <c r="C395" s="19"/>
       <c r="D395" s="20"/>
       <c r="E395" s="5"/>
       <c r="F395" s="5"/>
     </row>
-    <row r="396" ht="38" customHeight="1" spans="2:6">
+    <row r="396" ht="38" customHeight="1" spans="1:6">
+      <c r="A396" s="2"/>
       <c r="B396" s="5"/>
       <c r="C396" s="19"/>
       <c r="D396" s="20"/>
@@ -6513,15 +8199,15 @@
       <c r="E404" s="5"/>
       <c r="F404" s="5"/>
     </row>
-    <row r="405" ht="38" customHeight="1" spans="1:6">
-      <c r="A405"/>
+    <row r="405" ht="38" customHeight="1" spans="2:6">
       <c r="B405" s="5"/>
       <c r="C405" s="19"/>
       <c r="D405" s="20"/>
       <c r="E405" s="5"/>
       <c r="F405" s="5"/>
     </row>
-    <row r="406" ht="38" customHeight="1" spans="2:6">
+    <row r="406" ht="38" customHeight="1" spans="1:6">
+      <c r="A406" s="2"/>
       <c r="B406" s="5"/>
       <c r="C406" s="19"/>
       <c r="D406" s="20"/>
@@ -6584,15 +8270,15 @@
       <c r="E414" s="5"/>
       <c r="F414" s="5"/>
     </row>
-    <row r="415" ht="38" customHeight="1" spans="1:6">
-      <c r="A415"/>
+    <row r="415" ht="38" customHeight="1" spans="2:6">
       <c r="B415" s="5"/>
       <c r="C415" s="19"/>
       <c r="D415" s="20"/>
       <c r="E415" s="5"/>
       <c r="F415" s="5"/>
     </row>
-    <row r="416" ht="38" customHeight="1" spans="2:6">
+    <row r="416" ht="38" customHeight="1" spans="1:6">
+      <c r="A416" s="2"/>
       <c r="B416" s="5"/>
       <c r="C416" s="19"/>
       <c r="D416" s="20"/>
@@ -6655,15 +8341,15 @@
       <c r="E424" s="5"/>
       <c r="F424" s="5"/>
     </row>
-    <row r="425" ht="38" customHeight="1" spans="1:6">
-      <c r="A425"/>
+    <row r="425" ht="38" customHeight="1" spans="2:6">
       <c r="B425" s="5"/>
       <c r="C425" s="19"/>
       <c r="D425" s="20"/>
       <c r="E425" s="5"/>
       <c r="F425" s="5"/>
     </row>
-    <row r="426" ht="38" customHeight="1" spans="2:6">
+    <row r="426" ht="38" customHeight="1" spans="1:6">
+      <c r="A426" s="2"/>
       <c r="B426" s="5"/>
       <c r="C426" s="19"/>
       <c r="D426" s="20"/>
@@ -6726,15 +8412,15 @@
       <c r="E434" s="5"/>
       <c r="F434" s="5"/>
     </row>
-    <row r="435" ht="38" customHeight="1" spans="1:6">
-      <c r="A435"/>
+    <row r="435" ht="38" customHeight="1" spans="2:6">
       <c r="B435" s="5"/>
       <c r="C435" s="19"/>
       <c r="D435" s="20"/>
       <c r="E435" s="5"/>
       <c r="F435" s="5"/>
     </row>
-    <row r="436" ht="38" customHeight="1" spans="2:6">
+    <row r="436" ht="38" customHeight="1" spans="1:6">
+      <c r="A436" s="2"/>
       <c r="B436" s="5"/>
       <c r="C436" s="19"/>
       <c r="D436" s="20"/>
@@ -6797,15 +8483,15 @@
       <c r="E444" s="5"/>
       <c r="F444" s="5"/>
     </row>
-    <row r="445" ht="38" customHeight="1" spans="1:6">
-      <c r="A445"/>
+    <row r="445" ht="38" customHeight="1" spans="2:6">
       <c r="B445" s="5"/>
       <c r="C445" s="19"/>
       <c r="D445" s="20"/>
       <c r="E445" s="5"/>
       <c r="F445" s="5"/>
     </row>
-    <row r="446" ht="38" customHeight="1" spans="2:6">
+    <row r="446" ht="38" customHeight="1" spans="1:6">
+      <c r="A446" s="2"/>
       <c r="B446" s="5"/>
       <c r="C446" s="19"/>
       <c r="D446" s="20"/>
@@ -6868,15 +8554,15 @@
       <c r="E454" s="5"/>
       <c r="F454" s="5"/>
     </row>
-    <row r="455" ht="38" customHeight="1" spans="1:6">
-      <c r="A455"/>
+    <row r="455" ht="38" customHeight="1" spans="2:6">
       <c r="B455" s="5"/>
       <c r="C455" s="19"/>
       <c r="D455" s="20"/>
       <c r="E455" s="5"/>
       <c r="F455" s="5"/>
     </row>
-    <row r="456" ht="38" customHeight="1" spans="2:6">
+    <row r="456" ht="38" customHeight="1" spans="1:6">
+      <c r="A456" s="2"/>
       <c r="B456" s="5"/>
       <c r="C456" s="19"/>
       <c r="D456" s="20"/>
@@ -6939,15 +8625,15 @@
       <c r="E464" s="5"/>
       <c r="F464" s="5"/>
     </row>
-    <row r="465" ht="38" customHeight="1" spans="1:6">
-      <c r="A465"/>
+    <row r="465" ht="38" customHeight="1" spans="2:6">
       <c r="B465" s="5"/>
       <c r="C465" s="19"/>
       <c r="D465" s="20"/>
       <c r="E465" s="5"/>
       <c r="F465" s="5"/>
     </row>
-    <row r="466" ht="38" customHeight="1" spans="2:6">
+    <row r="466" ht="38" customHeight="1" spans="1:6">
+      <c r="A466" s="2"/>
       <c r="B466" s="5"/>
       <c r="C466" s="19"/>
       <c r="D466" s="20"/>
@@ -7010,15 +8696,15 @@
       <c r="E474" s="5"/>
       <c r="F474" s="5"/>
     </row>
-    <row r="475" ht="38" customHeight="1" spans="1:6">
-      <c r="A475"/>
+    <row r="475" ht="38" customHeight="1" spans="2:6">
       <c r="B475" s="5"/>
       <c r="C475" s="19"/>
       <c r="D475" s="20"/>
       <c r="E475" s="5"/>
       <c r="F475" s="5"/>
     </row>
-    <row r="476" ht="38" customHeight="1" spans="2:6">
+    <row r="476" ht="38" customHeight="1" spans="1:6">
+      <c r="A476" s="2"/>
       <c r="B476" s="5"/>
       <c r="C476" s="19"/>
       <c r="D476" s="20"/>
@@ -7081,15 +8767,15 @@
       <c r="E484" s="5"/>
       <c r="F484" s="5"/>
     </row>
-    <row r="485" ht="38" customHeight="1" spans="1:6">
-      <c r="A485"/>
+    <row r="485" ht="38" customHeight="1" spans="2:6">
       <c r="B485" s="5"/>
       <c r="C485" s="19"/>
       <c r="D485" s="20"/>
       <c r="E485" s="5"/>
       <c r="F485" s="5"/>
     </row>
-    <row r="486" ht="38" customHeight="1" spans="2:6">
+    <row r="486" ht="38" customHeight="1" spans="1:6">
+      <c r="A486" s="2"/>
       <c r="B486" s="5"/>
       <c r="C486" s="19"/>
       <c r="D486" s="20"/>
@@ -7152,15 +8838,15 @@
       <c r="E494" s="5"/>
       <c r="F494" s="5"/>
     </row>
-    <row r="495" ht="38" customHeight="1" spans="1:6">
-      <c r="A495"/>
+    <row r="495" ht="38" customHeight="1" spans="2:6">
       <c r="B495" s="5"/>
       <c r="C495" s="19"/>
       <c r="D495" s="20"/>
       <c r="E495" s="5"/>
       <c r="F495" s="5"/>
     </row>
-    <row r="496" ht="38" customHeight="1" spans="2:6">
+    <row r="496" ht="38" customHeight="1" spans="1:6">
+      <c r="A496" s="2"/>
       <c r="B496" s="5"/>
       <c r="C496" s="19"/>
       <c r="D496" s="20"/>
@@ -7223,15 +8909,15 @@
       <c r="E504" s="5"/>
       <c r="F504" s="5"/>
     </row>
-    <row r="505" ht="38" customHeight="1" spans="1:6">
-      <c r="A505"/>
+    <row r="505" ht="38" customHeight="1" spans="2:6">
       <c r="B505" s="5"/>
       <c r="C505" s="19"/>
       <c r="D505" s="20"/>
       <c r="E505" s="5"/>
       <c r="F505" s="5"/>
     </row>
-    <row r="506" ht="38" customHeight="1" spans="2:6">
+    <row r="506" ht="38" customHeight="1" spans="1:6">
+      <c r="A506" s="2"/>
       <c r="B506" s="5"/>
       <c r="C506" s="19"/>
       <c r="D506" s="20"/>
@@ -7294,15 +8980,15 @@
       <c r="E514" s="5"/>
       <c r="F514" s="5"/>
     </row>
-    <row r="515" ht="38" customHeight="1" spans="1:6">
-      <c r="A515"/>
+    <row r="515" ht="38" customHeight="1" spans="2:6">
       <c r="B515" s="5"/>
       <c r="C515" s="19"/>
       <c r="D515" s="20"/>
       <c r="E515" s="5"/>
       <c r="F515" s="5"/>
     </row>
-    <row r="516" ht="38" customHeight="1" spans="2:6">
+    <row r="516" ht="38" customHeight="1" spans="1:6">
+      <c r="A516" s="2"/>
       <c r="B516" s="5"/>
       <c r="C516" s="19"/>
       <c r="D516" s="20"/>
@@ -7358,8 +9044,15 @@
       <c r="E523" s="5"/>
       <c r="F523" s="5"/>
     </row>
+    <row r="524" ht="38" customHeight="1" spans="2:6">
+      <c r="B524" s="5"/>
+      <c r="C524" s="19"/>
+      <c r="D524" s="20"/>
+      <c r="E524" s="5"/>
+      <c r="F524" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="495">
+  <mergeCells count="507">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C6:D6"/>
@@ -7515,14 +9208,9 @@
     <mergeCell ref="C230:D230"/>
     <mergeCell ref="C231:D231"/>
     <mergeCell ref="C232:D232"/>
-    <mergeCell ref="C233:D233"/>
-    <mergeCell ref="C234:D234"/>
     <mergeCell ref="C235:D235"/>
     <mergeCell ref="C236:D236"/>
     <mergeCell ref="C237:D237"/>
-    <mergeCell ref="C238:D238"/>
-    <mergeCell ref="C239:D239"/>
-    <mergeCell ref="C240:D240"/>
     <mergeCell ref="C241:D241"/>
     <mergeCell ref="C242:D242"/>
     <mergeCell ref="C243:D243"/>
@@ -7543,9 +9231,6 @@
     <mergeCell ref="C258:D258"/>
     <mergeCell ref="C259:D259"/>
     <mergeCell ref="C260:D260"/>
-    <mergeCell ref="C261:D261"/>
-    <mergeCell ref="C262:D262"/>
-    <mergeCell ref="C263:D263"/>
     <mergeCell ref="C264:D264"/>
     <mergeCell ref="C265:D265"/>
     <mergeCell ref="C266:D266"/>
@@ -7560,10 +9245,6 @@
     <mergeCell ref="C275:D275"/>
     <mergeCell ref="C276:D276"/>
     <mergeCell ref="C277:D277"/>
-    <mergeCell ref="C278:D278"/>
-    <mergeCell ref="C279:D279"/>
-    <mergeCell ref="C280:D280"/>
-    <mergeCell ref="C281:D281"/>
     <mergeCell ref="C282:D282"/>
     <mergeCell ref="C283:D283"/>
     <mergeCell ref="C284:D284"/>
@@ -7578,39 +9259,19 @@
     <mergeCell ref="C293:D293"/>
     <mergeCell ref="C294:D294"/>
     <mergeCell ref="C295:D295"/>
-    <mergeCell ref="C296:D296"/>
-    <mergeCell ref="C297:D297"/>
-    <mergeCell ref="C298:D298"/>
-    <mergeCell ref="C299:D299"/>
     <mergeCell ref="C300:D300"/>
     <mergeCell ref="C301:D301"/>
     <mergeCell ref="C302:D302"/>
     <mergeCell ref="C303:D303"/>
-    <mergeCell ref="C304:D304"/>
-    <mergeCell ref="C305:D305"/>
-    <mergeCell ref="C306:D306"/>
-    <mergeCell ref="C307:D307"/>
-    <mergeCell ref="C308:D308"/>
     <mergeCell ref="C309:D309"/>
     <mergeCell ref="C310:D310"/>
-    <mergeCell ref="C311:D311"/>
-    <mergeCell ref="C312:D312"/>
-    <mergeCell ref="C313:D313"/>
-    <mergeCell ref="C314:D314"/>
-    <mergeCell ref="C315:D315"/>
-    <mergeCell ref="C316:D316"/>
     <mergeCell ref="C317:D317"/>
     <mergeCell ref="C318:D318"/>
     <mergeCell ref="C319:D319"/>
     <mergeCell ref="C320:D320"/>
     <mergeCell ref="C321:D321"/>
-    <mergeCell ref="C322:D322"/>
-    <mergeCell ref="C323:D323"/>
-    <mergeCell ref="C324:D324"/>
     <mergeCell ref="C325:D325"/>
     <mergeCell ref="C326:D326"/>
-    <mergeCell ref="C327:D327"/>
-    <mergeCell ref="C328:D328"/>
     <mergeCell ref="C329:D329"/>
     <mergeCell ref="C330:D330"/>
     <mergeCell ref="C331:D331"/>
@@ -7631,8 +9292,6 @@
     <mergeCell ref="C346:D346"/>
     <mergeCell ref="C347:D347"/>
     <mergeCell ref="C348:D348"/>
-    <mergeCell ref="C349:D349"/>
-    <mergeCell ref="C350:D350"/>
     <mergeCell ref="C351:D351"/>
     <mergeCell ref="C352:D352"/>
     <mergeCell ref="C353:D353"/>
@@ -7644,10 +9303,6 @@
     <mergeCell ref="C359:D359"/>
     <mergeCell ref="C360:D360"/>
     <mergeCell ref="C361:D361"/>
-    <mergeCell ref="C362:D362"/>
-    <mergeCell ref="C363:D363"/>
-    <mergeCell ref="C364:D364"/>
-    <mergeCell ref="C365:D365"/>
     <mergeCell ref="C366:D366"/>
     <mergeCell ref="C367:D367"/>
     <mergeCell ref="C368:D368"/>
@@ -7806,12 +9461,15 @@
     <mergeCell ref="C521:D521"/>
     <mergeCell ref="C522:D522"/>
     <mergeCell ref="C523:D523"/>
+    <mergeCell ref="C524:D524"/>
     <mergeCell ref="A2:A39"/>
     <mergeCell ref="A40:A73"/>
     <mergeCell ref="A74:A125"/>
     <mergeCell ref="A126:A150"/>
     <mergeCell ref="A151:A159"/>
     <mergeCell ref="A160:A186"/>
+    <mergeCell ref="A187:A275"/>
+    <mergeCell ref="A276:A326"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="B13:B15"/>
@@ -7849,14 +9507,62 @@
     <mergeCell ref="B211:B214"/>
     <mergeCell ref="B215:B218"/>
     <mergeCell ref="B219:B227"/>
+    <mergeCell ref="B231:B234"/>
+    <mergeCell ref="B235:B237"/>
+    <mergeCell ref="B238:B240"/>
+    <mergeCell ref="B241:B242"/>
+    <mergeCell ref="B243:B245"/>
+    <mergeCell ref="B246:B247"/>
+    <mergeCell ref="B251:B252"/>
+    <mergeCell ref="B253:B254"/>
+    <mergeCell ref="B255:B256"/>
+    <mergeCell ref="B257:B259"/>
+    <mergeCell ref="B260:B263"/>
+    <mergeCell ref="B264:B266"/>
+    <mergeCell ref="B267:B269"/>
+    <mergeCell ref="B270:B272"/>
+    <mergeCell ref="B273:B275"/>
+    <mergeCell ref="B276:B281"/>
+    <mergeCell ref="B282:B285"/>
+    <mergeCell ref="B287:B289"/>
+    <mergeCell ref="B290:B292"/>
+    <mergeCell ref="B296:B299"/>
+    <mergeCell ref="B300:B301"/>
+    <mergeCell ref="B302:B308"/>
+    <mergeCell ref="B309:B316"/>
+    <mergeCell ref="B317:B321"/>
+    <mergeCell ref="B322:B326"/>
+    <mergeCell ref="B327:B328"/>
+    <mergeCell ref="B329:B330"/>
+    <mergeCell ref="B331:B332"/>
+    <mergeCell ref="B333:B334"/>
+    <mergeCell ref="B335:B336"/>
+    <mergeCell ref="B337:B339"/>
+    <mergeCell ref="B340:B342"/>
+    <mergeCell ref="B346:B347"/>
+    <mergeCell ref="B348:B350"/>
+    <mergeCell ref="B351:B353"/>
+    <mergeCell ref="B354:B357"/>
+    <mergeCell ref="B358:B361"/>
+    <mergeCell ref="B362:B366"/>
+    <mergeCell ref="B369:B370"/>
+    <mergeCell ref="B374:B376"/>
+    <mergeCell ref="B377:B379"/>
     <mergeCell ref="C41:C44"/>
     <mergeCell ref="C63:C68"/>
     <mergeCell ref="C75:C83"/>
     <mergeCell ref="C206:C209"/>
+    <mergeCell ref="C278:C281"/>
+    <mergeCell ref="C296:C299"/>
+    <mergeCell ref="C304:C308"/>
+    <mergeCell ref="C311:C316"/>
+    <mergeCell ref="C322:C324"/>
+    <mergeCell ref="C362:C365"/>
     <mergeCell ref="D16:D18"/>
     <mergeCell ref="E27:E31"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sun Jan 16 16:26:34 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CISSP/CISSP知识点.xlsx
+++ b/笔记/CISSP/CISSP知识点.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277">
   <si>
     <t>章节</t>
   </si>
@@ -5285,22 +5285,84 @@
     <t>EAL1 功能测试</t>
   </si>
   <si>
+    <t>要求正确操作的一定置信度，但是在安全威胁不严重的时候可以用该级别。当应用了适当关注的独立保证来包含个人信息时，这个级别非常有用</t>
+  </si>
+  <si>
     <t>EAL2 结构测试</t>
   </si>
   <si>
+    <t>设计信息和测试结果的交付与良好的商业应用一致时可以应用该级别。在开发人员或用户要求从低级别到中等独立保证安全性时，这个界别非常有用。尤其是评估传统系统时，IT与该级别的关系很大。</t>
+  </si>
+  <si>
     <t>EAL3 系统地测试和检查</t>
   </si>
   <si>
+    <t>安全工程从设计阶段开始，并且随后未发生重大更改直至完成的时候可以用该级别。在开发人员和用户要求从低级到中等的度量保证安全性时，这个界别非常有用（包括对 TOE 及其开发的彻底研究）</t>
+  </si>
+  <si>
     <t>EAL4 系统地设计、测试和回顾</t>
   </si>
   <si>
+    <t>已使用严格、确定的安全工程和良好的商业开发实践时可以应用该级别。这个级别不要求大量的专业知识、技能或资源、涉及所有TOE安全功能的独立测试。</t>
+  </si>
+  <si>
     <t>EAL5 半正式设计和测试</t>
   </si>
   <si>
+    <t>使用严格的安全工程和商业开发实践（包括专业的安全工程技术）来进行半正式测试。开发人员或用户要求高级别的度量保证安全性时（以计划好的开发方式开始，随后进行严格的开发）可以应用该级别。</t>
+  </si>
+  <si>
     <t>EAL6 半正式验证、设计和测试</t>
   </si>
   <si>
+    <t>在设计、开发和测试的所有阶段都使用直接、严格的安全工程技术，从而生成优良的TOE。在需要高风险状况下的 TOE 可以应用该级别。此时受保护资产的价值会证明额外的成本是合理的。广泛的测试减少了渗透的风险、隐蔽通道的可能性以及被攻击的脆弱性。</t>
+  </si>
+  <si>
     <t>EAL7 正式验证、设计和测试</t>
+  </si>
+  <si>
+    <t>只用于最高风险状况或涉及高价值资产的情况。这个级别限于这样的 TOE：密切关注的安全功能性需要进行广泛的正式分析和测试。</t>
+  </si>
+  <si>
+    <t>CC 局限性</t>
+  </si>
+  <si>
+    <t>CC 指南并不确保用户对数据的操作方式也是安全的。</t>
+  </si>
+  <si>
+    <t>CC 指南也没有解决特定安全范围之外的管理问题。CC 指南不包括现场安全评估，也就是说，他们不涉及与人员、组织实践和过程或物理安全相关的控制。</t>
+  </si>
+  <si>
+    <t>也没有明确规定对加密算法强度进行评级的标准。</t>
+  </si>
+  <si>
+    <t>3.4 理解信息系统（IS）的安全功能</t>
+  </si>
+  <si>
+    <t>内存保护（Memory Protection）</t>
+  </si>
+  <si>
+    <r>
+      <t>内存保护是很安全组件，在操作系统中必须设计和实现。无论系统中执行哪些程序，都必须执行内存保护，否则可能导致不稳定、侵害完整性、拒绝服务和泄露等结果。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>内存保护用于防止活动的进程与不是专门指派或分配给他们的内存区域进行交互。</t>
+    </r>
+  </si>
+  <si>
+    <t>由于整个操作系统和所有应用程序都在内存中加载和运行，因此内存是攻击者真正能实施破坏的地方。如果攻击者想要与进程进行恶意交互，则需要知道输入攻击应该发送到的内存地址。如果操作系统不断改变这些地址（如Address Space Layout Randomization ASLR技术），将大大降低攻击成功的可能性。攻击者不知道访问在哪里，则无法进行破坏。</t>
+  </si>
+  <si>
+    <t>内存泄漏（Memroy Leak）</t>
+  </si>
+  <si>
+    <t>当应用程序请求使用一段内存时，操作系统会为其分配特定的内存空间。当应用程序使用完内存后，应该通知操作系统释放内存，一遍其他应用程序继续使用。担有些应用程序编写的不够规范，不会像操作系统表明该内存已不再使用。</t>
   </si>
 </sst>
 </file>
@@ -6193,9 +6255,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6212,6 +6271,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6478,7 +6540,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27784425" y="123308110"/>
+          <a:off x="27784425" y="123524010"/>
           <a:ext cx="7767955" cy="2211705"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -16104,10 +16166,10 @@
   <sheetPr/>
   <dimension ref="A1:F704"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C98" sqref="C98"/>
+      <selection pane="bottomLeft" activeCell="C105" sqref="C105:D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -16929,7 +16991,7 @@
       <c r="F73" s="30"/>
     </row>
     <row r="74" s="14" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A74" s="30" t="s">
+      <c r="A74" s="23" t="s">
         <v>1228</v>
       </c>
       <c r="B74" s="23" t="s">
@@ -16943,7 +17005,7 @@
       <c r="F74" s="30"/>
     </row>
     <row r="75" s="14" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A75" s="30"/>
+      <c r="A75" s="26"/>
       <c r="B75" s="26"/>
       <c r="C75" s="24" t="s">
         <v>1231</v>
@@ -16953,7 +17015,7 @@
       <c r="F75" s="30"/>
     </row>
     <row r="76" s="14" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A76" s="30"/>
+      <c r="A76" s="26"/>
       <c r="B76" s="29"/>
       <c r="C76" s="24" t="s">
         <v>1232</v>
@@ -16963,7 +17025,7 @@
       <c r="F76" s="30"/>
     </row>
     <row r="77" s="14" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A77" s="30"/>
+      <c r="A77" s="26"/>
       <c r="B77" s="23" t="s">
         <v>1233</v>
       </c>
@@ -16975,7 +17037,7 @@
       <c r="F77" s="30"/>
     </row>
     <row r="78" s="14" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A78" s="30"/>
+      <c r="A78" s="26"/>
       <c r="B78" s="29"/>
       <c r="C78" s="24" t="s">
         <v>1235</v>
@@ -16985,7 +17047,7 @@
       <c r="F78" s="30"/>
     </row>
     <row r="79" s="14" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A79" s="30"/>
+      <c r="A79" s="26"/>
       <c r="B79" s="23" t="s">
         <v>1236</v>
       </c>
@@ -16997,7 +17059,7 @@
       <c r="F79" s="30"/>
     </row>
     <row r="80" s="14" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A80" s="30"/>
+      <c r="A80" s="26"/>
       <c r="B80" s="26"/>
       <c r="C80" s="24" t="s">
         <v>1238</v>
@@ -17007,7 +17069,7 @@
       <c r="F80" s="30"/>
     </row>
     <row r="81" s="14" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A81" s="30"/>
+      <c r="A81" s="26"/>
       <c r="B81" s="26"/>
       <c r="C81" s="24" t="s">
         <v>1239</v>
@@ -17017,7 +17079,7 @@
       <c r="F81" s="30"/>
     </row>
     <row r="82" s="14" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A82" s="30"/>
+      <c r="A82" s="26"/>
       <c r="B82" s="26"/>
       <c r="C82" s="24" t="s">
         <v>1240</v>
@@ -17027,7 +17089,7 @@
       <c r="F82" s="30"/>
     </row>
     <row r="83" s="14" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A83" s="30"/>
+      <c r="A83" s="26"/>
       <c r="B83" s="26"/>
       <c r="C83" s="24" t="s">
         <v>1241</v>
@@ -17037,7 +17099,7 @@
       <c r="F83" s="30"/>
     </row>
     <row r="84" s="14" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A84" s="30"/>
+      <c r="A84" s="26"/>
       <c r="B84" s="29"/>
       <c r="C84" s="24" t="s">
         <v>1242</v>
@@ -17047,7 +17109,7 @@
       <c r="F84" s="30"/>
     </row>
     <row r="85" s="14" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A85" s="30"/>
+      <c r="A85" s="26"/>
       <c r="B85" s="23" t="s">
         <v>1243</v>
       </c>
@@ -17059,7 +17121,7 @@
       <c r="F85" s="30"/>
     </row>
     <row r="86" s="14" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A86" s="30"/>
+      <c r="A86" s="26"/>
       <c r="B86" s="26"/>
       <c r="C86" s="24" t="s">
         <v>1245</v>
@@ -17069,7 +17131,7 @@
       <c r="F86" s="30"/>
     </row>
     <row r="87" s="14" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A87" s="30"/>
+      <c r="A87" s="26"/>
       <c r="B87" s="26"/>
       <c r="C87" s="24" t="s">
         <v>1246</v>
@@ -17079,7 +17141,7 @@
       <c r="F87" s="30"/>
     </row>
     <row r="88" s="14" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A88" s="30"/>
+      <c r="A88" s="26"/>
       <c r="B88" s="29"/>
       <c r="C88" s="24" t="s">
         <v>1247</v>
@@ -17089,7 +17151,7 @@
       <c r="F88" s="30"/>
     </row>
     <row r="89" s="14" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A89" s="30"/>
+      <c r="A89" s="26"/>
       <c r="B89" s="23" t="s">
         <v>1248</v>
       </c>
@@ -17101,744 +17163,778 @@
       <c r="F89" s="30"/>
     </row>
     <row r="90" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A90" s="32"/>
+      <c r="A90" s="26"/>
       <c r="B90" s="26"/>
       <c r="C90" s="20" t="s">
         <v>1250</v>
       </c>
       <c r="D90" s="21"/>
-      <c r="E90" s="32"/>
-      <c r="F90" s="32"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="38"/>
     </row>
     <row r="91" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A91" s="32"/>
+      <c r="A91" s="26"/>
       <c r="B91" s="29"/>
-      <c r="C91" s="33" t="s">
+      <c r="C91" s="32" t="s">
         <v>1251</v>
       </c>
-      <c r="D91" s="34"/>
-      <c r="E91" s="32"/>
-      <c r="F91" s="32"/>
+      <c r="D91" s="33"/>
+      <c r="E91" s="38"/>
+      <c r="F91" s="38"/>
     </row>
     <row r="92" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A92" s="32"/>
-      <c r="B92" s="35" t="s">
+      <c r="A92" s="26"/>
+      <c r="B92" s="34" t="s">
         <v>1252</v>
       </c>
-      <c r="C92" s="36" t="s">
+      <c r="C92" s="35" t="s">
         <v>1253</v>
       </c>
-      <c r="D92" s="36"/>
-      <c r="E92" s="32"/>
-      <c r="F92" s="32"/>
+      <c r="D92" s="35" t="s">
+        <v>1254</v>
+      </c>
+      <c r="E92" s="38"/>
+      <c r="F92" s="38"/>
     </row>
     <row r="93" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A93" s="32"/>
-      <c r="B93" s="37"/>
+      <c r="A93" s="26"/>
+      <c r="B93" s="36"/>
       <c r="C93" s="27" t="s">
-        <v>1254</v>
-      </c>
-      <c r="D93" s="27"/>
-      <c r="E93" s="32"/>
-      <c r="F93" s="32"/>
+        <v>1255</v>
+      </c>
+      <c r="D93" s="27" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E93" s="38"/>
+      <c r="F93" s="38"/>
     </row>
     <row r="94" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A94" s="32"/>
-      <c r="B94" s="37"/>
-      <c r="C94" s="36" t="s">
-        <v>1255</v>
-      </c>
-      <c r="D94" s="36"/>
-      <c r="E94" s="32"/>
-      <c r="F94" s="32"/>
+      <c r="A94" s="26"/>
+      <c r="B94" s="36"/>
+      <c r="C94" s="35" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D94" s="35" t="s">
+        <v>1258</v>
+      </c>
+      <c r="E94" s="38"/>
+      <c r="F94" s="38"/>
     </row>
     <row r="95" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A95" s="32"/>
-      <c r="B95" s="37"/>
-      <c r="C95" s="36" t="s">
-        <v>1256</v>
-      </c>
-      <c r="D95" s="36"/>
-      <c r="E95" s="32"/>
-      <c r="F95" s="32"/>
+      <c r="A95" s="26"/>
+      <c r="B95" s="36"/>
+      <c r="C95" s="35" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D95" s="35" t="s">
+        <v>1260</v>
+      </c>
+      <c r="E95" s="38"/>
+      <c r="F95" s="38"/>
     </row>
     <row r="96" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A96" s="32"/>
-      <c r="B96" s="37"/>
-      <c r="C96" s="36" t="s">
-        <v>1257</v>
-      </c>
-      <c r="D96" s="36"/>
-      <c r="E96" s="32"/>
-      <c r="F96" s="32"/>
+      <c r="A96" s="26"/>
+      <c r="B96" s="36"/>
+      <c r="C96" s="35" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D96" s="35" t="s">
+        <v>1262</v>
+      </c>
+      <c r="E96" s="38"/>
+      <c r="F96" s="38"/>
     </row>
     <row r="97" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A97" s="32"/>
-      <c r="B97" s="37"/>
-      <c r="C97" s="36" t="s">
-        <v>1258</v>
-      </c>
-      <c r="D97" s="36"/>
-      <c r="E97" s="32"/>
-      <c r="F97" s="32"/>
+      <c r="A97" s="26"/>
+      <c r="B97" s="36"/>
+      <c r="C97" s="35" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D97" s="35" t="s">
+        <v>1264</v>
+      </c>
+      <c r="E97" s="38"/>
+      <c r="F97" s="38"/>
     </row>
     <row r="98" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A98" s="32"/>
-      <c r="B98" s="38"/>
-      <c r="C98" s="36" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D98" s="36"/>
-      <c r="E98" s="32"/>
-      <c r="F98" s="32"/>
+      <c r="A98" s="26"/>
+      <c r="B98" s="37"/>
+      <c r="C98" s="35" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D98" s="35" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E98" s="38"/>
+      <c r="F98" s="38"/>
     </row>
     <row r="99" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A99" s="32"/>
-      <c r="B99" s="32"/>
-      <c r="C99" s="33"/>
-      <c r="D99" s="34"/>
-      <c r="E99" s="32"/>
-      <c r="F99" s="32"/>
+      <c r="A99" s="26"/>
+      <c r="B99" s="34" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C99" s="32" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D99" s="33"/>
+      <c r="E99" s="38"/>
+      <c r="F99" s="38"/>
     </row>
     <row r="100" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A100" s="32"/>
-      <c r="B100" s="32"/>
-      <c r="C100" s="33"/>
-      <c r="D100" s="34"/>
-      <c r="E100" s="32"/>
-      <c r="F100" s="32"/>
+      <c r="A100" s="26"/>
+      <c r="B100" s="36"/>
+      <c r="C100" s="32" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D100" s="33"/>
+      <c r="E100" s="38"/>
+      <c r="F100" s="38"/>
     </row>
     <row r="101" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A101" s="32"/>
-      <c r="B101" s="32"/>
-      <c r="C101" s="33"/>
-      <c r="D101" s="34"/>
-      <c r="E101" s="32"/>
-      <c r="F101" s="32"/>
+      <c r="A101" s="29"/>
+      <c r="B101" s="37"/>
+      <c r="C101" s="32" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D101" s="33"/>
+      <c r="E101" s="38"/>
+      <c r="F101" s="38"/>
     </row>
     <row r="102" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A102" s="32"/>
-      <c r="B102" s="32"/>
-      <c r="C102" s="33"/>
-      <c r="D102" s="34"/>
-      <c r="E102" s="32"/>
-      <c r="F102" s="32"/>
-    </row>
-    <row r="103" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A103" s="32"/>
-      <c r="B103" s="32"/>
-      <c r="C103" s="33"/>
-      <c r="D103" s="34"/>
-      <c r="E103" s="32"/>
-      <c r="F103" s="32"/>
+      <c r="A102" s="38" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B102" s="34" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C102" s="20" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D102" s="33"/>
+      <c r="E102" s="38"/>
+      <c r="F102" s="38"/>
+    </row>
+    <row r="103" s="15" customFormat="1" ht="57" customHeight="1" spans="1:6">
+      <c r="A103" s="38"/>
+      <c r="B103" s="37"/>
+      <c r="C103" s="32" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D103" s="33"/>
+      <c r="E103" s="38"/>
+      <c r="F103" s="38"/>
     </row>
     <row r="104" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A104" s="32"/>
-      <c r="B104" s="32"/>
-      <c r="C104" s="33"/>
-      <c r="D104" s="34"/>
-      <c r="E104" s="32"/>
-      <c r="F104" s="32"/>
+      <c r="A104" s="38"/>
+      <c r="B104" s="38" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C104" s="32" t="s">
+        <v>1276</v>
+      </c>
+      <c r="D104" s="33"/>
+      <c r="E104" s="38"/>
+      <c r="F104" s="38"/>
     </row>
     <row r="105" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A105" s="32"/>
-      <c r="B105" s="32"/>
-      <c r="C105" s="33"/>
-      <c r="D105" s="34"/>
-      <c r="E105" s="32"/>
-      <c r="F105" s="32"/>
+      <c r="A105" s="38"/>
+      <c r="B105" s="38"/>
+      <c r="C105" s="32"/>
+      <c r="D105" s="33"/>
+      <c r="E105" s="38"/>
+      <c r="F105" s="38"/>
     </row>
     <row r="106" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A106" s="32"/>
-      <c r="B106" s="32"/>
-      <c r="C106" s="33"/>
-      <c r="D106" s="34"/>
-      <c r="E106" s="32"/>
-      <c r="F106" s="32"/>
+      <c r="A106" s="38"/>
+      <c r="B106" s="38"/>
+      <c r="C106" s="32"/>
+      <c r="D106" s="33"/>
+      <c r="E106" s="38"/>
+      <c r="F106" s="38"/>
     </row>
     <row r="107" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A107" s="32"/>
-      <c r="B107" s="32"/>
-      <c r="C107" s="33"/>
-      <c r="D107" s="34"/>
-      <c r="E107" s="32"/>
-      <c r="F107" s="32"/>
+      <c r="A107" s="38"/>
+      <c r="B107" s="38"/>
+      <c r="C107" s="32"/>
+      <c r="D107" s="33"/>
+      <c r="E107" s="38"/>
+      <c r="F107" s="38"/>
     </row>
     <row r="108" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A108" s="32"/>
-      <c r="B108" s="32"/>
-      <c r="C108" s="33"/>
-      <c r="D108" s="34"/>
-      <c r="E108" s="32"/>
-      <c r="F108" s="32"/>
+      <c r="A108" s="38"/>
+      <c r="B108" s="38"/>
+      <c r="C108" s="32"/>
+      <c r="D108" s="33"/>
+      <c r="E108" s="38"/>
+      <c r="F108" s="38"/>
     </row>
     <row r="109" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A109" s="32"/>
-      <c r="B109" s="32"/>
-      <c r="C109" s="33"/>
-      <c r="D109" s="34"/>
-      <c r="E109" s="32"/>
-      <c r="F109" s="32"/>
+      <c r="A109" s="38"/>
+      <c r="B109" s="38"/>
+      <c r="C109" s="32"/>
+      <c r="D109" s="33"/>
+      <c r="E109" s="38"/>
+      <c r="F109" s="38"/>
     </row>
     <row r="110" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A110" s="32"/>
-      <c r="B110" s="32"/>
-      <c r="C110" s="33"/>
-      <c r="D110" s="34"/>
-      <c r="E110" s="32"/>
-      <c r="F110" s="32"/>
+      <c r="A110" s="38"/>
+      <c r="B110" s="38"/>
+      <c r="C110" s="32"/>
+      <c r="D110" s="33"/>
+      <c r="E110" s="38"/>
+      <c r="F110" s="38"/>
     </row>
     <row r="111" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A111" s="32"/>
-      <c r="B111" s="32"/>
-      <c r="C111" s="33"/>
-      <c r="D111" s="34"/>
-      <c r="E111" s="32"/>
-      <c r="F111" s="32"/>
+      <c r="A111" s="38"/>
+      <c r="B111" s="38"/>
+      <c r="C111" s="32"/>
+      <c r="D111" s="33"/>
+      <c r="E111" s="38"/>
+      <c r="F111" s="38"/>
     </row>
     <row r="112" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A112" s="32"/>
-      <c r="B112" s="32"/>
-      <c r="C112" s="33"/>
-      <c r="D112" s="34"/>
-      <c r="E112" s="32"/>
-      <c r="F112" s="32"/>
+      <c r="A112" s="38"/>
+      <c r="B112" s="38"/>
+      <c r="C112" s="32"/>
+      <c r="D112" s="33"/>
+      <c r="E112" s="38"/>
+      <c r="F112" s="38"/>
     </row>
     <row r="113" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A113" s="32"/>
-      <c r="B113" s="32"/>
-      <c r="C113" s="33"/>
-      <c r="D113" s="34"/>
-      <c r="E113" s="32"/>
-      <c r="F113" s="32"/>
+      <c r="A113" s="38"/>
+      <c r="B113" s="38"/>
+      <c r="C113" s="32"/>
+      <c r="D113" s="33"/>
+      <c r="E113" s="38"/>
+      <c r="F113" s="38"/>
     </row>
     <row r="114" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A114" s="32"/>
-      <c r="B114" s="32"/>
-      <c r="C114" s="33"/>
-      <c r="D114" s="34"/>
-      <c r="E114" s="32"/>
-      <c r="F114" s="32"/>
+      <c r="A114" s="38"/>
+      <c r="B114" s="38"/>
+      <c r="C114" s="32"/>
+      <c r="D114" s="33"/>
+      <c r="E114" s="38"/>
+      <c r="F114" s="38"/>
     </row>
     <row r="115" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A115" s="32"/>
-      <c r="B115" s="32"/>
-      <c r="C115" s="33"/>
-      <c r="D115" s="34"/>
-      <c r="E115" s="32"/>
-      <c r="F115" s="32"/>
+      <c r="A115" s="38"/>
+      <c r="B115" s="38"/>
+      <c r="C115" s="32"/>
+      <c r="D115" s="33"/>
+      <c r="E115" s="38"/>
+      <c r="F115" s="38"/>
     </row>
     <row r="116" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A116" s="32"/>
-      <c r="B116" s="32"/>
-      <c r="C116" s="33"/>
-      <c r="D116" s="34"/>
-      <c r="E116" s="32"/>
-      <c r="F116" s="32"/>
+      <c r="A116" s="38"/>
+      <c r="B116" s="38"/>
+      <c r="C116" s="32"/>
+      <c r="D116" s="33"/>
+      <c r="E116" s="38"/>
+      <c r="F116" s="38"/>
     </row>
     <row r="117" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A117" s="32"/>
-      <c r="B117" s="32"/>
-      <c r="C117" s="33"/>
-      <c r="D117" s="34"/>
-      <c r="E117" s="32"/>
-      <c r="F117" s="32"/>
+      <c r="A117" s="38"/>
+      <c r="B117" s="38"/>
+      <c r="C117" s="32"/>
+      <c r="D117" s="33"/>
+      <c r="E117" s="38"/>
+      <c r="F117" s="38"/>
     </row>
     <row r="118" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A118" s="32"/>
-      <c r="B118" s="32"/>
-      <c r="C118" s="33"/>
-      <c r="D118" s="34"/>
-      <c r="E118" s="32"/>
-      <c r="F118" s="32"/>
+      <c r="A118" s="38"/>
+      <c r="B118" s="38"/>
+      <c r="C118" s="32"/>
+      <c r="D118" s="33"/>
+      <c r="E118" s="38"/>
+      <c r="F118" s="38"/>
     </row>
     <row r="119" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A119" s="32"/>
-      <c r="B119" s="32"/>
-      <c r="C119" s="33"/>
-      <c r="D119" s="34"/>
-      <c r="E119" s="32"/>
-      <c r="F119" s="32"/>
+      <c r="A119" s="38"/>
+      <c r="B119" s="38"/>
+      <c r="C119" s="32"/>
+      <c r="D119" s="33"/>
+      <c r="E119" s="38"/>
+      <c r="F119" s="38"/>
     </row>
     <row r="120" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A120" s="32"/>
-      <c r="B120" s="32"/>
-      <c r="C120" s="33"/>
-      <c r="D120" s="34"/>
-      <c r="E120" s="32"/>
-      <c r="F120" s="32"/>
+      <c r="A120" s="38"/>
+      <c r="B120" s="38"/>
+      <c r="C120" s="32"/>
+      <c r="D120" s="33"/>
+      <c r="E120" s="38"/>
+      <c r="F120" s="38"/>
     </row>
     <row r="121" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A121" s="32"/>
-      <c r="B121" s="32"/>
-      <c r="C121" s="33"/>
-      <c r="D121" s="34"/>
-      <c r="E121" s="32"/>
-      <c r="F121" s="32"/>
+      <c r="A121" s="38"/>
+      <c r="B121" s="38"/>
+      <c r="C121" s="32"/>
+      <c r="D121" s="33"/>
+      <c r="E121" s="38"/>
+      <c r="F121" s="38"/>
     </row>
     <row r="122" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A122" s="32"/>
-      <c r="B122" s="32"/>
-      <c r="C122" s="33"/>
-      <c r="D122" s="34"/>
-      <c r="E122" s="32"/>
-      <c r="F122" s="32"/>
+      <c r="A122" s="38"/>
+      <c r="B122" s="38"/>
+      <c r="C122" s="32"/>
+      <c r="D122" s="33"/>
+      <c r="E122" s="38"/>
+      <c r="F122" s="38"/>
     </row>
     <row r="123" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A123" s="32"/>
-      <c r="B123" s="32"/>
-      <c r="C123" s="33"/>
-      <c r="D123" s="34"/>
-      <c r="E123" s="32"/>
-      <c r="F123" s="32"/>
+      <c r="A123" s="38"/>
+      <c r="B123" s="38"/>
+      <c r="C123" s="32"/>
+      <c r="D123" s="33"/>
+      <c r="E123" s="38"/>
+      <c r="F123" s="38"/>
     </row>
     <row r="124" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A124" s="32"/>
-      <c r="B124" s="32"/>
-      <c r="C124" s="33"/>
-      <c r="D124" s="34"/>
-      <c r="E124" s="32"/>
-      <c r="F124" s="32"/>
+      <c r="A124" s="38"/>
+      <c r="B124" s="38"/>
+      <c r="C124" s="32"/>
+      <c r="D124" s="33"/>
+      <c r="E124" s="38"/>
+      <c r="F124" s="38"/>
     </row>
     <row r="125" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A125" s="32"/>
-      <c r="B125" s="32"/>
-      <c r="C125" s="33"/>
-      <c r="D125" s="34"/>
-      <c r="E125" s="32"/>
-      <c r="F125" s="32"/>
+      <c r="A125" s="38"/>
+      <c r="B125" s="38"/>
+      <c r="C125" s="32"/>
+      <c r="D125" s="33"/>
+      <c r="E125" s="38"/>
+      <c r="F125" s="38"/>
     </row>
     <row r="126" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A126" s="32"/>
-      <c r="B126" s="32"/>
-      <c r="C126" s="33"/>
-      <c r="D126" s="34"/>
-      <c r="E126" s="32"/>
-      <c r="F126" s="32"/>
+      <c r="A126" s="38"/>
+      <c r="B126" s="38"/>
+      <c r="C126" s="32"/>
+      <c r="D126" s="33"/>
+      <c r="E126" s="38"/>
+      <c r="F126" s="38"/>
     </row>
     <row r="127" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A127" s="32"/>
-      <c r="B127" s="32"/>
-      <c r="C127" s="33"/>
-      <c r="D127" s="34"/>
-      <c r="E127" s="32"/>
-      <c r="F127" s="32"/>
+      <c r="A127" s="38"/>
+      <c r="B127" s="38"/>
+      <c r="C127" s="32"/>
+      <c r="D127" s="33"/>
+      <c r="E127" s="38"/>
+      <c r="F127" s="38"/>
     </row>
     <row r="128" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A128" s="32"/>
-      <c r="B128" s="32"/>
-      <c r="C128" s="33"/>
-      <c r="D128" s="34"/>
-      <c r="E128" s="32"/>
-      <c r="F128" s="32"/>
+      <c r="A128" s="38"/>
+      <c r="B128" s="38"/>
+      <c r="C128" s="32"/>
+      <c r="D128" s="33"/>
+      <c r="E128" s="38"/>
+      <c r="F128" s="38"/>
     </row>
     <row r="129" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A129" s="32"/>
-      <c r="B129" s="32"/>
-      <c r="C129" s="33"/>
-      <c r="D129" s="34"/>
-      <c r="E129" s="32"/>
-      <c r="F129" s="32"/>
+      <c r="A129" s="38"/>
+      <c r="B129" s="38"/>
+      <c r="C129" s="32"/>
+      <c r="D129" s="33"/>
+      <c r="E129" s="38"/>
+      <c r="F129" s="38"/>
     </row>
     <row r="130" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A130" s="32"/>
-      <c r="B130" s="32"/>
-      <c r="C130" s="33"/>
-      <c r="D130" s="34"/>
-      <c r="E130" s="32"/>
-      <c r="F130" s="32"/>
+      <c r="A130" s="38"/>
+      <c r="B130" s="38"/>
+      <c r="C130" s="32"/>
+      <c r="D130" s="33"/>
+      <c r="E130" s="38"/>
+      <c r="F130" s="38"/>
     </row>
     <row r="131" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A131" s="32"/>
-      <c r="B131" s="32"/>
-      <c r="C131" s="33"/>
-      <c r="D131" s="34"/>
-      <c r="E131" s="32"/>
-      <c r="F131" s="32"/>
+      <c r="A131" s="38"/>
+      <c r="B131" s="38"/>
+      <c r="C131" s="32"/>
+      <c r="D131" s="33"/>
+      <c r="E131" s="38"/>
+      <c r="F131" s="38"/>
     </row>
     <row r="132" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A132" s="32"/>
-      <c r="B132" s="32"/>
-      <c r="C132" s="33"/>
-      <c r="D132" s="34"/>
-      <c r="E132" s="32"/>
-      <c r="F132" s="32"/>
+      <c r="A132" s="38"/>
+      <c r="B132" s="38"/>
+      <c r="C132" s="32"/>
+      <c r="D132" s="33"/>
+      <c r="E132" s="38"/>
+      <c r="F132" s="38"/>
     </row>
     <row r="133" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A133" s="32"/>
-      <c r="B133" s="32"/>
-      <c r="C133" s="33"/>
-      <c r="D133" s="34"/>
-      <c r="E133" s="32"/>
-      <c r="F133" s="32"/>
+      <c r="A133" s="38"/>
+      <c r="B133" s="38"/>
+      <c r="C133" s="32"/>
+      <c r="D133" s="33"/>
+      <c r="E133" s="38"/>
+      <c r="F133" s="38"/>
     </row>
     <row r="134" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A134" s="32"/>
-      <c r="B134" s="32"/>
-      <c r="C134" s="33"/>
-      <c r="D134" s="34"/>
-      <c r="E134" s="32"/>
-      <c r="F134" s="32"/>
+      <c r="A134" s="38"/>
+      <c r="B134" s="38"/>
+      <c r="C134" s="32"/>
+      <c r="D134" s="33"/>
+      <c r="E134" s="38"/>
+      <c r="F134" s="38"/>
     </row>
     <row r="135" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A135" s="32"/>
-      <c r="B135" s="32"/>
-      <c r="C135" s="33"/>
-      <c r="D135" s="34"/>
-      <c r="E135" s="32"/>
-      <c r="F135" s="32"/>
+      <c r="A135" s="38"/>
+      <c r="B135" s="38"/>
+      <c r="C135" s="32"/>
+      <c r="D135" s="33"/>
+      <c r="E135" s="38"/>
+      <c r="F135" s="38"/>
     </row>
     <row r="136" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A136" s="32"/>
-      <c r="B136" s="32"/>
-      <c r="C136" s="33"/>
-      <c r="D136" s="34"/>
-      <c r="E136" s="32"/>
-      <c r="F136" s="32"/>
+      <c r="A136" s="38"/>
+      <c r="B136" s="38"/>
+      <c r="C136" s="32"/>
+      <c r="D136" s="33"/>
+      <c r="E136" s="38"/>
+      <c r="F136" s="38"/>
     </row>
     <row r="137" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A137" s="32"/>
-      <c r="B137" s="32"/>
-      <c r="C137" s="33"/>
-      <c r="D137" s="34"/>
-      <c r="E137" s="32"/>
-      <c r="F137" s="32"/>
+      <c r="A137" s="38"/>
+      <c r="B137" s="38"/>
+      <c r="C137" s="32"/>
+      <c r="D137" s="33"/>
+      <c r="E137" s="38"/>
+      <c r="F137" s="38"/>
     </row>
     <row r="138" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A138" s="32"/>
-      <c r="B138" s="32"/>
-      <c r="C138" s="33"/>
-      <c r="D138" s="34"/>
-      <c r="E138" s="32"/>
-      <c r="F138" s="32"/>
+      <c r="A138" s="38"/>
+      <c r="B138" s="38"/>
+      <c r="C138" s="32"/>
+      <c r="D138" s="33"/>
+      <c r="E138" s="38"/>
+      <c r="F138" s="38"/>
     </row>
     <row r="139" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A139" s="32"/>
-      <c r="B139" s="32"/>
-      <c r="C139" s="33"/>
-      <c r="D139" s="34"/>
-      <c r="E139" s="32"/>
-      <c r="F139" s="32"/>
+      <c r="A139" s="38"/>
+      <c r="B139" s="38"/>
+      <c r="C139" s="32"/>
+      <c r="D139" s="33"/>
+      <c r="E139" s="38"/>
+      <c r="F139" s="38"/>
     </row>
     <row r="140" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A140" s="32"/>
-      <c r="B140" s="32"/>
-      <c r="C140" s="33"/>
-      <c r="D140" s="34"/>
-      <c r="E140" s="32"/>
-      <c r="F140" s="32"/>
+      <c r="A140" s="38"/>
+      <c r="B140" s="38"/>
+      <c r="C140" s="32"/>
+      <c r="D140" s="33"/>
+      <c r="E140" s="38"/>
+      <c r="F140" s="38"/>
     </row>
     <row r="141" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A141" s="32"/>
-      <c r="B141" s="32"/>
-      <c r="C141" s="33"/>
-      <c r="D141" s="34"/>
-      <c r="E141" s="32"/>
-      <c r="F141" s="32"/>
+      <c r="A141" s="38"/>
+      <c r="B141" s="38"/>
+      <c r="C141" s="32"/>
+      <c r="D141" s="33"/>
+      <c r="E141" s="38"/>
+      <c r="F141" s="38"/>
     </row>
     <row r="142" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A142" s="32"/>
-      <c r="B142" s="32"/>
-      <c r="C142" s="33"/>
-      <c r="D142" s="34"/>
-      <c r="E142" s="32"/>
-      <c r="F142" s="32"/>
+      <c r="A142" s="38"/>
+      <c r="B142" s="38"/>
+      <c r="C142" s="32"/>
+      <c r="D142" s="33"/>
+      <c r="E142" s="38"/>
+      <c r="F142" s="38"/>
     </row>
     <row r="143" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A143" s="32"/>
-      <c r="B143" s="32"/>
-      <c r="C143" s="33"/>
-      <c r="D143" s="34"/>
-      <c r="E143" s="32"/>
-      <c r="F143" s="32"/>
+      <c r="A143" s="38"/>
+      <c r="B143" s="38"/>
+      <c r="C143" s="32"/>
+      <c r="D143" s="33"/>
+      <c r="E143" s="38"/>
+      <c r="F143" s="38"/>
     </row>
     <row r="144" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A144" s="32"/>
-      <c r="B144" s="32"/>
-      <c r="C144" s="33"/>
-      <c r="D144" s="34"/>
-      <c r="E144" s="32"/>
-      <c r="F144" s="32"/>
+      <c r="A144" s="38"/>
+      <c r="B144" s="38"/>
+      <c r="C144" s="32"/>
+      <c r="D144" s="33"/>
+      <c r="E144" s="38"/>
+      <c r="F144" s="38"/>
     </row>
     <row r="145" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A145" s="32"/>
-      <c r="B145" s="32"/>
-      <c r="C145" s="33"/>
-      <c r="D145" s="34"/>
-      <c r="E145" s="32"/>
-      <c r="F145" s="32"/>
+      <c r="A145" s="38"/>
+      <c r="B145" s="38"/>
+      <c r="C145" s="32"/>
+      <c r="D145" s="33"/>
+      <c r="E145" s="38"/>
+      <c r="F145" s="38"/>
     </row>
     <row r="146" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A146" s="32"/>
-      <c r="B146" s="32"/>
-      <c r="C146" s="33"/>
-      <c r="D146" s="34"/>
-      <c r="E146" s="32"/>
-      <c r="F146" s="32"/>
+      <c r="A146" s="38"/>
+      <c r="B146" s="38"/>
+      <c r="C146" s="32"/>
+      <c r="D146" s="33"/>
+      <c r="E146" s="38"/>
+      <c r="F146" s="38"/>
     </row>
     <row r="147" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A147" s="32"/>
-      <c r="B147" s="32"/>
-      <c r="C147" s="33"/>
-      <c r="D147" s="34"/>
-      <c r="E147" s="32"/>
-      <c r="F147" s="32"/>
+      <c r="A147" s="38"/>
+      <c r="B147" s="38"/>
+      <c r="C147" s="32"/>
+      <c r="D147" s="33"/>
+      <c r="E147" s="38"/>
+      <c r="F147" s="38"/>
     </row>
     <row r="148" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A148" s="32"/>
-      <c r="B148" s="32"/>
-      <c r="C148" s="33"/>
-      <c r="D148" s="34"/>
-      <c r="E148" s="32"/>
-      <c r="F148" s="32"/>
+      <c r="A148" s="38"/>
+      <c r="B148" s="38"/>
+      <c r="C148" s="32"/>
+      <c r="D148" s="33"/>
+      <c r="E148" s="38"/>
+      <c r="F148" s="38"/>
     </row>
     <row r="149" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A149" s="32"/>
-      <c r="B149" s="32"/>
-      <c r="C149" s="33"/>
-      <c r="D149" s="34"/>
-      <c r="E149" s="32"/>
-      <c r="F149" s="32"/>
+      <c r="A149" s="38"/>
+      <c r="B149" s="38"/>
+      <c r="C149" s="32"/>
+      <c r="D149" s="33"/>
+      <c r="E149" s="38"/>
+      <c r="F149" s="38"/>
     </row>
     <row r="150" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A150" s="32"/>
-      <c r="B150" s="32"/>
-      <c r="C150" s="33"/>
-      <c r="D150" s="34"/>
-      <c r="E150" s="32"/>
-      <c r="F150" s="32"/>
+      <c r="A150" s="38"/>
+      <c r="B150" s="38"/>
+      <c r="C150" s="32"/>
+      <c r="D150" s="33"/>
+      <c r="E150" s="38"/>
+      <c r="F150" s="38"/>
     </row>
     <row r="151" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A151" s="32"/>
-      <c r="B151" s="32"/>
-      <c r="C151" s="33"/>
-      <c r="D151" s="34"/>
-      <c r="E151" s="32"/>
-      <c r="F151" s="32"/>
+      <c r="A151" s="38"/>
+      <c r="B151" s="38"/>
+      <c r="C151" s="32"/>
+      <c r="D151" s="33"/>
+      <c r="E151" s="38"/>
+      <c r="F151" s="38"/>
     </row>
     <row r="152" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A152" s="32"/>
-      <c r="B152" s="32"/>
-      <c r="C152" s="33"/>
-      <c r="D152" s="34"/>
-      <c r="E152" s="32"/>
-      <c r="F152" s="32"/>
+      <c r="A152" s="38"/>
+      <c r="B152" s="38"/>
+      <c r="C152" s="32"/>
+      <c r="D152" s="33"/>
+      <c r="E152" s="38"/>
+      <c r="F152" s="38"/>
     </row>
     <row r="153" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A153" s="32"/>
-      <c r="B153" s="32"/>
-      <c r="C153" s="33"/>
-      <c r="D153" s="34"/>
-      <c r="E153" s="32"/>
-      <c r="F153" s="32"/>
+      <c r="A153" s="38"/>
+      <c r="B153" s="38"/>
+      <c r="C153" s="32"/>
+      <c r="D153" s="33"/>
+      <c r="E153" s="38"/>
+      <c r="F153" s="38"/>
     </row>
     <row r="154" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A154" s="32"/>
-      <c r="B154" s="32"/>
-      <c r="C154" s="33"/>
-      <c r="D154" s="34"/>
-      <c r="E154" s="32"/>
-      <c r="F154" s="32"/>
+      <c r="A154" s="38"/>
+      <c r="B154" s="38"/>
+      <c r="C154" s="32"/>
+      <c r="D154" s="33"/>
+      <c r="E154" s="38"/>
+      <c r="F154" s="38"/>
     </row>
     <row r="155" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A155" s="32"/>
-      <c r="B155" s="32"/>
-      <c r="C155" s="33"/>
-      <c r="D155" s="34"/>
-      <c r="E155" s="32"/>
-      <c r="F155" s="32"/>
+      <c r="A155" s="38"/>
+      <c r="B155" s="38"/>
+      <c r="C155" s="32"/>
+      <c r="D155" s="33"/>
+      <c r="E155" s="38"/>
+      <c r="F155" s="38"/>
     </row>
     <row r="156" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A156" s="32"/>
-      <c r="B156" s="32"/>
-      <c r="C156" s="33"/>
-      <c r="D156" s="34"/>
-      <c r="E156" s="32"/>
-      <c r="F156" s="32"/>
+      <c r="A156" s="38"/>
+      <c r="B156" s="38"/>
+      <c r="C156" s="32"/>
+      <c r="D156" s="33"/>
+      <c r="E156" s="38"/>
+      <c r="F156" s="38"/>
     </row>
     <row r="157" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A157" s="32"/>
-      <c r="B157" s="32"/>
-      <c r="C157" s="33"/>
-      <c r="D157" s="34"/>
-      <c r="E157" s="32"/>
-      <c r="F157" s="32"/>
+      <c r="A157" s="38"/>
+      <c r="B157" s="38"/>
+      <c r="C157" s="32"/>
+      <c r="D157" s="33"/>
+      <c r="E157" s="38"/>
+      <c r="F157" s="38"/>
     </row>
     <row r="158" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A158" s="32"/>
-      <c r="B158" s="32"/>
-      <c r="C158" s="33"/>
-      <c r="D158" s="34"/>
-      <c r="E158" s="32"/>
-      <c r="F158" s="32"/>
+      <c r="A158" s="38"/>
+      <c r="B158" s="38"/>
+      <c r="C158" s="32"/>
+      <c r="D158" s="33"/>
+      <c r="E158" s="38"/>
+      <c r="F158" s="38"/>
     </row>
     <row r="159" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A159" s="32"/>
-      <c r="B159" s="32"/>
-      <c r="C159" s="33"/>
-      <c r="D159" s="34"/>
-      <c r="E159" s="32"/>
-      <c r="F159" s="32"/>
+      <c r="A159" s="38"/>
+      <c r="B159" s="38"/>
+      <c r="C159" s="32"/>
+      <c r="D159" s="33"/>
+      <c r="E159" s="38"/>
+      <c r="F159" s="38"/>
     </row>
     <row r="160" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A160" s="32"/>
-      <c r="B160" s="32"/>
-      <c r="C160" s="33"/>
-      <c r="D160" s="34"/>
-      <c r="E160" s="32"/>
-      <c r="F160" s="32"/>
+      <c r="A160" s="38"/>
+      <c r="B160" s="38"/>
+      <c r="C160" s="32"/>
+      <c r="D160" s="33"/>
+      <c r="E160" s="38"/>
+      <c r="F160" s="38"/>
     </row>
     <row r="161" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A161" s="32"/>
-      <c r="B161" s="32"/>
-      <c r="C161" s="33"/>
-      <c r="D161" s="34"/>
-      <c r="E161" s="32"/>
-      <c r="F161" s="32"/>
+      <c r="A161" s="38"/>
+      <c r="B161" s="38"/>
+      <c r="C161" s="32"/>
+      <c r="D161" s="33"/>
+      <c r="E161" s="38"/>
+      <c r="F161" s="38"/>
     </row>
     <row r="162" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A162" s="32"/>
-      <c r="B162" s="32"/>
-      <c r="C162" s="33"/>
-      <c r="D162" s="34"/>
-      <c r="E162" s="32"/>
-      <c r="F162" s="32"/>
+      <c r="A162" s="38"/>
+      <c r="B162" s="38"/>
+      <c r="C162" s="32"/>
+      <c r="D162" s="33"/>
+      <c r="E162" s="38"/>
+      <c r="F162" s="38"/>
     </row>
     <row r="163" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A163" s="32"/>
-      <c r="B163" s="32"/>
-      <c r="C163" s="33"/>
-      <c r="D163" s="34"/>
-      <c r="E163" s="32"/>
-      <c r="F163" s="32"/>
+      <c r="A163" s="38"/>
+      <c r="B163" s="38"/>
+      <c r="C163" s="32"/>
+      <c r="D163" s="33"/>
+      <c r="E163" s="38"/>
+      <c r="F163" s="38"/>
     </row>
     <row r="164" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A164" s="32"/>
-      <c r="B164" s="32"/>
-      <c r="C164" s="33"/>
-      <c r="D164" s="34"/>
-      <c r="E164" s="32"/>
-      <c r="F164" s="32"/>
+      <c r="A164" s="38"/>
+      <c r="B164" s="38"/>
+      <c r="C164" s="32"/>
+      <c r="D164" s="33"/>
+      <c r="E164" s="38"/>
+      <c r="F164" s="38"/>
     </row>
     <row r="165" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A165" s="32"/>
-      <c r="B165" s="32"/>
-      <c r="C165" s="33"/>
-      <c r="D165" s="34"/>
-      <c r="E165" s="32"/>
-      <c r="F165" s="32"/>
+      <c r="A165" s="38"/>
+      <c r="B165" s="38"/>
+      <c r="C165" s="32"/>
+      <c r="D165" s="33"/>
+      <c r="E165" s="38"/>
+      <c r="F165" s="38"/>
     </row>
     <row r="166" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A166" s="32"/>
-      <c r="B166" s="32"/>
-      <c r="C166" s="33"/>
-      <c r="D166" s="34"/>
-      <c r="E166" s="32"/>
-      <c r="F166" s="32"/>
+      <c r="A166" s="38"/>
+      <c r="B166" s="38"/>
+      <c r="C166" s="32"/>
+      <c r="D166" s="33"/>
+      <c r="E166" s="38"/>
+      <c r="F166" s="38"/>
     </row>
     <row r="167" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A167" s="32"/>
-      <c r="B167" s="32"/>
-      <c r="C167" s="33"/>
-      <c r="D167" s="34"/>
-      <c r="E167" s="32"/>
-      <c r="F167" s="32"/>
+      <c r="A167" s="38"/>
+      <c r="B167" s="38"/>
+      <c r="C167" s="32"/>
+      <c r="D167" s="33"/>
+      <c r="E167" s="38"/>
+      <c r="F167" s="38"/>
     </row>
     <row r="168" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A168" s="32"/>
-      <c r="B168" s="32"/>
-      <c r="C168" s="33"/>
-      <c r="D168" s="34"/>
-      <c r="E168" s="32"/>
-      <c r="F168" s="32"/>
+      <c r="A168" s="38"/>
+      <c r="B168" s="38"/>
+      <c r="C168" s="32"/>
+      <c r="D168" s="33"/>
+      <c r="E168" s="38"/>
+      <c r="F168" s="38"/>
     </row>
     <row r="169" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A169" s="32"/>
-      <c r="B169" s="32"/>
-      <c r="C169" s="33"/>
-      <c r="D169" s="34"/>
-      <c r="E169" s="32"/>
-      <c r="F169" s="32"/>
+      <c r="A169" s="38"/>
+      <c r="B169" s="38"/>
+      <c r="C169" s="32"/>
+      <c r="D169" s="33"/>
+      <c r="E169" s="38"/>
+      <c r="F169" s="38"/>
     </row>
     <row r="170" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A170" s="32"/>
-      <c r="B170" s="32"/>
-      <c r="C170" s="33"/>
-      <c r="D170" s="34"/>
-      <c r="E170" s="32"/>
-      <c r="F170" s="32"/>
+      <c r="A170" s="38"/>
+      <c r="B170" s="38"/>
+      <c r="C170" s="32"/>
+      <c r="D170" s="33"/>
+      <c r="E170" s="38"/>
+      <c r="F170" s="38"/>
     </row>
     <row r="171" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A171" s="32"/>
-      <c r="B171" s="32"/>
+      <c r="A171" s="38"/>
+      <c r="B171" s="38"/>
       <c r="C171" s="20"/>
       <c r="D171" s="21"/>
-      <c r="E171" s="32"/>
-      <c r="F171" s="32"/>
+      <c r="E171" s="38"/>
+      <c r="F171" s="38"/>
     </row>
     <row r="172" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A172" s="32"/>
-      <c r="B172" s="32"/>
+      <c r="A172" s="38"/>
+      <c r="B172" s="38"/>
       <c r="C172" s="20"/>
       <c r="D172" s="21"/>
-      <c r="E172" s="32"/>
-      <c r="F172" s="32"/>
+      <c r="E172" s="38"/>
+      <c r="F172" s="38"/>
     </row>
     <row r="173" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A173" s="32"/>
-      <c r="B173" s="32"/>
-      <c r="C173" s="33"/>
-      <c r="D173" s="34"/>
-      <c r="E173" s="32"/>
-      <c r="F173" s="32"/>
+      <c r="A173" s="38"/>
+      <c r="B173" s="38"/>
+      <c r="C173" s="32"/>
+      <c r="D173" s="33"/>
+      <c r="E173" s="38"/>
+      <c r="F173" s="38"/>
     </row>
     <row r="174" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A174" s="32"/>
-      <c r="B174" s="32"/>
-      <c r="C174" s="33"/>
-      <c r="D174" s="34"/>
-      <c r="E174" s="32"/>
-      <c r="F174" s="32"/>
+      <c r="A174" s="38"/>
+      <c r="B174" s="38"/>
+      <c r="C174" s="32"/>
+      <c r="D174" s="33"/>
+      <c r="E174" s="38"/>
+      <c r="F174" s="38"/>
     </row>
     <row r="175" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A175" s="32"/>
-      <c r="B175" s="32"/>
-      <c r="C175" s="33"/>
-      <c r="D175" s="34"/>
-      <c r="E175" s="32"/>
-      <c r="F175" s="32"/>
+      <c r="A175" s="38"/>
+      <c r="B175" s="38"/>
+      <c r="C175" s="32"/>
+      <c r="D175" s="33"/>
+      <c r="E175" s="38"/>
+      <c r="F175" s="38"/>
     </row>
     <row r="176" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A176" s="32"/>
-      <c r="B176" s="32"/>
+      <c r="A176" s="38"/>
+      <c r="B176" s="38"/>
       <c r="C176" s="20"/>
       <c r="D176" s="21"/>
-      <c r="E176" s="32"/>
-      <c r="F176" s="32"/>
+      <c r="E176" s="38"/>
+      <c r="F176" s="38"/>
     </row>
     <row r="177" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A177" s="32"/>
-      <c r="B177" s="32"/>
+      <c r="A177" s="38"/>
+      <c r="B177" s="38"/>
       <c r="C177" s="20"/>
       <c r="D177" s="21"/>
-      <c r="E177" s="32"/>
-      <c r="F177" s="32"/>
+      <c r="E177" s="38"/>
+      <c r="F177" s="38"/>
     </row>
     <row r="178" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A178" s="32"/>
-      <c r="B178" s="32"/>
-      <c r="C178" s="33"/>
-      <c r="D178" s="34"/>
-      <c r="E178" s="32"/>
-      <c r="F178" s="32"/>
+      <c r="A178" s="38"/>
+      <c r="B178" s="38"/>
+      <c r="C178" s="32"/>
+      <c r="D178" s="33"/>
+      <c r="E178" s="38"/>
+      <c r="F178" s="38"/>
     </row>
     <row r="179" s="15" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A179" s="32"/>
-      <c r="B179" s="32"/>
-      <c r="C179" s="33"/>
-      <c r="D179" s="34"/>
-      <c r="E179" s="32"/>
-      <c r="F179" s="32"/>
+      <c r="A179" s="38"/>
+      <c r="B179" s="38"/>
+      <c r="C179" s="32"/>
+      <c r="D179" s="33"/>
+      <c r="E179" s="38"/>
+      <c r="F179" s="38"/>
     </row>
     <row r="180" s="14" customFormat="1" customHeight="1" spans="1:6">
       <c r="A180" s="30"/>
@@ -20816,7 +20912,7 @@
     <row r="703" s="14" customFormat="1" customHeight="1"/>
     <row r="704" s="14" customFormat="1" customHeight="1"/>
   </sheetData>
-  <mergeCells count="536">
+  <mergeCells count="539">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
@@ -21325,6 +21421,7 @@
     <mergeCell ref="C529:D529"/>
     <mergeCell ref="A2:A38"/>
     <mergeCell ref="A39:A73"/>
+    <mergeCell ref="A74:A101"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="B9:B11"/>
@@ -21351,6 +21448,8 @@
     <mergeCell ref="B85:B88"/>
     <mergeCell ref="B89:B91"/>
     <mergeCell ref="B92:B98"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="B102:B103"/>
     <mergeCell ref="C25:C31"/>
     <mergeCell ref="C60:C62"/>
   </mergeCells>

</xml_diff>

<commit_message>
Mon Jan 31 03:19:51 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CISSP/CISSP知识点.xlsx
+++ b/笔记/CISSP/CISSP知识点.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680">
   <si>
     <t>章节</t>
   </si>
@@ -7036,6 +7036,46 @@
   </si>
   <si>
     <t>通过对数据散列值的比较可以验证数据完整性。</t>
+  </si>
+  <si>
+    <t>散列函数的5个基本要求</t>
+  </si>
+  <si>
+    <t>输入值可以是任意长度。</t>
+  </si>
+  <si>
+    <t>输出值具有固定的长度。</t>
+  </si>
+  <si>
+    <t>散列函数在计算任何输入值时要相对容易。</t>
+  </si>
+  <si>
+    <t>散列函数是单向的（输出值不能逆向计算出输入值）。</t>
+  </si>
+  <si>
+    <t>散列函数是不会发生冲突的（意味着找到产生相同散列值的两条消息是及其困难的）。</t>
+  </si>
+  <si>
+    <t>MD5</t>
+  </si>
+  <si>
+    <r>
+      <t>MD5算法产生128位消息摘要。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>实现了额外的安全特性，显著降低了消息只要的生成速度。</t>
+    </r>
+  </si>
+  <si>
+    <t>md5 协议会产生冲突，表名它不是一种单向函数。</t>
+  </si>
+  <si>
+    <t>SHA</t>
   </si>
 </sst>
 </file>
@@ -17804,10 +17844,10 @@
   <sheetPr/>
   <dimension ref="A1:F812"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A347" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A353" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B352" sqref="B352:B355"/>
+      <selection pane="bottomLeft" activeCell="C361" sqref="C361:D361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -21782,63 +21822,83 @@
     </row>
     <row r="356" s="13" customFormat="1" customHeight="1" spans="1:6">
       <c r="A356" s="23"/>
-      <c r="B356" s="23"/>
-      <c r="C356" s="19"/>
-      <c r="D356" s="20"/>
+      <c r="B356" s="26" t="s">
+        <v>1670</v>
+      </c>
+      <c r="C356" s="7" t="s">
+        <v>1671</v>
+      </c>
+      <c r="D356" s="8"/>
       <c r="E356" s="23"/>
       <c r="F356" s="23"/>
     </row>
     <row r="357" s="13" customFormat="1" customHeight="1" spans="1:6">
       <c r="A357" s="23"/>
-      <c r="B357" s="23"/>
-      <c r="C357" s="19"/>
-      <c r="D357" s="20"/>
+      <c r="B357" s="27"/>
+      <c r="C357" s="7" t="s">
+        <v>1672</v>
+      </c>
+      <c r="D357" s="8"/>
       <c r="E357" s="23"/>
       <c r="F357" s="23"/>
     </row>
     <row r="358" s="13" customFormat="1" customHeight="1" spans="1:6">
       <c r="A358" s="23"/>
-      <c r="B358" s="23"/>
-      <c r="C358" s="19"/>
+      <c r="B358" s="27"/>
+      <c r="C358" s="19" t="s">
+        <v>1673</v>
+      </c>
       <c r="D358" s="20"/>
       <c r="E358" s="23"/>
       <c r="F358" s="23"/>
     </row>
     <row r="359" s="13" customFormat="1" customHeight="1" spans="1:6">
       <c r="A359" s="23"/>
-      <c r="B359" s="23"/>
-      <c r="C359" s="19"/>
+      <c r="B359" s="27"/>
+      <c r="C359" s="19" t="s">
+        <v>1674</v>
+      </c>
       <c r="D359" s="20"/>
       <c r="E359" s="23"/>
       <c r="F359" s="23"/>
     </row>
     <row r="360" s="13" customFormat="1" customHeight="1" spans="1:6">
       <c r="A360" s="23"/>
-      <c r="B360" s="23"/>
-      <c r="C360" s="19"/>
+      <c r="B360" s="28"/>
+      <c r="C360" s="19" t="s">
+        <v>1675</v>
+      </c>
       <c r="D360" s="20"/>
       <c r="E360" s="23"/>
       <c r="F360" s="23"/>
     </row>
     <row r="361" s="13" customFormat="1" customHeight="1" spans="1:6">
       <c r="A361" s="23"/>
-      <c r="B361" s="23"/>
-      <c r="C361" s="19"/>
+      <c r="B361" s="26" t="s">
+        <v>1676</v>
+      </c>
+      <c r="C361" s="7" t="s">
+        <v>1677</v>
+      </c>
       <c r="D361" s="20"/>
       <c r="E361" s="23"/>
       <c r="F361" s="23"/>
     </row>
     <row r="362" s="13" customFormat="1" customHeight="1" spans="1:6">
       <c r="A362" s="23"/>
-      <c r="B362" s="23"/>
-      <c r="C362" s="19"/>
+      <c r="B362" s="28"/>
+      <c r="C362" s="19" t="s">
+        <v>1678</v>
+      </c>
       <c r="D362" s="20"/>
       <c r="E362" s="23"/>
       <c r="F362" s="23"/>
     </row>
     <row r="363" s="13" customFormat="1" customHeight="1" spans="1:6">
       <c r="A363" s="23"/>
-      <c r="B363" s="23"/>
+      <c r="B363" s="23" t="s">
+        <v>1679</v>
+      </c>
       <c r="C363" s="19"/>
       <c r="D363" s="20"/>
       <c r="E363" s="23"/>
@@ -23456,7 +23516,7 @@
     <row r="811" s="14" customFormat="1" customHeight="1"/>
     <row r="812" s="14" customFormat="1" customHeight="1"/>
   </sheetData>
-  <mergeCells count="548">
+  <mergeCells count="550">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
@@ -23998,6 +24058,8 @@
     <mergeCell ref="B346:B348"/>
     <mergeCell ref="B349:B351"/>
     <mergeCell ref="B352:B355"/>
+    <mergeCell ref="B356:B360"/>
+    <mergeCell ref="B361:B362"/>
     <mergeCell ref="C25:C31"/>
     <mergeCell ref="C60:C62"/>
     <mergeCell ref="C172:C178"/>

</xml_diff>

<commit_message>
Tue Mar 29 08:53:30 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CISSP/CISSP知识点.xlsx
+++ b/笔记/CISSP/CISSP知识点.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3932">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3989">
   <si>
     <t>章节</t>
   </si>
@@ -16449,6 +16449,196 @@
   </si>
   <si>
     <t>能力成熟度模型</t>
+  </si>
+  <si>
+    <r>
+      <t>CMM是有美国国防部和卡内基梅隆大学软件工程研究所（SEI）联合开发的。它源于1980年代需要衡量和改进新兴的软件开发领域，因为处理能力的提高和成本的降低导致了计算机系统的广泛采用。由于当时计算机科学还是一个新兴领域，开发项目的评估、控制和管理往往很差，因此SEI将一套成功项目通用的最佳实践正式化。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>该模型的最初目的是评估政府承包商按时和按预算交付项目的能力</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，但其他开发和业务流程开始采用成熟度模型思维方式。</t>
+    </r>
+  </si>
+  <si>
+    <t>认识到CMM正在适应新的商业流程，SEI设计了能力成熟度模型集成（CMMI）。它最初的设计是开发（CMMI-DEV），服务（CMMI-SVC）以及产品和服务获取（CMMI-ACQ）方面的专门应用，该框架的最新版本2.0于2018年发布。</t>
+  </si>
+  <si>
+    <t>CMMI模型</t>
+  </si>
+  <si>
+    <t>初始级</t>
+  </si>
+  <si>
+    <t>流程是不可预测的，主要是被动的。这是一个典型的大体上只执行临时性过程的组织机构。</t>
+  </si>
+  <si>
+    <t>管理级</t>
+  </si>
+  <si>
+    <t>流程被描述或记录为项目的特征，而且往往是被动的。某些项目可能管理良好且可重复，但这种成功并没有在整个组织中得到利用。</t>
+  </si>
+  <si>
+    <t>已定义级</t>
+  </si>
+  <si>
+    <t>流程对组织来说是有特点的，是主动的。处于第三级的组织在不同的项目/工作中都有记录的流程，并采取积极措施确保项目的成功，如项目风险的管理。</t>
+  </si>
+  <si>
+    <t>量化管理</t>
+  </si>
+  <si>
+    <t>通过测量来测量和控制过程。这是一个手机和响应指标的组织。</t>
+  </si>
+  <si>
+    <t>优化级</t>
+  </si>
+  <si>
+    <t>组织专注于流程改进。处于第五级的组织有文件记录的流程，利用所学到的经验主动控制，并有强大的监督功能来收集指标和管理活动。</t>
+  </si>
+  <si>
+    <t>软件保证成熟度模型</t>
+  </si>
+  <si>
+    <t>软件保证成熟度模型（SAMM）由开放网络应用安全项目（OWASP）维护，SAMM是一个实施软件安全计划的规范框架，冲抵是将安全活动整合到现有的SDLC中。它提供了一个行动计划，用于评估当前状态，确定目标状态，并在整个SDLC中实施必要的改进，包括对流程、人员、知识和工具的更新。</t>
+  </si>
+  <si>
+    <t>治理</t>
+  </si>
+  <si>
+    <t>战略和衡量标准、政策与合规、教育和指导</t>
+  </si>
+  <si>
+    <t>设计</t>
+  </si>
+  <si>
+    <t>威胁评估、安全要求、安全架构</t>
+  </si>
+  <si>
+    <t>安全建设、安全部署、缺陷管理</t>
+  </si>
+  <si>
+    <t>核实</t>
+  </si>
+  <si>
+    <t>架构评估、需求驱动测试、安全测试</t>
+  </si>
+  <si>
+    <t>运营</t>
+  </si>
+  <si>
+    <t>事故管理、环境管理、运营管理</t>
+  </si>
+  <si>
+    <t>在每组实践中，都有活动流，它们通常代表不同的职责。如，在安全测试 A 中，需要可以由 QA 功能管理的自动化测试工具，而在流 B 中，需要对高风险组件进行手动安全测试。此测试是一项专门的功能，需要应用程序安全或渗透测试经验。每个安全实践也以三个成熟度级别表示。</t>
+  </si>
+  <si>
+    <t>执行安全测试（手动和基于工具的）以发现安全缺陷。</t>
+  </si>
+  <si>
+    <t>执行自动化并辅以常规的人工安全渗透测试，是开发过程中的安全测试更加完整和高效。</t>
+  </si>
+  <si>
+    <t>在开发和部署过程中嵌入安全测试。</t>
+  </si>
+  <si>
+    <t>成熟度模型总结</t>
+  </si>
+  <si>
+    <t>成熟度模型对于确定一个组织的实践所达到的能力和有效性水平是非常有用的，同时也为改进工作指明了方向。它们对于诸如软件开发和安全等复杂活动非常有用，在这些活动中需要一致的、可重复的实践，并且可以衡量增量改进，以证明与管理、操作或安全开销有关的成本。</t>
+  </si>
+  <si>
+    <t>操作和维护</t>
+  </si>
+  <si>
+    <t>操作和维护，通常被称为Q&amp;M，是指系统在实际使用中，在所谓的生产环境中运行的阶段，也就是说，它们被终端用户积极使用。测试、验证和确认活动标志着开发的结束，而向操作和维护的过渡通常被称为推广或部署。所有操作和安全任务确实支持系统安全的目标，特别是可用性的目标。</t>
+  </si>
+  <si>
+    <t>连续性</t>
+  </si>
+  <si>
+    <t>系统在面对不利条件时的恢复能力，以及在中断发生时的恢复能力，是至关重要的。业务连续性、灾难恢复和网络弹性的活动都发生在运行和维护阶段，如生成系统备份。</t>
+  </si>
+  <si>
+    <t>监测和事件响应</t>
+  </si>
+  <si>
+    <t>实时生产系统是大多数安全事件发生的地方，所以组织的监测能力的很大一部分将集中在这个环境。当事件被发现时，调查和恢复的过程通常集中在补救问题和恢复生产正常。服务台响应和数字取证等流程对于确保安全事件得到正确调查至关重要。</t>
+  </si>
+  <si>
+    <t>漏洞和补丁管理</t>
+  </si>
+  <si>
+    <t>扫描系统中的缺陷并进行补救是一项重要的、持续的安全任务。一些缺陷可能会导致SDLC的迭代，特别是对于定制软件，尽管第三方软件的常规补丁部署是这项工作的主要内容。</t>
+  </si>
+  <si>
+    <t>虽然控制对开发和测试环境的访问是很重要的，但大多数系统的用户通常比开发人员多得多，而且敏感数据通常不会在测试或开发中使用。授权、审查和撤销访问的过程将主要集中在操作系统上。</t>
+  </si>
+  <si>
+    <t>变更和配置管理</t>
+  </si>
+  <si>
+    <t>本章单独讨论管理源代码更改的问题。运行中的系统可能被置于配置管理之下，有明确的请求、审查和实施变更的过程，以保持安全基线。</t>
+  </si>
+  <si>
+    <t>对许多系统进行安全管理的一个关键方面是将它们保持在一个已知的、安全的状态，这就是配置管理的功能。然而，但是，变更是必要的，因此可以请求、审查、实施和测试变更的过程也是必要的，这是变更管理的目标。这些结构化流程使系统能够灵活地适应不断变化的需求或环境，同时还充分解决安全问题，以防止对系统安全状态产生不利影响的变化。</t>
+  </si>
+  <si>
+    <t>变更管理通常不属于安全部门的职责或范围，但安全从业人员确实需要积极参与到这个过程中。必须审查变更对安全的潜在影响，必须记录测试计划以确保安全不受不利影响，并且在变更失败的情况下可能会触发安全流程。例如，一个失败的变更的可能会调用业务连续性流程，直到变更被逆转。</t>
+  </si>
+  <si>
+    <t>变更管理流程可以在多个不同级别上实施，具有相应的严格程度和流程集。在组织层面，操作系统（OS）更换等变化需要大量预算和资源规划。在源代码级别，开发人员可以遵循安全编码表尊，如在代码被签入存储库之前评论代码和执行同行评审，存储库充当组织源代码的配置和变更管理系统。代码保持在已知良好状态，批准的更改方法（如拉取请求和提交）必须遵循规则，以确保源代码的完整性不会因未经批准的开发人员更改而丢失。在某些时候，代码也可能达到完成状态，在此之后不允许更改，在一个称为冻结的过程中。这对于执行测试、验证和验证练习非常有用，因为正在发生更改的测试代码可能会导致误报或无意义的发现。</t>
+  </si>
+  <si>
+    <t>变更管理阶段和安全实践</t>
+  </si>
+  <si>
+    <t>请求</t>
+  </si>
+  <si>
+    <t>许多变更过程涉及提交票据或其他正式的变更请求；票据系统的优势在于能够捕获所有与变更有关的细节都在一个地方。该请求必须掌握变更的全部细节，以及预期的资源要求和影响。</t>
+  </si>
+  <si>
+    <t>评估和批准</t>
+  </si>
+  <si>
+    <t>一旦记录下来，变更就由CMB审查，以确定变更的所有预期要求和影响。这要遵循一套记录的标准，其中应包括审查任何安全影响，如引入新的风险或对现有安全控制的不利影响。了解这些影响并确保有足够的资源来解决这些问题，在CMB批准变更之前是至关重要的。</t>
+  </si>
+  <si>
+    <t>变更开发</t>
+  </si>
+  <si>
+    <t>一旦一个变更被批准，负责的各方必须制定一个计划来实际执行该变更，例如安排时间来执行所需的IT任务，收集必要的资源，购买或开发变更的系统组件。这些行动必须遵循和批准的变更请求。</t>
+  </si>
+  <si>
+    <t>在制定了计划之后，就可以实施变更了。与开发阶段一样，所有被批准的变更程序都必须被遵守。如果变更不成功，则需要回退或回滚程序，建立这样的计划和程序通常是对变更批准的一个要求。</t>
+  </si>
+  <si>
+    <t>测试</t>
+  </si>
+  <si>
+    <t>必须对新改变的系统进行测试，以确保这些改变是按预期进行的，现有的功能没有被破坏，而且安全控制仍然按期运行。根据组织和变化的规模，这种测试可能包括高度正式的活动，如认证和鉴定。</t>
+  </si>
+  <si>
+    <t>事后总结</t>
+  </si>
+  <si>
+    <t>通常需要进行一些变更后的活动。必须完成对所执行的记录，因为变更后系统是新的已知状态，它将由配置管理来维护。新实施的功能可能需要对用户进行培训，任何经验教训都应该被记录下来，以便持续改进流程。这个阶段也可以成为事后报告、经验教训或回顾性报告，但识别改进机会的目标是相同的。</t>
+  </si>
+  <si>
+    <t>紧急变更管理</t>
   </si>
 </sst>
 </file>
@@ -17901,7 +18091,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27710765" y="123892310"/>
+          <a:off x="27710765" y="125441710"/>
           <a:ext cx="7767955" cy="2211705"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -17943,7 +18133,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27710765" y="123892310"/>
+          <a:off x="27710765" y="125441710"/>
           <a:ext cx="7767955" cy="2211705"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -51518,9 +51708,9 @@
   <dimension ref="A1:F1025"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51:D51"/>
+      <selection pane="bottomLeft" activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -52099,275 +52289,403 @@
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" s="2" customFormat="1" customHeight="1" spans="1:6">
+    <row r="51" s="2" customFormat="1" ht="65" customHeight="1" spans="1:6">
       <c r="A51" s="5"/>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="8" t="s">
         <v>3931</v>
       </c>
-      <c r="C51" s="6"/>
+      <c r="C51" s="6" t="s">
+        <v>3932</v>
+      </c>
       <c r="D51" s="7"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
     </row>
     <row r="52" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="6"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="6" t="s">
+        <v>3933</v>
+      </c>
       <c r="D52" s="7"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
     </row>
     <row r="53" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="7"/>
+      <c r="B53" s="8" t="s">
+        <v>3934</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>3935</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>3936</v>
+      </c>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
     </row>
     <row r="54" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="7"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="5" t="s">
+        <v>3937</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>3938</v>
+      </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
     </row>
     <row r="55" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="7"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="5" t="s">
+        <v>3939</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>3940</v>
+      </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
     </row>
     <row r="56" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="7"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="5" t="s">
+        <v>3941</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>3942</v>
+      </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
     </row>
     <row r="57" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="7"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="5" t="s">
+        <v>3943</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>3944</v>
+      </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
     </row>
     <row r="58" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="6"/>
+      <c r="B58" s="8" t="s">
+        <v>3945</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>3946</v>
+      </c>
       <c r="D58" s="7"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
     </row>
     <row r="59" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="7"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="5" t="s">
+        <v>3947</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>3948</v>
+      </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
     </row>
     <row r="60" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="7"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="5" t="s">
+        <v>3949</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>3950</v>
+      </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
     </row>
     <row r="61" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="7"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>3951</v>
+      </c>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
     </row>
     <row r="62" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="7"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="5" t="s">
+        <v>3952</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>3953</v>
+      </c>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
     </row>
     <row r="63" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="7"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="5" t="s">
+        <v>3954</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>3955</v>
+      </c>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="6"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="6" t="s">
+        <v>3956</v>
+      </c>
       <c r="D64" s="7"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="7"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="5">
+        <v>1</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>3957</v>
+      </c>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="7"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="5">
+        <v>2</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>3958</v>
+      </c>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="7"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="5">
+        <v>3</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>3959</v>
+      </c>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="6"/>
+      <c r="B68" s="5" t="s">
+        <v>3960</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>3961</v>
+      </c>
       <c r="D68" s="7"/>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="6"/>
+      <c r="B69" s="8" t="s">
+        <v>3962</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>3963</v>
+      </c>
       <c r="D69" s="7"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="7"/>
+      <c r="B70" s="10"/>
+      <c r="C70" s="9" t="s">
+        <v>3964</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>3965</v>
+      </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="7"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="9" t="s">
+        <v>3966</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>3967</v>
+      </c>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
     </row>
     <row r="72" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A72" s="5"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="7"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="9" t="s">
+        <v>3968</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>3969</v>
+      </c>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
     </row>
     <row r="73" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="7"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="9" t="s">
+        <v>2562</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>3970</v>
+      </c>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
     </row>
     <row r="74" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="6"/>
-      <c r="D74" s="7"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="9" t="s">
+        <v>3971</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>3972</v>
+      </c>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
     </row>
-    <row r="75" s="2" customFormat="1" customHeight="1" spans="1:6">
+    <row r="75" s="2" customFormat="1" ht="55" customHeight="1" spans="1:6">
       <c r="A75" s="5"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="6"/>
+      <c r="B75" s="8" t="s">
+        <v>2420</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>3973</v>
+      </c>
       <c r="D75" s="7"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
     </row>
     <row r="76" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="6"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="6" t="s">
+        <v>3974</v>
+      </c>
       <c r="D76" s="7"/>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
     </row>
-    <row r="77" s="2" customFormat="1" customHeight="1" spans="1:6">
+    <row r="77" s="2" customFormat="1" ht="86" customHeight="1" spans="1:6">
       <c r="A77" s="5"/>
-      <c r="B77" s="5"/>
-      <c r="C77" s="6"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="6" t="s">
+        <v>3975</v>
+      </c>
       <c r="D77" s="7"/>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
     </row>
-    <row r="78" s="2" customFormat="1" customHeight="1" spans="1:6">
+    <row r="78" s="2" customFormat="1" ht="41" customHeight="1" spans="1:6">
       <c r="A78" s="5"/>
-      <c r="B78" s="5"/>
-      <c r="C78" s="6"/>
-      <c r="D78" s="7"/>
+      <c r="B78" s="8" t="s">
+        <v>3976</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>3977</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>3978</v>
+      </c>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
     </row>
-    <row r="79" s="2" customFormat="1" customHeight="1" spans="1:6">
+    <row r="79" s="2" customFormat="1" ht="50" customHeight="1" spans="1:6">
       <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="7"/>
+      <c r="B79" s="10"/>
+      <c r="C79" s="9" t="s">
+        <v>3979</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>3980</v>
+      </c>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
     </row>
     <row r="80" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="7"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="9" t="s">
+        <v>3981</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>3982</v>
+      </c>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
     </row>
     <row r="81" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A81" s="5"/>
-      <c r="B81" s="5"/>
-      <c r="C81" s="6"/>
-      <c r="D81" s="7"/>
+      <c r="B81" s="10"/>
+      <c r="C81" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>3983</v>
+      </c>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
     </row>
     <row r="82" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A82" s="5"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="6"/>
-      <c r="D82" s="7"/>
+      <c r="B82" s="10"/>
+      <c r="C82" s="9" t="s">
+        <v>3984</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>3985</v>
+      </c>
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
     </row>
-    <row r="83" s="2" customFormat="1" customHeight="1" spans="1:6">
+    <row r="83" s="2" customFormat="1" ht="65" customHeight="1" spans="1:6">
       <c r="A83" s="5"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="6"/>
-      <c r="D83" s="7"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="9" t="s">
+        <v>3986</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>3987</v>
+      </c>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
     </row>
     <row r="84" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A84" s="5"/>
-      <c r="B84" s="5"/>
+      <c r="B84" s="5" t="s">
+        <v>3988</v>
+      </c>
       <c r="C84" s="6"/>
       <c r="D84" s="7"/>
       <c r="E84" s="5"/>
@@ -56430,7 +56748,7 @@
     <row r="1024" s="2" customFormat="1" customHeight="1"/>
     <row r="1025" s="2" customFormat="1" customHeight="1"/>
   </sheetData>
-  <mergeCells count="519">
+  <mergeCells count="501">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C8:D8"/>
@@ -56465,37 +56783,13 @@
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
     <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
     <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
     <mergeCell ref="C75:D75"/>
     <mergeCell ref="C76:D76"/>
     <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
     <mergeCell ref="C84:D84"/>
     <mergeCell ref="C85:D85"/>
     <mergeCell ref="C86:D86"/>
@@ -56950,6 +57244,12 @@
     <mergeCell ref="B41:B45"/>
     <mergeCell ref="B46:B48"/>
     <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="B58:B67"/>
+    <mergeCell ref="B69:B74"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="B78:B83"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Thu Apr  7 23:30:33 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CISSP/CISSP知识点.xlsx
+++ b/笔记/CISSP/CISSP知识点.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4233">
   <si>
     <t>章节</t>
   </si>
@@ -17755,6 +17755,122 @@
       </rPr>
       <t>。在这两种情况下，不知情的用户在下载和部署软件时，除了合法的软件外，还得到了不需要的恶意软件。始终确保你审查对开放源码软件所做的修改，以确保他们是预期的和正确的文件，并且只从合法的、官方的软件库下载开放源码软件。</t>
     </r>
+  </si>
+  <si>
+    <t>第三方软件</t>
+  </si>
+  <si>
+    <t>第三方软件是由你的组织直接控制之外的公司根据合同开发的，所开发的软件通常供你的组织度独家使用。</t>
+  </si>
+  <si>
+    <r>
+      <t>如同所有收购的软件一样，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>放弃对软体开发过程的控制也存在固有的风险，需要有专门的缓解策略来执行合同、服务级别协议（SLA）和额外的验收测试，以确保交付的软件符合组织的要求。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>使用第三方开发软件是一个应该在慎重考虑成本和收益后作出的决定。专业的第三方开发公司所能提供的质量或交付速度，可以证明所需的高质量开发和项目管理监督成本是合理的。</t>
+    </r>
+  </si>
+  <si>
+    <t>源代码本身的可用性是第三方软件安全需要考虑的另一个重要方面。如果开发机构倒闭了，签约机构可能会发现自己没有关键系统的支持；代码托管是一种合同安排，通常用来防止这种情况的发生。开发机构将源代码的副本存放在一个可信的第三方，即托管机构。签约组织可以在有限的情况下获得代码，如开发商倒闭或违反合同，这使得系统的支持和开发得以继续。</t>
+  </si>
+  <si>
+    <t>托管服务</t>
+  </si>
+  <si>
+    <t>云服务是通过计量消费来收费的，这通常是一种按使用量付费的模式。选择正确的服务将取决于一个组织的需求和技术能力。</t>
+  </si>
+  <si>
+    <t>新兴的云服务必须考虑到软件的安全性，包括无服务器和微服务架构，这些架构结合了管理软件、基础设施和平台的元素，可以更快地部署代码。架构云服务的选择会影响消费者的软件安全评估能力和责任。</t>
+  </si>
+  <si>
+    <t>评估分担的责任</t>
+  </si>
+  <si>
+    <t>共同责任模式在处理各种安全任务方面，定义了云服务提供商（CSP）和云消费者之间的分界线。</t>
+  </si>
+  <si>
+    <t>在所有服务模型中，消费者有责任验证CSP对特定用途的适用性，如处理高度敏感的数据。执行软件评估时可用的控制级别将告知特定CSP或云部署模型的选择；</t>
+  </si>
+  <si>
+    <t>在IaaS中，消费者将拥有最大的灵活性来部署软件，因此也最有能力进行软件评估。IaaS提供了信息系统功能的构件，因此评估软件安全评估将包括COTS、OSS和第三方软件，以适合消费者在IaaS环境中部署的软件类型。</t>
+  </si>
+  <si>
+    <t>在PaaS中，一些选项已经脱离了消费者的控制，因此需要一些补偿过程，如审查审计报告和软件保证的SLA。</t>
+  </si>
+  <si>
+    <t>SaaS为消费者提供了最少的直接评估软件安全的选择，然而，鉴于SaaS供应商的共享性质，通常有关于CSP的软件开发、测试和托管安全实践的审计报告和强有力的控制文件。</t>
+  </si>
+  <si>
+    <t>审计和保证</t>
+  </si>
+  <si>
+    <r>
+      <t>与所有第三方和供应链安全问题一样，保证是托管软件的一个关键概念。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>通常会有一个受信任的第三方参与，以审计的形式进行公证的审查。这可以防止CSP受到消费者的不断审查，同时为消费者提供一个关于安全控制的设计、实施和有效性的可信信息来源。</t>
+    </r>
+  </si>
+  <si>
+    <t>有多个与云计算相关的安全和合规框架，服务组织控制（SOC）、云安全联盟安全信任保证和风险（CSA STAR）和ISO 27000系列（包括ISO27001、27017、27018和27034）等框架都提供了一些与云服务和应用相关的保证。CSP也可以报告对其他框架（如CMMI或BSIMM）的成熟度或遵守的情况，以此向消费者保证CSP的软件开发和托管实践是健全的，不会出现不可接受的风险。</t>
+  </si>
+  <si>
+    <t>8.5 定义并应用安全编码准则和标准</t>
+  </si>
+  <si>
+    <t>定义并应用安全编码准则和标准</t>
+  </si>
+  <si>
+    <t>政策提供了关于目标和期望的高层侧战略指导，而标准和指南则为具体的任务和活动提供指导。标准通常是强制性的，而指南是旨在为如何实现特定目标或任务提供指导的建议。</t>
+  </si>
+  <si>
+    <t>应该为软件开发人员提供指导方针和标准，使他们能够编写代码，以实现组织的战略目标，特别是要求保障系统和数据的保密性、完整性和可用性。</t>
+  </si>
+  <si>
+    <t>源代码层面的安全弱点和漏洞</t>
+  </si>
+  <si>
+    <t>弱点和漏洞密切相关，但这两个术语之间存在细微差别。漏洞的存在是由于存在软件弱点，例如系统源代码中错误和缺陷，这可能是由于在架构、开发和实施系统时候做出的错误或不正确的设计选择造成的。在没有切实可行的方法来利用它们的系统中可能存在弱点，在这种情况下，它们不是漏洞；弱点也会影响系统的非安全方面，例如导致搜索性能缓慢的糟糕的数据库设计。作为CISSP，认识到这一区别很重要，因为组织中的其他团队可能会解决非安全弱点，而漏洞与CISSP负责的安全风险直接相关。</t>
+  </si>
+  <si>
+    <t>相比之下，漏洞是可以利用软件系统中的弱点的方式。非安全性弱点显示是不可利用的，一些不安全的源代码级弱点可以通过整个系统的其他部分来弥补，例如防止缓冲区溢出情况的OS内存管理器，否则由编写不良的源代码所允许。这是软件安全测试中面临的挑战之一：如果源代码弱点不可利用，则修复弱点的成本效益分析可能无法支持修复它所需的努力和资源。肯定地断言弱点不可利用可能很困难，因此使用了有争议的主观衡量标准。</t>
+  </si>
+  <si>
+    <t>漏洞通常是由其存在的软件来追踪的，更具体的是由受影响的版本来追踪，使组织能够确定一个漏洞是否影响他们的系统。弱点和漏洞被编入目录，并使用通用系统进行评分，以帮助识别、交流和测试它们。</t>
+  </si>
+  <si>
+    <t>这种跟踪和评分对于确定补丁等修复措施的优先次序和部署补偿性控制措施非常有用。</t>
+  </si>
+  <si>
+    <t>应用程序编程接口的安全</t>
+  </si>
+  <si>
+    <t>API提供了对系统功能的标准化访问，而不需要了解其内部工作原理。可以通过API访问的功能通常被称为通过API暴露，这意味着它们可以使用标准化的方法（和HTTP请求）被调用。表示状态传输或REST  API使用类似于Web应用程序的URL暴露功能，并接收使用常见的HTTP动词如GET和POST的命令，以检索或发送数据到API。与其为每个应用程序创建一个自定义的通信方案，使用REST API允许其他程序使用这些不偏理解的协议进行交互。</t>
+  </si>
+  <si>
+    <t>API是模块化软件开发的一种形式，现代应用架构经常依靠API在复杂系统的功能、模块或层级之间发送数据。还有其他形式的API，包括现代操作系统中用于访问通用系统功能的内部软件的API，如在用户界面上创建交式窗口，用户在系统组件之间交换信息的简单对象访问协议（SOAP）API，以及用于在分布式系统中跨节点执行功能的RCP API。大多数云服务器都建立在API基础上，云环境管理、数据处理等任务，以及数据存储桶和机器学习模型等服务通过URL（通常称为API端点）暴露给用户。</t>
+  </si>
+  <si>
+    <t>API的功能与网络应用程序基本相同，量程的安全要求往往相似。第一个也是最明显的步骤是了解一个特定的系统和它的API所面临的风险。它是一个可公开访问的API，允许读取或更新敏感信息的访问吗？这样的API显然会面临很高的保密性和完整性风险，应该实施适当的安全控制，以确保信息不会被未经授权的用户或程序通过API读取或改变。API是否只读地访问公共信息，如天气数据？在这种情况下，保密性和访问控制不可能是一个高优先级。</t>
   </si>
 </sst>
 </file>
@@ -19207,7 +19323,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28302585" y="147146010"/>
+          <a:off x="28302585" y="149825710"/>
           <a:ext cx="7767955" cy="2211705"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -19249,7 +19365,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28302585" y="147146010"/>
+          <a:off x="28302585" y="149825710"/>
           <a:ext cx="7767955" cy="2211705"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -52823,10 +52939,10 @@
   <sheetPr/>
   <dimension ref="A1:F1025"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A228" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B211" sqref="B211:B214"/>
+      <selection pane="bottomLeft" activeCell="C231" sqref="C231:D231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -55172,7 +55288,7 @@
       <c r="F203" s="6"/>
     </row>
     <row r="204" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A204" s="6" t="s">
+      <c r="A204" s="16" t="s">
         <v>4184</v>
       </c>
       <c r="B204" s="16" t="s">
@@ -55186,7 +55302,7 @@
       <c r="F204" s="6"/>
     </row>
     <row r="205" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A205" s="6"/>
+      <c r="A205" s="17"/>
       <c r="B205" s="19"/>
       <c r="C205" s="7" t="s">
         <v>4187</v>
@@ -55196,7 +55312,7 @@
       <c r="F205" s="6"/>
     </row>
     <row r="206" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A206" s="6"/>
+      <c r="A206" s="17"/>
       <c r="B206" s="16" t="s">
         <v>4188</v>
       </c>
@@ -55208,7 +55324,7 @@
       <c r="F206" s="6"/>
     </row>
     <row r="207" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A207" s="6"/>
+      <c r="A207" s="17"/>
       <c r="B207" s="17"/>
       <c r="C207" s="7" t="s">
         <v>4190</v>
@@ -55218,7 +55334,7 @@
       <c r="F207" s="6"/>
     </row>
     <row r="208" s="2" customFormat="1" ht="63" customHeight="1" spans="1:6">
-      <c r="A208" s="6"/>
+      <c r="A208" s="17"/>
       <c r="B208" s="17"/>
       <c r="C208" s="10" t="s">
         <v>4191</v>
@@ -55230,7 +55346,7 @@
       <c r="F208" s="6"/>
     </row>
     <row r="209" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A209" s="6"/>
+      <c r="A209" s="17"/>
       <c r="B209" s="17"/>
       <c r="C209" s="10" t="s">
         <v>4193</v>
@@ -55242,7 +55358,7 @@
       <c r="F209" s="6"/>
     </row>
     <row r="210" s="2" customFormat="1" ht="60" customHeight="1" spans="1:6">
-      <c r="A210" s="6"/>
+      <c r="A210" s="17"/>
       <c r="B210" s="19"/>
       <c r="C210" s="10" t="s">
         <v>4195</v>
@@ -55254,7 +55370,7 @@
       <c r="F210" s="6"/>
     </row>
     <row r="211" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A211" s="6"/>
+      <c r="A211" s="17"/>
       <c r="B211" s="16" t="s">
         <v>4197</v>
       </c>
@@ -55266,7 +55382,7 @@
       <c r="F211" s="6"/>
     </row>
     <row r="212" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A212" s="6"/>
+      <c r="A212" s="17"/>
       <c r="B212" s="17"/>
       <c r="C212" s="7" t="s">
         <v>4199</v>
@@ -55276,7 +55392,7 @@
       <c r="F212" s="6"/>
     </row>
     <row r="213" s="2" customFormat="1" ht="90" customHeight="1" spans="1:6">
-      <c r="A213" s="6"/>
+      <c r="A213" s="17"/>
       <c r="B213" s="17"/>
       <c r="C213" s="22" t="s">
         <v>4200</v>
@@ -55288,7 +55404,7 @@
       <c r="F213" s="6"/>
     </row>
     <row r="214" s="2" customFormat="1" ht="80" customHeight="1" spans="1:6">
-      <c r="A214" s="6"/>
+      <c r="A214" s="17"/>
       <c r="B214" s="19"/>
       <c r="C214" s="22" t="s">
         <v>4202</v>
@@ -55300,169 +55416,227 @@
       <c r="F214" s="6"/>
     </row>
     <row r="215" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A215" s="6"/>
-      <c r="B215" s="6"/>
-      <c r="C215" s="7"/>
+      <c r="A215" s="17"/>
+      <c r="B215" s="16" t="s">
+        <v>4204</v>
+      </c>
+      <c r="C215" s="7" t="s">
+        <v>4205</v>
+      </c>
       <c r="D215" s="8"/>
       <c r="E215" s="6"/>
       <c r="F215" s="6"/>
     </row>
-    <row r="216" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A216" s="6"/>
-      <c r="B216" s="6"/>
-      <c r="C216" s="7"/>
+    <row r="216" s="2" customFormat="1" ht="55" customHeight="1" spans="1:6">
+      <c r="A216" s="17"/>
+      <c r="B216" s="17"/>
+      <c r="C216" s="7" t="s">
+        <v>4206</v>
+      </c>
       <c r="D216" s="8"/>
       <c r="E216" s="6"/>
       <c r="F216" s="6"/>
     </row>
-    <row r="217" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A217" s="6"/>
-      <c r="B217" s="6"/>
-      <c r="C217" s="7"/>
-      <c r="D217" s="8"/>
+    <row r="217" s="2" customFormat="1" ht="54" customHeight="1" spans="1:6">
+      <c r="A217" s="17"/>
+      <c r="B217" s="19"/>
+      <c r="C217" s="15" t="s">
+        <v>4207</v>
+      </c>
+      <c r="D217" s="18"/>
       <c r="E217" s="6"/>
       <c r="F217" s="6"/>
     </row>
     <row r="218" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A218" s="6"/>
-      <c r="B218" s="6"/>
-      <c r="C218" s="7"/>
+      <c r="A218" s="17"/>
+      <c r="B218" s="16" t="s">
+        <v>4208</v>
+      </c>
+      <c r="C218" s="7" t="s">
+        <v>4209</v>
+      </c>
       <c r="D218" s="8"/>
       <c r="E218" s="6"/>
       <c r="F218" s="6"/>
     </row>
     <row r="219" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A219" s="6"/>
-      <c r="B219" s="6"/>
-      <c r="C219" s="7"/>
+      <c r="A219" s="17"/>
+      <c r="B219" s="19"/>
+      <c r="C219" s="7" t="s">
+        <v>4210</v>
+      </c>
       <c r="D219" s="8"/>
       <c r="E219" s="6"/>
       <c r="F219" s="6"/>
     </row>
     <row r="220" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A220" s="6"/>
-      <c r="B220" s="6"/>
-      <c r="C220" s="7"/>
+      <c r="A220" s="17"/>
+      <c r="B220" s="16" t="s">
+        <v>4211</v>
+      </c>
+      <c r="C220" s="7" t="s">
+        <v>4212</v>
+      </c>
       <c r="D220" s="8"/>
       <c r="E220" s="6"/>
       <c r="F220" s="6"/>
     </row>
     <row r="221" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A221" s="6"/>
-      <c r="B221" s="6"/>
-      <c r="C221" s="7"/>
+      <c r="A221" s="17"/>
+      <c r="B221" s="17"/>
+      <c r="C221" s="7" t="s">
+        <v>4213</v>
+      </c>
       <c r="D221" s="8"/>
       <c r="E221" s="6"/>
       <c r="F221" s="6"/>
     </row>
     <row r="222" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A222" s="6"/>
-      <c r="B222" s="6"/>
-      <c r="C222" s="7"/>
+      <c r="A222" s="17"/>
+      <c r="B222" s="17"/>
+      <c r="C222" s="7" t="s">
+        <v>4214</v>
+      </c>
       <c r="D222" s="8"/>
       <c r="E222" s="6"/>
       <c r="F222" s="6"/>
     </row>
     <row r="223" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A223" s="6"/>
-      <c r="B223" s="6"/>
-      <c r="C223" s="7"/>
+      <c r="A223" s="17"/>
+      <c r="B223" s="17"/>
+      <c r="C223" s="7" t="s">
+        <v>4215</v>
+      </c>
       <c r="D223" s="8"/>
       <c r="E223" s="6"/>
       <c r="F223" s="6"/>
     </row>
     <row r="224" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A224" s="6"/>
-      <c r="B224" s="6"/>
-      <c r="C224" s="7"/>
-      <c r="D224" s="8"/>
+      <c r="A224" s="17"/>
+      <c r="B224" s="19"/>
+      <c r="C224" s="15" t="s">
+        <v>4216</v>
+      </c>
+      <c r="D224" s="18"/>
       <c r="E224" s="6"/>
       <c r="F224" s="6"/>
     </row>
     <row r="225" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A225" s="6"/>
-      <c r="B225" s="6"/>
-      <c r="C225" s="7"/>
+      <c r="A225" s="17"/>
+      <c r="B225" s="16" t="s">
+        <v>4217</v>
+      </c>
+      <c r="C225" s="15" t="s">
+        <v>4218</v>
+      </c>
       <c r="D225" s="8"/>
       <c r="E225" s="6"/>
       <c r="F225" s="6"/>
     </row>
-    <row r="226" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A226" s="6"/>
-      <c r="B226" s="6"/>
-      <c r="C226" s="7"/>
+    <row r="226" s="2" customFormat="1" ht="65" customHeight="1" spans="1:6">
+      <c r="A226" s="19"/>
+      <c r="B226" s="19"/>
+      <c r="C226" s="7" t="s">
+        <v>4219</v>
+      </c>
       <c r="D226" s="8"/>
       <c r="E226" s="6"/>
       <c r="F226" s="6"/>
     </row>
     <row r="227" s="2" customFormat="1" customHeight="1" spans="1:6">
-      <c r="A227" s="6"/>
-      <c r="B227" s="6"/>
-      <c r="C227" s="7"/>
+      <c r="A227" s="6" t="s">
+        <v>4220</v>
+      </c>
+      <c r="B227" s="16" t="s">
+        <v>4221</v>
+      </c>
+      <c r="C227" s="7" t="s">
+        <v>4222</v>
+      </c>
       <c r="D227" s="8"/>
       <c r="E227" s="6"/>
       <c r="F227" s="6"/>
     </row>
     <row r="228" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A228" s="6"/>
-      <c r="B228" s="6"/>
-      <c r="C228" s="7"/>
+      <c r="B228" s="19"/>
+      <c r="C228" s="7" t="s">
+        <v>4223</v>
+      </c>
       <c r="D228" s="8"/>
       <c r="E228" s="6"/>
       <c r="F228" s="6"/>
     </row>
-    <row r="229" s="2" customFormat="1" customHeight="1" spans="1:6">
+    <row r="229" s="2" customFormat="1" ht="73" customHeight="1" spans="1:6">
       <c r="A229" s="6"/>
-      <c r="B229" s="6"/>
-      <c r="C229" s="7"/>
+      <c r="B229" s="16" t="s">
+        <v>4224</v>
+      </c>
+      <c r="C229" s="7" t="s">
+        <v>4225</v>
+      </c>
       <c r="D229" s="8"/>
       <c r="E229" s="6"/>
       <c r="F229" s="6"/>
     </row>
-    <row r="230" s="2" customFormat="1" customHeight="1" spans="1:6">
+    <row r="230" s="2" customFormat="1" ht="61" customHeight="1" spans="1:6">
       <c r="A230" s="6"/>
-      <c r="B230" s="6"/>
-      <c r="C230" s="7"/>
+      <c r="B230" s="17"/>
+      <c r="C230" s="7" t="s">
+        <v>4226</v>
+      </c>
       <c r="D230" s="8"/>
       <c r="E230" s="6"/>
       <c r="F230" s="6"/>
     </row>
     <row r="231" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A231" s="6"/>
-      <c r="B231" s="6"/>
-      <c r="C231" s="7"/>
+      <c r="B231" s="17"/>
+      <c r="C231" s="7" t="s">
+        <v>4227</v>
+      </c>
       <c r="D231" s="8"/>
       <c r="E231" s="6"/>
       <c r="F231" s="6"/>
     </row>
     <row r="232" s="2" customFormat="1" customHeight="1" spans="1:6">
       <c r="A232" s="6"/>
-      <c r="B232" s="6"/>
-      <c r="C232" s="7"/>
+      <c r="B232" s="19"/>
+      <c r="C232" s="7" t="s">
+        <v>4228</v>
+      </c>
       <c r="D232" s="8"/>
       <c r="E232" s="6"/>
       <c r="F232" s="6"/>
     </row>
-    <row r="233" s="2" customFormat="1" customHeight="1" spans="1:6">
+    <row r="233" s="2" customFormat="1" ht="74" customHeight="1" spans="1:6">
       <c r="A233" s="6"/>
-      <c r="B233" s="6"/>
-      <c r="C233" s="7"/>
+      <c r="B233" s="16" t="s">
+        <v>4229</v>
+      </c>
+      <c r="C233" s="7" t="s">
+        <v>4230</v>
+      </c>
       <c r="D233" s="8"/>
       <c r="E233" s="6"/>
       <c r="F233" s="6"/>
     </row>
-    <row r="234" s="2" customFormat="1" customHeight="1" spans="1:6">
+    <row r="234" s="2" customFormat="1" ht="79" customHeight="1" spans="1:6">
       <c r="A234" s="6"/>
-      <c r="B234" s="6"/>
-      <c r="C234" s="7"/>
+      <c r="B234" s="17"/>
+      <c r="C234" s="7" t="s">
+        <v>4231</v>
+      </c>
       <c r="D234" s="8"/>
       <c r="E234" s="6"/>
       <c r="F234" s="6"/>
     </row>
-    <row r="235" s="2" customFormat="1" customHeight="1" spans="1:6">
+    <row r="235" s="2" customFormat="1" ht="70" customHeight="1" spans="1:6">
       <c r="A235" s="6"/>
-      <c r="B235" s="6"/>
-      <c r="C235" s="7"/>
+      <c r="B235" s="19"/>
+      <c r="C235" s="7" t="s">
+        <v>4232</v>
+      </c>
       <c r="D235" s="8"/>
       <c r="E235" s="6"/>
       <c r="F235" s="6"/>
@@ -58316,7 +58490,7 @@
     <row r="1024" s="2" customFormat="1" customHeight="1"/>
     <row r="1025" s="2" customFormat="1" customHeight="1"/>
   </sheetData>
-  <mergeCells count="483">
+  <mergeCells count="491">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C8:D8"/>
@@ -58753,6 +58927,7 @@
     <mergeCell ref="A2:A90"/>
     <mergeCell ref="A91:A166"/>
     <mergeCell ref="A167:A203"/>
+    <mergeCell ref="A204:A226"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B25"/>
@@ -58800,6 +58975,13 @@
     <mergeCell ref="B204:B205"/>
     <mergeCell ref="B206:B210"/>
     <mergeCell ref="B211:B214"/>
+    <mergeCell ref="B215:B217"/>
+    <mergeCell ref="B218:B219"/>
+    <mergeCell ref="B220:B224"/>
+    <mergeCell ref="B225:B226"/>
+    <mergeCell ref="B227:B228"/>
+    <mergeCell ref="B229:B232"/>
+    <mergeCell ref="B233:B235"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Fri Oct 14 13:39:15 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CISSP/CISSP知识点.xlsx
+++ b/笔记/CISSP/CISSP知识点.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="23980" activeTab="1"/>
+    <workbookView windowHeight="23980"/>
   </bookViews>
   <sheets>
     <sheet name="领域1-安全与风险管理" sheetId="1" r:id="rId1"/>
@@ -288,12 +288,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t>防止未经授权的数据更改</t>
     </r>
     <r>
@@ -21227,10 +21221,10 @@
   <sheetPr/>
   <dimension ref="A1:G533"/>
   <sheetViews>
-    <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A287" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A275" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C305" sqref="C305:D305"/>
+      <selection pane="bottomLeft" activeCell="E292" sqref="E292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="6"/>
@@ -27827,7 +27821,7 @@
   <sheetPr/>
   <dimension ref="A1:F837"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C57" sqref="C57:D57"/>
@@ -30685,9 +30679,9 @@
   <dimension ref="A1:F810"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C430" sqref="C430:D430"/>
+      <selection pane="bottomLeft" activeCell="C141" sqref="C141:D141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -38248,9 +38242,9 @@
   <dimension ref="A1:F880"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A264" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A260" sqref="A260:A327"/>
+      <selection pane="bottomLeft" activeCell="C284" sqref="C284:D284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -43676,8 +43670,8 @@
   <sheetPr/>
   <dimension ref="A1:F696"/>
   <sheetViews>
-    <sheetView zoomScale="105" zoomScaleNormal="105" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:D16"/>
+    <sheetView zoomScale="105" zoomScaleNormal="105" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -46742,10 +46736,10 @@
   <sheetPr/>
   <dimension ref="A1:F721"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14:D14"/>
+      <selection pane="bottomLeft" activeCell="C89" sqref="C89:D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -50046,9 +50040,9 @@
   <dimension ref="A1:F718"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A297" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C326" sqref="C326:D326"/>
+      <selection pane="bottomLeft" activeCell="C108" sqref="C108:D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -54936,9 +54930,9 @@
   <dimension ref="A1:F752"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D82" sqref="D82"/>
+      <selection pane="bottomLeft" activeCell="B233" sqref="B233:B235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
Fri Nov  4 13:04:15 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CISSP/CISSP知识点.xlsx
+++ b/笔记/CISSP/CISSP知识点.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="23980"/>
+    <workbookView windowHeight="23980" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="领域1-安全与风险管理" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="领域7-安全运营" sheetId="7" r:id="rId7"/>
     <sheet name="领域8-软件开发安全" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -288,6 +288,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>防止未经授权的数据更改</t>
     </r>
     <r>
@@ -19334,8 +19340,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -19446,14 +19452,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -19469,17 +19467,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19501,33 +19505,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -19539,23 +19521,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19576,7 +19543,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -19584,7 +19551,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19649,7 +19655,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19661,7 +19667,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19673,7 +19691,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19685,13 +19781,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19703,97 +19793,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19805,13 +19811,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19829,7 +19829,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -20017,16 +20023,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -20048,6 +20054,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -20056,132 +20086,108 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="33" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -20190,43 +20196,43 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -21221,8 +21227,8 @@
   <sheetPr/>
   <dimension ref="A1:G533"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A275" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A526" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="E292" sqref="E292"/>
     </sheetView>
@@ -27822,9 +27828,9 @@
   <dimension ref="A1:F837"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57:D57"/>
+      <selection pane="bottomLeft" activeCell="C161" sqref="C161:D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -30679,7 +30685,7 @@
   <dimension ref="A1:F810"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A465" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C141" sqref="C141:D141"/>
     </sheetView>
@@ -38242,9 +38248,9 @@
   <dimension ref="A1:F880"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A264" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C284" sqref="C284:D284"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -43670,8 +43676,8 @@
   <sheetPr/>
   <dimension ref="A1:F696"/>
   <sheetViews>
-    <sheetView zoomScale="105" zoomScaleNormal="105" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView zoomScale="105" zoomScaleNormal="105" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99:B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -54929,10 +54935,10 @@
   <sheetPr/>
   <dimension ref="A1:F752"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B233" sqref="B233:B235"/>
+      <selection pane="bottomLeft" activeCell="C234" sqref="C234:D234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
Sat Jul 29 09:02:36 CST 2023
</commit_message>
<xml_diff>
--- a/笔记/CISSP/CISSP知识点.xlsx
+++ b/笔记/CISSP/CISSP知识点.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16700" activeTab="1"/>
+    <workbookView windowHeight="24020" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="领域1-安全与风险管理" sheetId="1" r:id="rId1"/>
@@ -19340,9 +19340,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="43">
@@ -19452,6 +19452,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -19460,18 +19468,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -19482,11 +19482,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -19503,22 +19526,6 @@
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -19552,6 +19559,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -19560,37 +19590,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19666,25 +19666,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19702,13 +19726,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19720,7 +19756,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19732,73 +19786,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19816,7 +19804,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19828,25 +19834,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -20000,6 +20000,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -20015,6 +20039,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -20026,24 +20074,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -20067,147 +20097,117 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -20216,34 +20216,34 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="18" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -21239,7 +21239,7 @@
   <dimension ref="A1:G533"/>
   <sheetViews>
     <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A526" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="E292" sqref="E292"/>
     </sheetView>
@@ -27838,8 +27838,8 @@
   <sheetPr/>
   <dimension ref="A1:F837"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
@@ -30696,7 +30696,7 @@
   <dimension ref="A1:F810"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A465" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A332" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C141" sqref="C141:D141"/>
     </sheetView>
@@ -38258,10 +38258,10 @@
   <sheetPr/>
   <dimension ref="A1:F880"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A268" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A380" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C283" sqref="C283:D283"/>
+      <selection pane="bottomLeft" activeCell="D389" sqref="D389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -46754,7 +46754,7 @@
   <dimension ref="A1:F721"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C89" sqref="C89:D89"/>
     </sheetView>
@@ -50057,9 +50057,9 @@
   <dimension ref="A1:F718"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A284" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C108" sqref="C108:D108"/>
+      <selection pane="bottomLeft" activeCell="B315" sqref="B315:B317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
Fri Sep  8 11:30:02 CST 2023
</commit_message>
<xml_diff>
--- a/笔记/CISSP/CISSP知识点.xlsx
+++ b/笔记/CISSP/CISSP知识点.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="24020" activeTab="3"/>
+    <workbookView windowHeight="16820" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="领域1-安全与风险管理" sheetId="1" r:id="rId1"/>
@@ -19452,9 +19452,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19467,49 +19467,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -19529,53 +19498,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19590,7 +19514,83 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19666,19 +19666,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19690,25 +19690,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19720,37 +19726,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19768,7 +19744,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19780,25 +19786,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19810,37 +19828,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -20000,16 +20000,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -20018,8 +20018,17 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -20043,7 +20052,33 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -20062,188 +20097,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -21239,9 +21239,9 @@
   <dimension ref="A1:G533"/>
   <sheetViews>
     <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E292" sqref="E292"/>
+      <selection pane="bottomLeft" activeCell="A191" sqref="A191:A279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="6"/>
@@ -27838,10 +27838,10 @@
   <sheetPr/>
   <dimension ref="A1:F837"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -30698,7 +30698,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A332" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C141" sqref="C141:D141"/>
+      <selection pane="bottomLeft" activeCell="B341" sqref="B341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -38258,7 +38258,7 @@
   <sheetPr/>
   <dimension ref="A1:F880"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A380" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D389" sqref="D389"/>
@@ -43687,8 +43687,8 @@
   <sheetPr/>
   <dimension ref="A1:F696"/>
   <sheetViews>
-    <sheetView zoomScale="105" zoomScaleNormal="105" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99:B108"/>
+    <sheetView zoomScale="105" zoomScaleNormal="105" topLeftCell="D17" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -46754,9 +46754,9 @@
   <dimension ref="A1:F721"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C89" sqref="C89:D89"/>
+      <selection pane="bottomLeft" activeCell="C129" sqref="C129:D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>
@@ -50056,10 +50056,10 @@
   <sheetPr/>
   <dimension ref="A1:F718"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A284" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A350" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B315" sqref="B315:B317"/>
+      <selection pane="bottomLeft" activeCell="A353" sqref="A353:A365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.2734375" defaultRowHeight="40" customHeight="1" outlineLevelCol="5"/>

</xml_diff>